<commit_message>
Adding Dragosel to the forecast portfolio
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,72 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>20.08.202519</t>
-  </si>
-  <si>
-    <t>20.08.202520</t>
-  </si>
-  <si>
-    <t>20.08.202521</t>
-  </si>
-  <si>
-    <t>20.08.202522</t>
-  </si>
-  <si>
-    <t>20.08.202523</t>
-  </si>
-  <si>
-    <t>20.08.202524</t>
-  </si>
-  <si>
-    <t>21.08.20251</t>
-  </si>
-  <si>
-    <t>21.08.20252</t>
-  </si>
-  <si>
-    <t>21.08.20253</t>
-  </si>
-  <si>
-    <t>21.08.20254</t>
-  </si>
-  <si>
-    <t>21.08.20255</t>
-  </si>
-  <si>
-    <t>21.08.20256</t>
-  </si>
-  <si>
-    <t>21.08.20257</t>
-  </si>
-  <si>
-    <t>21.08.20258</t>
-  </si>
-  <si>
-    <t>21.08.20259</t>
-  </si>
-  <si>
-    <t>21.08.202510</t>
-  </si>
-  <si>
-    <t>21.08.202511</t>
-  </si>
-  <si>
-    <t>21.08.202512</t>
-  </si>
-  <si>
-    <t>21.08.202513</t>
-  </si>
-  <si>
-    <t>21.08.202514</t>
-  </si>
-  <si>
-    <t>21.08.202515</t>
-  </si>
-  <si>
-    <t>21.08.202516</t>
-  </si>
-  <si>
     <t>21.08.202517</t>
   </si>
   <si>
@@ -533,6 +467,72 @@
   </si>
   <si>
     <t>27.08.202519</t>
+  </si>
+  <si>
+    <t>27.08.202520</t>
+  </si>
+  <si>
+    <t>27.08.202521</t>
+  </si>
+  <si>
+    <t>27.08.202522</t>
+  </si>
+  <si>
+    <t>27.08.202523</t>
+  </si>
+  <si>
+    <t>27.08.202524</t>
+  </si>
+  <si>
+    <t>28.08.20251</t>
+  </si>
+  <si>
+    <t>28.08.20252</t>
+  </si>
+  <si>
+    <t>28.08.20253</t>
+  </si>
+  <si>
+    <t>28.08.20254</t>
+  </si>
+  <si>
+    <t>28.08.20255</t>
+  </si>
+  <si>
+    <t>28.08.20256</t>
+  </si>
+  <si>
+    <t>28.08.20257</t>
+  </si>
+  <si>
+    <t>28.08.20258</t>
+  </si>
+  <si>
+    <t>28.08.20259</t>
+  </si>
+  <si>
+    <t>28.08.202510</t>
+  </si>
+  <si>
+    <t>28.08.202511</t>
+  </si>
+  <si>
+    <t>28.08.202512</t>
+  </si>
+  <si>
+    <t>28.08.202513</t>
+  </si>
+  <si>
+    <t>28.08.202514</t>
+  </si>
+  <si>
+    <t>28.08.202515</t>
+  </si>
+  <si>
+    <t>28.08.202516</t>
+  </si>
+  <si>
+    <t>28.08.202517</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45889</v>
+        <v>45890</v>
       </c>
       <c r="B2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>0.175</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45889</v>
+        <v>45890</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3">
-        <v>0.219</v>
+        <v>0.175</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45889</v>
+        <v>45890</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>0.293</v>
+        <v>0.999</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45889</v>
+        <v>45890</v>
       </c>
       <c r="B5">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>0.129</v>
+        <v>0.635</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45889</v>
+        <v>45890</v>
       </c>
       <c r="B6">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>0.129</v>
+        <v>0.305</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45889</v>
+        <v>45890</v>
       </c>
       <c r="B7">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7">
-        <v>0.129</v>
+        <v>0.141</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1003,10 +1003,10 @@
         <v>45890</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>0.048</v>
+        <v>0.141</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1017,10 +1017,10 @@
         <v>45890</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C9">
-        <v>0.043</v>
+        <v>0.141</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0.043</v>
+        <v>0.135</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>0.043</v>
+        <v>0.135</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>0.043</v>
+        <v>0.135</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>0.023</v>
+        <v>0.048</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>0.138</v>
+        <v>0.023</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>0.594</v>
+        <v>0.023</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>1.492</v>
+        <v>0.1</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17">
-        <v>2.175</v>
+        <v>0.471</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>2.99</v>
+        <v>1.067</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19">
-        <v>3.442</v>
+        <v>1.613</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B20">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>3.763</v>
+        <v>1.862</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B21">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21">
-        <v>3.859</v>
+        <v>1.986</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B22">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22">
-        <v>2.185</v>
+        <v>2.436</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B23">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C23">
-        <v>1.998</v>
+        <v>2.424</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B24">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24">
-        <v>2.721</v>
+        <v>2.26</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B25">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25">
-        <v>1.953</v>
+        <v>1.923</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B26">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>0.983</v>
+        <v>1.451</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B27">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C27">
-        <v>0.5610000000000001</v>
+        <v>1.04</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B28">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C28">
-        <v>0.305</v>
+        <v>0.509</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B29">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>0.141</v>
+        <v>0.47</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B30">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C30">
-        <v>0.141</v>
+        <v>0.126</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45890</v>
+        <v>45891</v>
       </c>
       <c r="B31">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C31">
-        <v>0.141</v>
+        <v>0.028</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1339,10 +1339,10 @@
         <v>45891</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C32">
-        <v>0.135</v>
+        <v>0.028</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1353,10 +1353,10 @@
         <v>45891</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C33">
-        <v>0.135</v>
+        <v>0.028</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>0.135</v>
+        <v>0.023</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>0.048</v>
+        <v>0.023</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>0.043</v>
+        <v>0.023</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>0.023</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B38">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C38">
-        <v>0.125</v>
+        <v>0.023</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B39">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C39">
-        <v>0.502</v>
+        <v>0.023</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C40">
-        <v>1.033</v>
+        <v>0.046</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C41">
-        <v>1.953</v>
+        <v>0.303</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B42">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C42">
-        <v>2.49</v>
+        <v>0.864</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B43">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C43">
-        <v>2.94</v>
+        <v>1.434</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B44">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C44">
-        <v>2.995</v>
+        <v>1.828</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B45">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C45">
-        <v>3.289</v>
+        <v>1.799</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B46">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C46">
-        <v>3.077</v>
+        <v>1.822</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B47">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C47">
-        <v>2.485</v>
+        <v>1.964</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B48">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C48">
-        <v>1.923</v>
+        <v>1.656</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B49">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C49">
-        <v>1.084</v>
+        <v>1.4</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B50">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C50">
-        <v>0.647</v>
+        <v>0.978</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B51">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C51">
-        <v>0.473</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B52">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C52">
-        <v>0.129</v>
+        <v>0.412</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B53">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C53">
-        <v>0.028</v>
+        <v>0.47</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B54">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C54">
-        <v>0.028</v>
+        <v>0.126</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,10 +1658,10 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45891</v>
+        <v>45892</v>
       </c>
       <c r="B55">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C55">
         <v>0.028</v>
@@ -1675,10 +1675,10 @@
         <v>45892</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C56">
-        <v>0.023</v>
+        <v>0.028</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1689,10 +1689,10 @@
         <v>45892</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C57">
-        <v>0.023</v>
+        <v>0.028</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,10 +1700,10 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58">
         <v>0.023</v>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B59">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C59">
         <v>0.023</v>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C60">
         <v>0.023</v>
@@ -1742,10 +1742,10 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B61">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C61">
         <v>0.023</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B62">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C62">
-        <v>0.07099999999999999</v>
+        <v>0.023</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B63">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C63">
-        <v>0.409</v>
+        <v>0.023</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B64">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C64">
-        <v>0.906</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B65">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C65">
-        <v>1.397</v>
+        <v>0.488</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B66">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C66">
-        <v>1.916</v>
+        <v>0.957</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B67">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C67">
-        <v>2.026</v>
+        <v>1.875</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B68">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C68">
-        <v>2.172</v>
+        <v>2.488</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B69">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C69">
-        <v>2.149</v>
+        <v>3.455</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B70">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C70">
-        <v>1.992</v>
+        <v>3.617</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B71">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C71">
-        <v>1.648</v>
+        <v>3.12</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B72">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C72">
-        <v>1.439</v>
+        <v>2.997</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B73">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C73">
-        <v>0.998</v>
+        <v>2.453</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B74">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C74">
-        <v>0.494</v>
+        <v>1.934</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B75">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C75">
-        <v>0.47</v>
+        <v>1.09</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B76">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C76">
-        <v>0.126</v>
+        <v>0.575</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B77">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C77">
-        <v>0.028</v>
+        <v>0.48</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B78">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C78">
-        <v>0.028</v>
+        <v>0.222</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45892</v>
+        <v>45893</v>
       </c>
       <c r="B79">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C79">
-        <v>0.028</v>
+        <v>0.124</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2011,10 +2011,10 @@
         <v>45893</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C80">
-        <v>0.023</v>
+        <v>0.124</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2025,10 +2025,10 @@
         <v>45893</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C81">
-        <v>0.023</v>
+        <v>0.124</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C82">
-        <v>0.023</v>
+        <v>0.135</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B83">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C83">
-        <v>0.023</v>
+        <v>0.135</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B84">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C84">
-        <v>0.023</v>
+        <v>0.135</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B85">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C85">
-        <v>0.023</v>
+        <v>0.135</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B86">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C86">
-        <v>0.046</v>
+        <v>0.135</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B87">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C87">
-        <v>0.302</v>
+        <v>0.048</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B88">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C88">
-        <v>0.828</v>
+        <v>0.15</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B89">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C89">
-        <v>1.46</v>
+        <v>0.502</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B90">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C90">
-        <v>2.079</v>
+        <v>1.368</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B91">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C91">
-        <v>2.407</v>
+        <v>2.091</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B92">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C92">
-        <v>2.708</v>
+        <v>3.045</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B93">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C93">
-        <v>2.865</v>
+        <v>3.833</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B94">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C94">
-        <v>3.069</v>
+        <v>3.168</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B95">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C95">
-        <v>2.984</v>
+        <v>4.1</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B96">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C96">
-        <v>2.409</v>
+        <v>3.93</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B97">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C97">
-        <v>1.873</v>
+        <v>3.423</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B98">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C98">
-        <v>0.967</v>
+        <v>2.567</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B99">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C99">
-        <v>0.489</v>
+        <v>1.907</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B100">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C100">
-        <v>0.236</v>
+        <v>0.967</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B101">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C101">
-        <v>0.141</v>
+        <v>0.489</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B102">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C102">
-        <v>0.042</v>
+        <v>0.219</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45893</v>
+        <v>45894</v>
       </c>
       <c r="B103">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C103">
-        <v>0.028</v>
+        <v>0.141</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2347,10 +2347,10 @@
         <v>45894</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C104">
-        <v>0.023</v>
+        <v>0.042</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2361,10 +2361,10 @@
         <v>45894</v>
       </c>
       <c r="B105">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C105">
-        <v>0.023</v>
+        <v>0.028</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,10 +2372,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B106">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C106">
         <v>0.023</v>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B107">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C107">
         <v>0.023</v>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B108">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C108">
         <v>0.023</v>
@@ -2414,10 +2414,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B109">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C109">
         <v>0.023</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B110">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C110">
-        <v>0.1</v>
+        <v>0.023</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B111">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C111">
-        <v>0.497</v>
+        <v>0.048</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B112">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C112">
-        <v>1.585</v>
+        <v>0.147</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B113">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C113">
-        <v>1.986</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B114">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C114">
-        <v>2.378</v>
+        <v>1.555</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B115">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C115">
-        <v>2.708</v>
+        <v>2.065</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B116">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C116">
-        <v>2.874</v>
+        <v>2.803</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B117">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C117">
-        <v>2.997</v>
+        <v>3.348</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B118">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C118">
-        <v>2.984</v>
+        <v>3.583</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B119">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C119">
-        <v>2.501</v>
+        <v>3.62</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B120">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C120">
-        <v>2.279</v>
+        <v>3.62</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B121">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C121">
-        <v>1.873</v>
+        <v>3.448</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B122">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C122">
-        <v>0.983</v>
+        <v>2.552</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B123">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C123">
-        <v>0.489</v>
+        <v>1.963</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B124">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C124">
-        <v>0.219</v>
+        <v>0.983</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B125">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C125">
-        <v>0.124</v>
+        <v>0.544</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B126">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C126">
-        <v>0.124</v>
+        <v>0.219</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,10 +2666,10 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45894</v>
+        <v>45895</v>
       </c>
       <c r="B127">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C127">
         <v>0.124</v>
@@ -2683,10 +2683,10 @@
         <v>45895</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C128">
-        <v>0.135</v>
+        <v>0.124</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2697,10 +2697,10 @@
         <v>45895</v>
       </c>
       <c r="B129">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C129">
-        <v>0.135</v>
+        <v>0.124</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,10 +2708,10 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B130">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C130">
         <v>0.135</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B131">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C131">
         <v>0.135</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B132">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C132">
         <v>0.135</v>
@@ -2750,10 +2750,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B133">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C133">
         <v>0.135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B134">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C134">
-        <v>0.15</v>
+        <v>0.135</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B135">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C135">
-        <v>0.517</v>
+        <v>0.135</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B136">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C136">
-        <v>1.376</v>
+        <v>0.15</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B137">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C137">
-        <v>1.986</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B138">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C138">
-        <v>2.657</v>
+        <v>1.561</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B139">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C139">
-        <v>3.348</v>
+        <v>2.065</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B140">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C140">
-        <v>3.427</v>
+        <v>2.803</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B141">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C141">
-        <v>3.62</v>
+        <v>3.348</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B142">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C142">
-        <v>3.496</v>
+        <v>3.468</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B143">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C143">
-        <v>3.166</v>
+        <v>3.62</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B144">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C144">
-        <v>2.402</v>
+        <v>3.311</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B145">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C145">
-        <v>1.907</v>
+        <v>3.192</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B146">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C146">
-        <v>0.983</v>
+        <v>2.402</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B147">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C147">
-        <v>0.544</v>
+        <v>1.873</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B148">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C148">
-        <v>0.219</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B149">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C149">
-        <v>0.124</v>
+        <v>0.483</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B150">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C150">
-        <v>0.124</v>
+        <v>0.225</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,10 +3002,10 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="B151">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C151">
         <v>0.124</v>
@@ -3019,10 +3019,10 @@
         <v>45896</v>
       </c>
       <c r="B152">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C152">
-        <v>0.135</v>
+        <v>0.124</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3033,10 +3033,10 @@
         <v>45896</v>
       </c>
       <c r="B153">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C153">
-        <v>0.135</v>
+        <v>0.124</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,10 +3044,10 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B154">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C154">
         <v>0.135</v>
@@ -3058,10 +3058,10 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B155">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C155">
         <v>0.135</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B156">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C156">
         <v>0.135</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B157">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C157">
         <v>0.135</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B158">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C158">
-        <v>0.15</v>
+        <v>0.048</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B159">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C159">
-        <v>0.443</v>
+        <v>0.048</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B160">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C160">
-        <v>1.025</v>
+        <v>0.15</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B161">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C161">
-        <v>1.697</v>
+        <v>0.538</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B162">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C162">
-        <v>1.999</v>
+        <v>1.376</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B163">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C163">
-        <v>2.28</v>
+        <v>2.194</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B164">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C164">
-        <v>2.657</v>
+        <v>2.779</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B165">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C165">
-        <v>2.997</v>
+        <v>3.066</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B166">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C166">
-        <v>3.147</v>
+        <v>3.348</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B167">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C167">
-        <v>3.09</v>
+        <v>3.496</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B168">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C168">
-        <v>2.358</v>
+        <v>3.38</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B169">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C169">
-        <v>1.907</v>
+        <v>2.997</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45896</v>
+        <v>45897</v>
       </c>
       <c r="B170">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C170">
-        <v>0.983</v>
+        <v>2.395</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
retraining the models for Elnet and 3D Steel
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>21.08.202517</t>
-  </si>
-  <si>
-    <t>21.08.202518</t>
-  </si>
-  <si>
-    <t>21.08.202519</t>
-  </si>
-  <si>
-    <t>21.08.202520</t>
-  </si>
-  <si>
-    <t>21.08.202521</t>
-  </si>
-  <si>
-    <t>21.08.202522</t>
-  </si>
-  <si>
-    <t>21.08.202523</t>
-  </si>
-  <si>
-    <t>21.08.202524</t>
-  </si>
-  <si>
-    <t>22.08.20251</t>
-  </si>
-  <si>
-    <t>22.08.20252</t>
-  </si>
-  <si>
-    <t>22.08.20253</t>
-  </si>
-  <si>
-    <t>22.08.20254</t>
-  </si>
-  <si>
-    <t>22.08.20255</t>
-  </si>
-  <si>
-    <t>22.08.20256</t>
-  </si>
-  <si>
-    <t>22.08.20257</t>
-  </si>
-  <si>
-    <t>22.08.20258</t>
-  </si>
-  <si>
-    <t>22.08.20259</t>
-  </si>
-  <si>
-    <t>22.08.202510</t>
-  </si>
-  <si>
-    <t>22.08.202511</t>
-  </si>
-  <si>
-    <t>22.08.202512</t>
-  </si>
-  <si>
-    <t>22.08.202513</t>
-  </si>
-  <si>
-    <t>22.08.202514</t>
-  </si>
-  <si>
-    <t>22.08.202515</t>
-  </si>
-  <si>
-    <t>22.08.202516</t>
-  </si>
-  <si>
-    <t>22.08.202517</t>
-  </si>
-  <si>
-    <t>22.08.202518</t>
-  </si>
-  <si>
-    <t>22.08.202519</t>
-  </si>
-  <si>
-    <t>22.08.202520</t>
-  </si>
-  <si>
-    <t>22.08.202521</t>
-  </si>
-  <si>
-    <t>22.08.202522</t>
-  </si>
-  <si>
-    <t>22.08.202523</t>
-  </si>
-  <si>
-    <t>22.08.202524</t>
-  </si>
-  <si>
-    <t>23.08.20251</t>
-  </si>
-  <si>
-    <t>23.08.20252</t>
-  </si>
-  <si>
-    <t>23.08.20253</t>
-  </si>
-  <si>
-    <t>23.08.20254</t>
-  </si>
-  <si>
-    <t>23.08.20255</t>
-  </si>
-  <si>
-    <t>23.08.20256</t>
-  </si>
-  <si>
-    <t>23.08.20257</t>
-  </si>
-  <si>
-    <t>23.08.20258</t>
-  </si>
-  <si>
-    <t>23.08.20259</t>
-  </si>
-  <si>
-    <t>23.08.202510</t>
-  </si>
-  <si>
-    <t>23.08.202511</t>
-  </si>
-  <si>
-    <t>23.08.202512</t>
-  </si>
-  <si>
-    <t>23.08.202513</t>
-  </si>
-  <si>
-    <t>23.08.202514</t>
-  </si>
-  <si>
-    <t>23.08.202515</t>
-  </si>
-  <si>
-    <t>23.08.202516</t>
-  </si>
-  <si>
-    <t>23.08.202517</t>
-  </si>
-  <si>
-    <t>23.08.202518</t>
-  </si>
-  <si>
-    <t>23.08.202519</t>
-  </si>
-  <si>
-    <t>23.08.202520</t>
-  </si>
-  <si>
-    <t>23.08.202521</t>
-  </si>
-  <si>
-    <t>23.08.202522</t>
-  </si>
-  <si>
-    <t>23.08.202523</t>
-  </si>
-  <si>
-    <t>23.08.202524</t>
-  </si>
-  <si>
-    <t>24.08.20251</t>
-  </si>
-  <si>
-    <t>24.08.20252</t>
-  </si>
-  <si>
-    <t>24.08.20253</t>
-  </si>
-  <si>
-    <t>24.08.20254</t>
-  </si>
-  <si>
-    <t>24.08.20255</t>
-  </si>
-  <si>
-    <t>24.08.20256</t>
-  </si>
-  <si>
-    <t>24.08.20257</t>
-  </si>
-  <si>
-    <t>24.08.20258</t>
-  </si>
-  <si>
-    <t>24.08.20259</t>
-  </si>
-  <si>
-    <t>24.08.202510</t>
-  </si>
-  <si>
-    <t>24.08.202511</t>
-  </si>
-  <si>
-    <t>24.08.202512</t>
-  </si>
-  <si>
-    <t>24.08.202513</t>
-  </si>
-  <si>
-    <t>24.08.202514</t>
-  </si>
-  <si>
-    <t>24.08.202515</t>
-  </si>
-  <si>
-    <t>24.08.202516</t>
-  </si>
-  <si>
-    <t>24.08.202517</t>
-  </si>
-  <si>
-    <t>24.08.202518</t>
-  </si>
-  <si>
-    <t>24.08.202519</t>
-  </si>
-  <si>
-    <t>24.08.202520</t>
-  </si>
-  <si>
-    <t>24.08.202521</t>
-  </si>
-  <si>
-    <t>24.08.202522</t>
-  </si>
-  <si>
-    <t>24.08.202523</t>
-  </si>
-  <si>
-    <t>24.08.202524</t>
-  </si>
-  <si>
-    <t>25.08.20251</t>
-  </si>
-  <si>
-    <t>25.08.20252</t>
-  </si>
-  <si>
-    <t>25.08.20253</t>
-  </si>
-  <si>
-    <t>25.08.20254</t>
-  </si>
-  <si>
-    <t>25.08.20255</t>
-  </si>
-  <si>
-    <t>25.08.20256</t>
-  </si>
-  <si>
-    <t>25.08.20257</t>
-  </si>
-  <si>
-    <t>25.08.20258</t>
-  </si>
-  <si>
-    <t>25.08.20259</t>
-  </si>
-  <si>
-    <t>25.08.202510</t>
-  </si>
-  <si>
-    <t>25.08.202511</t>
-  </si>
-  <si>
-    <t>25.08.202512</t>
-  </si>
-  <si>
-    <t>25.08.202513</t>
-  </si>
-  <si>
-    <t>25.08.202514</t>
-  </si>
-  <si>
-    <t>25.08.202515</t>
-  </si>
-  <si>
-    <t>25.08.202516</t>
-  </si>
-  <si>
-    <t>25.08.202517</t>
-  </si>
-  <si>
-    <t>25.08.202518</t>
-  </si>
-  <si>
-    <t>25.08.202519</t>
-  </si>
-  <si>
-    <t>25.08.202520</t>
-  </si>
-  <si>
-    <t>25.08.202521</t>
-  </si>
-  <si>
-    <t>25.08.202522</t>
-  </si>
-  <si>
-    <t>25.08.202523</t>
-  </si>
-  <si>
-    <t>25.08.202524</t>
-  </si>
-  <si>
-    <t>26.08.20251</t>
-  </si>
-  <si>
-    <t>26.08.20252</t>
-  </si>
-  <si>
-    <t>26.08.20253</t>
-  </si>
-  <si>
-    <t>26.08.20254</t>
-  </si>
-  <si>
-    <t>26.08.20255</t>
-  </si>
-  <si>
-    <t>26.08.20256</t>
-  </si>
-  <si>
-    <t>26.08.20257</t>
-  </si>
-  <si>
-    <t>26.08.20258</t>
-  </si>
-  <si>
-    <t>26.08.20259</t>
-  </si>
-  <si>
-    <t>26.08.202510</t>
-  </si>
-  <si>
-    <t>26.08.202511</t>
-  </si>
-  <si>
-    <t>26.08.202512</t>
-  </si>
-  <si>
-    <t>26.08.202513</t>
-  </si>
-  <si>
-    <t>26.08.202514</t>
-  </si>
-  <si>
-    <t>26.08.202515</t>
-  </si>
-  <si>
-    <t>26.08.202516</t>
-  </si>
-  <si>
-    <t>26.08.202517</t>
-  </si>
-  <si>
-    <t>26.08.202518</t>
-  </si>
-  <si>
-    <t>26.08.202519</t>
-  </si>
-  <si>
-    <t>26.08.202520</t>
-  </si>
-  <si>
-    <t>26.08.202521</t>
-  </si>
-  <si>
-    <t>26.08.202522</t>
-  </si>
-  <si>
-    <t>26.08.202523</t>
-  </si>
-  <si>
-    <t>26.08.202524</t>
-  </si>
-  <si>
-    <t>27.08.20251</t>
-  </si>
-  <si>
-    <t>27.08.20252</t>
-  </si>
-  <si>
-    <t>27.08.20253</t>
-  </si>
-  <si>
-    <t>27.08.20254</t>
-  </si>
-  <si>
-    <t>27.08.20255</t>
-  </si>
-  <si>
-    <t>27.08.20256</t>
-  </si>
-  <si>
-    <t>27.08.20257</t>
-  </si>
-  <si>
-    <t>27.08.20258</t>
-  </si>
-  <si>
-    <t>27.08.20259</t>
-  </si>
-  <si>
-    <t>27.08.202510</t>
-  </si>
-  <si>
-    <t>27.08.202511</t>
-  </si>
-  <si>
-    <t>27.08.202512</t>
-  </si>
-  <si>
-    <t>27.08.202513</t>
-  </si>
-  <si>
-    <t>27.08.202514</t>
-  </si>
-  <si>
-    <t>27.08.202515</t>
-  </si>
-  <si>
-    <t>27.08.202516</t>
-  </si>
-  <si>
-    <t>27.08.202517</t>
-  </si>
-  <si>
-    <t>27.08.202518</t>
-  </si>
-  <si>
-    <t>27.08.202519</t>
-  </si>
-  <si>
-    <t>27.08.202520</t>
-  </si>
-  <si>
-    <t>27.08.202521</t>
-  </si>
-  <si>
-    <t>27.08.202522</t>
-  </si>
-  <si>
-    <t>27.08.202523</t>
-  </si>
-  <si>
-    <t>27.08.202524</t>
-  </si>
-  <si>
-    <t>28.08.20251</t>
-  </si>
-  <si>
-    <t>28.08.20252</t>
-  </si>
-  <si>
-    <t>28.08.20253</t>
-  </si>
-  <si>
-    <t>28.08.20254</t>
-  </si>
-  <si>
-    <t>28.08.20255</t>
-  </si>
-  <si>
-    <t>28.08.20256</t>
-  </si>
-  <si>
-    <t>28.08.20257</t>
-  </si>
-  <si>
-    <t>28.08.20258</t>
-  </si>
-  <si>
-    <t>28.08.20259</t>
-  </si>
-  <si>
-    <t>28.08.202510</t>
-  </si>
-  <si>
-    <t>28.08.202511</t>
-  </si>
-  <si>
-    <t>28.08.202512</t>
-  </si>
-  <si>
-    <t>28.08.202513</t>
-  </si>
-  <si>
-    <t>28.08.202514</t>
-  </si>
-  <si>
-    <t>28.08.202515</t>
-  </si>
-  <si>
-    <t>28.08.202516</t>
-  </si>
-  <si>
-    <t>28.08.202517</t>
+    <t>18.09.202511</t>
+  </si>
+  <si>
+    <t>18.09.202512</t>
+  </si>
+  <si>
+    <t>18.09.202513</t>
+  </si>
+  <si>
+    <t>18.09.202514</t>
+  </si>
+  <si>
+    <t>18.09.202515</t>
+  </si>
+  <si>
+    <t>18.09.202516</t>
+  </si>
+  <si>
+    <t>18.09.202517</t>
+  </si>
+  <si>
+    <t>18.09.202518</t>
+  </si>
+  <si>
+    <t>18.09.202519</t>
+  </si>
+  <si>
+    <t>18.09.202520</t>
+  </si>
+  <si>
+    <t>18.09.202521</t>
+  </si>
+  <si>
+    <t>18.09.202522</t>
+  </si>
+  <si>
+    <t>18.09.202523</t>
+  </si>
+  <si>
+    <t>18.09.202524</t>
+  </si>
+  <si>
+    <t>19.09.20251</t>
+  </si>
+  <si>
+    <t>19.09.20252</t>
+  </si>
+  <si>
+    <t>19.09.20253</t>
+  </si>
+  <si>
+    <t>19.09.20254</t>
+  </si>
+  <si>
+    <t>19.09.20255</t>
+  </si>
+  <si>
+    <t>19.09.20256</t>
+  </si>
+  <si>
+    <t>19.09.20257</t>
+  </si>
+  <si>
+    <t>19.09.20258</t>
+  </si>
+  <si>
+    <t>19.09.20259</t>
+  </si>
+  <si>
+    <t>19.09.202510</t>
+  </si>
+  <si>
+    <t>19.09.202511</t>
+  </si>
+  <si>
+    <t>19.09.202512</t>
+  </si>
+  <si>
+    <t>19.09.202513</t>
+  </si>
+  <si>
+    <t>19.09.202514</t>
+  </si>
+  <si>
+    <t>19.09.202515</t>
+  </si>
+  <si>
+    <t>19.09.202516</t>
+  </si>
+  <si>
+    <t>19.09.202517</t>
+  </si>
+  <si>
+    <t>19.09.202518</t>
+  </si>
+  <si>
+    <t>19.09.202519</t>
+  </si>
+  <si>
+    <t>19.09.202520</t>
+  </si>
+  <si>
+    <t>19.09.202521</t>
+  </si>
+  <si>
+    <t>19.09.202522</t>
+  </si>
+  <si>
+    <t>19.09.202523</t>
+  </si>
+  <si>
+    <t>19.09.202524</t>
+  </si>
+  <si>
+    <t>20.09.20251</t>
+  </si>
+  <si>
+    <t>20.09.20252</t>
+  </si>
+  <si>
+    <t>20.09.20253</t>
+  </si>
+  <si>
+    <t>20.09.20254</t>
+  </si>
+  <si>
+    <t>20.09.20255</t>
+  </si>
+  <si>
+    <t>20.09.20256</t>
+  </si>
+  <si>
+    <t>20.09.20257</t>
+  </si>
+  <si>
+    <t>20.09.20258</t>
+  </si>
+  <si>
+    <t>20.09.20259</t>
+  </si>
+  <si>
+    <t>20.09.202510</t>
+  </si>
+  <si>
+    <t>20.09.202511</t>
+  </si>
+  <si>
+    <t>20.09.202512</t>
+  </si>
+  <si>
+    <t>20.09.202513</t>
+  </si>
+  <si>
+    <t>20.09.202514</t>
+  </si>
+  <si>
+    <t>20.09.202515</t>
+  </si>
+  <si>
+    <t>20.09.202516</t>
+  </si>
+  <si>
+    <t>20.09.202517</t>
+  </si>
+  <si>
+    <t>20.09.202518</t>
+  </si>
+  <si>
+    <t>20.09.202519</t>
+  </si>
+  <si>
+    <t>20.09.202520</t>
+  </si>
+  <si>
+    <t>20.09.202521</t>
+  </si>
+  <si>
+    <t>20.09.202522</t>
+  </si>
+  <si>
+    <t>20.09.202523</t>
+  </si>
+  <si>
+    <t>20.09.202524</t>
+  </si>
+  <si>
+    <t>21.09.20251</t>
+  </si>
+  <si>
+    <t>21.09.20252</t>
+  </si>
+  <si>
+    <t>21.09.20253</t>
+  </si>
+  <si>
+    <t>21.09.20254</t>
+  </si>
+  <si>
+    <t>21.09.20255</t>
+  </si>
+  <si>
+    <t>21.09.20256</t>
+  </si>
+  <si>
+    <t>21.09.20257</t>
+  </si>
+  <si>
+    <t>21.09.20258</t>
+  </si>
+  <si>
+    <t>21.09.20259</t>
+  </si>
+  <si>
+    <t>21.09.202510</t>
+  </si>
+  <si>
+    <t>21.09.202511</t>
+  </si>
+  <si>
+    <t>21.09.202512</t>
+  </si>
+  <si>
+    <t>21.09.202513</t>
+  </si>
+  <si>
+    <t>21.09.202514</t>
+  </si>
+  <si>
+    <t>21.09.202515</t>
+  </si>
+  <si>
+    <t>21.09.202516</t>
+  </si>
+  <si>
+    <t>21.09.202517</t>
+  </si>
+  <si>
+    <t>21.09.202518</t>
+  </si>
+  <si>
+    <t>21.09.202519</t>
+  </si>
+  <si>
+    <t>21.09.202520</t>
+  </si>
+  <si>
+    <t>21.09.202521</t>
+  </si>
+  <si>
+    <t>21.09.202522</t>
+  </si>
+  <si>
+    <t>21.09.202523</t>
+  </si>
+  <si>
+    <t>21.09.202524</t>
+  </si>
+  <si>
+    <t>22.09.20251</t>
+  </si>
+  <si>
+    <t>22.09.20252</t>
+  </si>
+  <si>
+    <t>22.09.20253</t>
+  </si>
+  <si>
+    <t>22.09.20254</t>
+  </si>
+  <si>
+    <t>22.09.20255</t>
+  </si>
+  <si>
+    <t>22.09.20256</t>
+  </si>
+  <si>
+    <t>22.09.20257</t>
+  </si>
+  <si>
+    <t>22.09.20258</t>
+  </si>
+  <si>
+    <t>22.09.20259</t>
+  </si>
+  <si>
+    <t>22.09.202510</t>
+  </si>
+  <si>
+    <t>22.09.202511</t>
+  </si>
+  <si>
+    <t>22.09.202512</t>
+  </si>
+  <si>
+    <t>22.09.202513</t>
+  </si>
+  <si>
+    <t>22.09.202514</t>
+  </si>
+  <si>
+    <t>22.09.202515</t>
+  </si>
+  <si>
+    <t>22.09.202516</t>
+  </si>
+  <si>
+    <t>22.09.202517</t>
+  </si>
+  <si>
+    <t>22.09.202518</t>
+  </si>
+  <si>
+    <t>22.09.202519</t>
+  </si>
+  <si>
+    <t>22.09.202520</t>
+  </si>
+  <si>
+    <t>22.09.202521</t>
+  </si>
+  <si>
+    <t>22.09.202522</t>
+  </si>
+  <si>
+    <t>22.09.202523</t>
+  </si>
+  <si>
+    <t>22.09.202524</t>
+  </si>
+  <si>
+    <t>23.09.20251</t>
+  </si>
+  <si>
+    <t>23.09.20252</t>
+  </si>
+  <si>
+    <t>23.09.20253</t>
+  </si>
+  <si>
+    <t>23.09.20254</t>
+  </si>
+  <si>
+    <t>23.09.20255</t>
+  </si>
+  <si>
+    <t>23.09.20256</t>
+  </si>
+  <si>
+    <t>23.09.20257</t>
+  </si>
+  <si>
+    <t>23.09.20258</t>
+  </si>
+  <si>
+    <t>23.09.20259</t>
+  </si>
+  <si>
+    <t>23.09.202510</t>
+  </si>
+  <si>
+    <t>23.09.202511</t>
+  </si>
+  <si>
+    <t>23.09.202512</t>
+  </si>
+  <si>
+    <t>23.09.202513</t>
+  </si>
+  <si>
+    <t>23.09.202514</t>
+  </si>
+  <si>
+    <t>23.09.202515</t>
+  </si>
+  <si>
+    <t>23.09.202516</t>
+  </si>
+  <si>
+    <t>23.09.202517</t>
+  </si>
+  <si>
+    <t>23.09.202518</t>
+  </si>
+  <si>
+    <t>23.09.202519</t>
+  </si>
+  <si>
+    <t>23.09.202520</t>
+  </si>
+  <si>
+    <t>23.09.202521</t>
+  </si>
+  <si>
+    <t>23.09.202522</t>
+  </si>
+  <si>
+    <t>23.09.202523</t>
+  </si>
+  <si>
+    <t>23.09.202524</t>
+  </si>
+  <si>
+    <t>24.09.20251</t>
+  </si>
+  <si>
+    <t>24.09.20252</t>
+  </si>
+  <si>
+    <t>24.09.20253</t>
+  </si>
+  <si>
+    <t>24.09.20254</t>
+  </si>
+  <si>
+    <t>24.09.20255</t>
+  </si>
+  <si>
+    <t>24.09.20256</t>
+  </si>
+  <si>
+    <t>24.09.20257</t>
+  </si>
+  <si>
+    <t>24.09.20258</t>
+  </si>
+  <si>
+    <t>24.09.20259</t>
+  </si>
+  <si>
+    <t>24.09.202510</t>
+  </si>
+  <si>
+    <t>24.09.202511</t>
+  </si>
+  <si>
+    <t>24.09.202512</t>
+  </si>
+  <si>
+    <t>24.09.202513</t>
+  </si>
+  <si>
+    <t>24.09.202514</t>
+  </si>
+  <si>
+    <t>24.09.202515</t>
+  </si>
+  <si>
+    <t>24.09.202516</t>
+  </si>
+  <si>
+    <t>24.09.202517</t>
+  </si>
+  <si>
+    <t>24.09.202518</t>
+  </si>
+  <si>
+    <t>24.09.202519</t>
+  </si>
+  <si>
+    <t>24.09.202520</t>
+  </si>
+  <si>
+    <t>24.09.202521</t>
+  </si>
+  <si>
+    <t>24.09.202522</t>
+  </si>
+  <si>
+    <t>24.09.202523</t>
+  </si>
+  <si>
+    <t>24.09.202524</t>
+  </si>
+  <si>
+    <t>25.09.20251</t>
+  </si>
+  <si>
+    <t>25.09.20252</t>
+  </si>
+  <si>
+    <t>25.09.20253</t>
+  </si>
+  <si>
+    <t>25.09.20254</t>
+  </si>
+  <si>
+    <t>25.09.20255</t>
+  </si>
+  <si>
+    <t>25.09.20256</t>
+  </si>
+  <si>
+    <t>25.09.20257</t>
+  </si>
+  <si>
+    <t>25.09.20258</t>
+  </si>
+  <si>
+    <t>25.09.20259</t>
+  </si>
+  <si>
+    <t>25.09.202510</t>
+  </si>
+  <si>
+    <t>25.09.202511</t>
   </si>
 </sst>
 </file>
@@ -916,13 +916,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="B2">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C2">
-        <v>0.175</v>
+        <v>0.034</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="B3">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>0.175</v>
+        <v>0.034</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="B4">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>0.999</v>
+        <v>3.386</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>0.635</v>
+        <v>3.267</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="B6">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>0.305</v>
+        <v>3.226</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="B7">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>0.141</v>
+        <v>2.949</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="B8">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>0.141</v>
+        <v>1.972</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="B9">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9">
-        <v>0.141</v>
+        <v>1.282</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45891</v>
+        <v>45918</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>0.135</v>
+        <v>0.465</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45891</v>
+        <v>45918</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>0.135</v>
+        <v>0.235</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45891</v>
+        <v>45918</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C12">
-        <v>0.135</v>
+        <v>0.068</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45891</v>
+        <v>45918</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C13">
-        <v>0.048</v>
+        <v>0.015</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45891</v>
+        <v>45918</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C14">
-        <v>0.023</v>
+        <v>0.015</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45891</v>
+        <v>45918</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>0.023</v>
+        <v>0.02</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>0.1</v>
+        <v>0.018</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>0.471</v>
+        <v>0.018</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>1.067</v>
+        <v>0.018</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>1.613</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B20">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>1.862</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C21">
-        <v>1.986</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B22">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>2.436</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B23">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>2.424</v>
+        <v>0.3</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B24">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C24">
-        <v>2.26</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B25">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C25">
-        <v>1.923</v>
+        <v>2.183</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B26">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C26">
-        <v>1.451</v>
+        <v>2.891</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B27">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C27">
-        <v>1.04</v>
+        <v>3.411</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B28">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C28">
-        <v>0.509</v>
+        <v>3.72</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B29">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C29">
-        <v>0.47</v>
+        <v>3.472</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B30">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C30">
-        <v>0.126</v>
+        <v>3.265</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B31">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C31">
-        <v>0.028</v>
+        <v>3.1</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B32">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C32">
-        <v>0.028</v>
+        <v>1.93</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="B33">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C33">
-        <v>0.028</v>
+        <v>1.193</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45892</v>
+        <v>45919</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C34">
-        <v>0.023</v>
+        <v>0.474</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45892</v>
+        <v>45919</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C35">
-        <v>0.023</v>
+        <v>0.213</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45892</v>
+        <v>45919</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C36">
-        <v>0.023</v>
+        <v>0.075</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45892</v>
+        <v>45919</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C37">
-        <v>0.023</v>
+        <v>0.022</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45892</v>
+        <v>45919</v>
       </c>
       <c r="B38">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C38">
-        <v>0.023</v>
+        <v>0.027</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45892</v>
+        <v>45919</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C39">
-        <v>0.023</v>
+        <v>0.027</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>0.046</v>
+        <v>0.025</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C41">
-        <v>0.303</v>
+        <v>0.018</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B42">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C42">
-        <v>0.864</v>
+        <v>0.018</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B43">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C43">
-        <v>1.434</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B44">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C44">
-        <v>1.828</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B45">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C45">
-        <v>1.799</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B46">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C46">
-        <v>1.822</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B47">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C47">
-        <v>1.964</v>
+        <v>0.392</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B48">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C48">
-        <v>1.656</v>
+        <v>1.108</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B49">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C49">
-        <v>1.4</v>
+        <v>2.107</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B50">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C50">
-        <v>0.978</v>
+        <v>2.799</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B51">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C51">
-        <v>0.8169999999999999</v>
+        <v>3.525</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B52">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C52">
-        <v>0.412</v>
+        <v>3.536</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B53">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C53">
-        <v>0.47</v>
+        <v>3.457</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B54">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C54">
-        <v>0.126</v>
+        <v>3.284</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B55">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C55">
-        <v>0.028</v>
+        <v>3.012</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B56">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C56">
-        <v>0.028</v>
+        <v>2.279</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45892</v>
+        <v>45920</v>
       </c>
       <c r="B57">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C57">
-        <v>0.028</v>
+        <v>1.193</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45893</v>
+        <v>45920</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C58">
-        <v>0.023</v>
+        <v>0.471</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45893</v>
+        <v>45920</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C59">
-        <v>0.023</v>
+        <v>0.213</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45893</v>
+        <v>45920</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C60">
-        <v>0.023</v>
+        <v>0.075</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45893</v>
+        <v>45920</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C61">
-        <v>0.023</v>
+        <v>0.027</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45893</v>
+        <v>45920</v>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C62">
-        <v>0.023</v>
+        <v>0.027</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45893</v>
+        <v>45920</v>
       </c>
       <c r="B63">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C63">
-        <v>0.023</v>
+        <v>0.027</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C64">
-        <v>0.07099999999999999</v>
+        <v>0.025</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B65">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C65">
-        <v>0.488</v>
+        <v>0.025</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B66">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C66">
-        <v>0.957</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B67">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C67">
-        <v>1.875</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B68">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C68">
-        <v>2.488</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B69">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C69">
-        <v>3.455</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B70">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C70">
-        <v>3.617</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B71">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C71">
-        <v>3.12</v>
+        <v>0.392</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B72">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C72">
-        <v>2.997</v>
+        <v>0.819</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B73">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C73">
-        <v>2.453</v>
+        <v>2.046</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B74">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C74">
-        <v>1.934</v>
+        <v>2.837</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B75">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C75">
-        <v>1.09</v>
+        <v>3.513</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B76">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C76">
-        <v>0.575</v>
+        <v>3.742</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B77">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C77">
-        <v>0.48</v>
+        <v>3.529</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B78">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C78">
-        <v>0.222</v>
+        <v>3.337</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B79">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C79">
-        <v>0.124</v>
+        <v>3.057</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B80">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C80">
-        <v>0.124</v>
+        <v>2.237</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45893</v>
+        <v>45921</v>
       </c>
       <c r="B81">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C81">
-        <v>0.124</v>
+        <v>1.197</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45894</v>
+        <v>45921</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C82">
-        <v>0.135</v>
+        <v>0.436</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45894</v>
+        <v>45921</v>
       </c>
       <c r="B83">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C83">
-        <v>0.135</v>
+        <v>0.213</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45894</v>
+        <v>45921</v>
       </c>
       <c r="B84">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C84">
-        <v>0.135</v>
+        <v>0.075</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45894</v>
+        <v>45921</v>
       </c>
       <c r="B85">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C85">
-        <v>0.135</v>
+        <v>0.027</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45894</v>
+        <v>45921</v>
       </c>
       <c r="B86">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C86">
-        <v>0.135</v>
+        <v>0.027</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45894</v>
+        <v>45921</v>
       </c>
       <c r="B87">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C87">
-        <v>0.048</v>
+        <v>0.018</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B88">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C88">
-        <v>0.15</v>
+        <v>0.016</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B89">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C89">
-        <v>0.502</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B90">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C90">
-        <v>1.368</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B91">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C91">
-        <v>2.091</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B92">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C92">
-        <v>3.045</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B93">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C93">
-        <v>3.833</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B94">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C94">
-        <v>3.168</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B95">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C95">
-        <v>4.1</v>
+        <v>0.392</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B96">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C96">
-        <v>3.93</v>
+        <v>0.826</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B97">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C97">
-        <v>3.423</v>
+        <v>1.869</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B98">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C98">
-        <v>2.567</v>
+        <v>2.523</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B99">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C99">
-        <v>1.907</v>
+        <v>3.668</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B100">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C100">
-        <v>0.967</v>
+        <v>3.749</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B101">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C101">
-        <v>0.489</v>
+        <v>3.481</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B102">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C102">
-        <v>0.219</v>
+        <v>3.384</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B103">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C103">
-        <v>0.141</v>
+        <v>2.994</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B104">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C104">
-        <v>0.042</v>
+        <v>1.946</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45894</v>
+        <v>45922</v>
       </c>
       <c r="B105">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C105">
-        <v>0.028</v>
+        <v>1.122</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45895</v>
+        <v>45922</v>
       </c>
       <c r="B106">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C106">
-        <v>0.023</v>
+        <v>0.366</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45895</v>
+        <v>45922</v>
       </c>
       <c r="B107">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C107">
-        <v>0.023</v>
+        <v>0.213</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45895</v>
+        <v>45922</v>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C108">
-        <v>0.023</v>
+        <v>0.075</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45895</v>
+        <v>45922</v>
       </c>
       <c r="B109">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C109">
-        <v>0.023</v>
+        <v>0.022</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45895</v>
+        <v>45922</v>
       </c>
       <c r="B110">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C110">
-        <v>0.023</v>
+        <v>0.027</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45895</v>
+        <v>45922</v>
       </c>
       <c r="B111">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C111">
-        <v>0.048</v>
+        <v>0.02</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B112">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C112">
-        <v>0.147</v>
+        <v>0</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B113">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C113">
-        <v>0.5580000000000001</v>
+        <v>0</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B114">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C114">
-        <v>1.555</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B115">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C115">
-        <v>2.065</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B116">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C116">
-        <v>2.803</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B117">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C117">
-        <v>3.348</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B118">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C118">
-        <v>3.583</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B119">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C119">
-        <v>3.62</v>
+        <v>0.347</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B120">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C120">
-        <v>3.62</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B121">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C121">
-        <v>3.448</v>
+        <v>1.66</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B122">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C122">
-        <v>2.552</v>
+        <v>2.343</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B123">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C123">
-        <v>1.963</v>
+        <v>3.088</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B124">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C124">
-        <v>0.983</v>
+        <v>3.53</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B125">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C125">
-        <v>0.544</v>
+        <v>3.322</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B126">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C126">
-        <v>0.219</v>
+        <v>3.258</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B127">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C127">
-        <v>0.124</v>
+        <v>2.881</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B128">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C128">
-        <v>0.124</v>
+        <v>2.009</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45895</v>
+        <v>45923</v>
       </c>
       <c r="B129">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C129">
-        <v>0.124</v>
+        <v>1.021</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45896</v>
+        <v>45923</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C130">
-        <v>0.135</v>
+        <v>0.338</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45896</v>
+        <v>45923</v>
       </c>
       <c r="B131">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C131">
-        <v>0.135</v>
+        <v>0.205</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45896</v>
+        <v>45923</v>
       </c>
       <c r="B132">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C132">
-        <v>0.135</v>
+        <v>0.075</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45896</v>
+        <v>45923</v>
       </c>
       <c r="B133">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C133">
-        <v>0.135</v>
+        <v>0.022</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45896</v>
+        <v>45923</v>
       </c>
       <c r="B134">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C134">
-        <v>0.135</v>
+        <v>0.022</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45896</v>
+        <v>45923</v>
       </c>
       <c r="B135">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C135">
-        <v>0.135</v>
+        <v>0.027</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B136">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C136">
-        <v>0.15</v>
+        <v>0.025</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B137">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C137">
-        <v>0.5580000000000001</v>
+        <v>0.016</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B138">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C138">
-        <v>1.561</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B139">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C139">
-        <v>2.065</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B140">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C140">
-        <v>2.803</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B141">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C141">
-        <v>3.348</v>
+        <v>0</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B142">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C142">
-        <v>3.468</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B143">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C143">
-        <v>3.62</v>
+        <v>0.354</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B144">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C144">
-        <v>3.311</v>
+        <v>0.956</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B145">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C145">
-        <v>3.192</v>
+        <v>2.002</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B146">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C146">
-        <v>2.402</v>
+        <v>2.762</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B147">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C147">
-        <v>1.873</v>
+        <v>3.591</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B148">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C148">
-        <v>0.9370000000000001</v>
+        <v>3.551</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B149">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C149">
-        <v>0.483</v>
+        <v>3.414</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B150">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C150">
-        <v>0.225</v>
+        <v>3.345</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B151">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C151">
-        <v>0.124</v>
+        <v>2.968</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B152">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C152">
-        <v>0.124</v>
+        <v>1.815</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45896</v>
+        <v>45924</v>
       </c>
       <c r="B153">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C153">
-        <v>0.124</v>
+        <v>1.005</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45897</v>
+        <v>45924</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C154">
-        <v>0.135</v>
+        <v>0.289</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45897</v>
+        <v>45924</v>
       </c>
       <c r="B155">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C155">
-        <v>0.135</v>
+        <v>0.066</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45897</v>
+        <v>45924</v>
       </c>
       <c r="B156">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C156">
-        <v>0.135</v>
+        <v>0.066</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45897</v>
+        <v>45924</v>
       </c>
       <c r="B157">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C157">
-        <v>0.135</v>
+        <v>0.013</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45897</v>
+        <v>45924</v>
       </c>
       <c r="B158">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C158">
-        <v>0.048</v>
+        <v>0.022</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45897</v>
+        <v>45924</v>
       </c>
       <c r="B159">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C159">
-        <v>0.048</v>
+        <v>0.022</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B160">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C160">
-        <v>0.15</v>
+        <v>0.019</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B161">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C161">
-        <v>0.538</v>
+        <v>0.019</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B162">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C162">
-        <v>1.376</v>
+        <v>0.019</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B163">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C163">
-        <v>2.194</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B164">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C164">
-        <v>2.779</v>
+        <v>0.029</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B165">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C165">
-        <v>3.066</v>
+        <v>0.013</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B166">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C166">
-        <v>3.348</v>
+        <v>0.013</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B167">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C167">
-        <v>3.496</v>
+        <v>0.525</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B168">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C168">
-        <v>3.38</v>
+        <v>0.594</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B169">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C169">
-        <v>2.997</v>
+        <v>0.951</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="B170">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C170">
-        <v>2.395</v>
+        <v>1.731</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Retraining the models for 3D Steel and Elnet
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,102 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>18.09.202511</t>
-  </si>
-  <si>
-    <t>18.09.202512</t>
-  </si>
-  <si>
-    <t>18.09.202513</t>
-  </si>
-  <si>
-    <t>18.09.202514</t>
-  </si>
-  <si>
-    <t>18.09.202515</t>
-  </si>
-  <si>
-    <t>18.09.202516</t>
-  </si>
-  <si>
-    <t>18.09.202517</t>
-  </si>
-  <si>
-    <t>18.09.202518</t>
-  </si>
-  <si>
-    <t>18.09.202519</t>
-  </si>
-  <si>
-    <t>18.09.202520</t>
-  </si>
-  <si>
-    <t>18.09.202521</t>
-  </si>
-  <si>
-    <t>18.09.202522</t>
-  </si>
-  <si>
-    <t>18.09.202523</t>
-  </si>
-  <si>
-    <t>18.09.202524</t>
-  </si>
-  <si>
-    <t>19.09.20251</t>
-  </si>
-  <si>
-    <t>19.09.20252</t>
-  </si>
-  <si>
-    <t>19.09.20253</t>
-  </si>
-  <si>
-    <t>19.09.20254</t>
-  </si>
-  <si>
-    <t>19.09.20255</t>
-  </si>
-  <si>
-    <t>19.09.20256</t>
-  </si>
-  <si>
-    <t>19.09.20257</t>
-  </si>
-  <si>
-    <t>19.09.20258</t>
-  </si>
-  <si>
-    <t>19.09.20259</t>
-  </si>
-  <si>
-    <t>19.09.202510</t>
-  </si>
-  <si>
-    <t>19.09.202511</t>
-  </si>
-  <si>
-    <t>19.09.202512</t>
-  </si>
-  <si>
-    <t>19.09.202513</t>
-  </si>
-  <si>
-    <t>19.09.202514</t>
-  </si>
-  <si>
-    <t>19.09.202515</t>
-  </si>
-  <si>
-    <t>19.09.202516</t>
-  </si>
-  <si>
-    <t>19.09.202517</t>
-  </si>
-  <si>
-    <t>19.09.202518</t>
-  </si>
-  <si>
     <t>19.09.202519</t>
   </si>
   <si>
@@ -533,6 +437,102 @@
   </si>
   <si>
     <t>25.09.202511</t>
+  </si>
+  <si>
+    <t>25.09.202512</t>
+  </si>
+  <si>
+    <t>25.09.202513</t>
+  </si>
+  <si>
+    <t>25.09.202514</t>
+  </si>
+  <si>
+    <t>25.09.202515</t>
+  </si>
+  <si>
+    <t>25.09.202516</t>
+  </si>
+  <si>
+    <t>25.09.202517</t>
+  </si>
+  <si>
+    <t>25.09.202518</t>
+  </si>
+  <si>
+    <t>25.09.202519</t>
+  </si>
+  <si>
+    <t>25.09.202520</t>
+  </si>
+  <si>
+    <t>25.09.202521</t>
+  </si>
+  <si>
+    <t>25.09.202522</t>
+  </si>
+  <si>
+    <t>25.09.202523</t>
+  </si>
+  <si>
+    <t>25.09.202524</t>
+  </si>
+  <si>
+    <t>26.09.20251</t>
+  </si>
+  <si>
+    <t>26.09.20252</t>
+  </si>
+  <si>
+    <t>26.09.20253</t>
+  </si>
+  <si>
+    <t>26.09.20254</t>
+  </si>
+  <si>
+    <t>26.09.20255</t>
+  </si>
+  <si>
+    <t>26.09.20256</t>
+  </si>
+  <si>
+    <t>26.09.20257</t>
+  </si>
+  <si>
+    <t>26.09.20258</t>
+  </si>
+  <si>
+    <t>26.09.20259</t>
+  </si>
+  <si>
+    <t>26.09.202510</t>
+  </si>
+  <si>
+    <t>26.09.202511</t>
+  </si>
+  <si>
+    <t>26.09.202512</t>
+  </si>
+  <si>
+    <t>26.09.202513</t>
+  </si>
+  <si>
+    <t>26.09.202514</t>
+  </si>
+  <si>
+    <t>26.09.202515</t>
+  </si>
+  <si>
+    <t>26.09.202516</t>
+  </si>
+  <si>
+    <t>26.09.202517</t>
+  </si>
+  <si>
+    <t>26.09.202518</t>
+  </si>
+  <si>
+    <t>26.09.202519</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45918</v>
+        <v>45919</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>0.034</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45918</v>
+        <v>45919</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>0.034</v>
+        <v>0.039</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45918</v>
+        <v>45919</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>3.386</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45918</v>
+        <v>45919</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C5">
-        <v>3.267</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45918</v>
+        <v>45919</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C6">
-        <v>3.226</v>
+        <v>0.019</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45918</v>
+        <v>45919</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C7">
-        <v>2.949</v>
+        <v>0.02</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45918</v>
+        <v>45920</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>1.972</v>
+        <v>0.018</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45918</v>
+        <v>45920</v>
       </c>
       <c r="B9">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>1.282</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45918</v>
+        <v>45920</v>
       </c>
       <c r="B10">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>0.465</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45918</v>
+        <v>45920</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>0.235</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45918</v>
+        <v>45920</v>
       </c>
       <c r="B12">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>0.068</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45918</v>
+        <v>45920</v>
       </c>
       <c r="B13">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>0.015</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45918</v>
+        <v>45920</v>
       </c>
       <c r="B14">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>0.015</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45918</v>
+        <v>45920</v>
       </c>
       <c r="B15">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>0.02</v>
+        <v>0.392</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>0.018</v>
+        <v>1.117</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>0.018</v>
+        <v>1.814</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>0.018</v>
+        <v>2.597</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>3.545</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>3.468</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>3.254</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>3.174</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C23">
-        <v>0.3</v>
+        <v>2.622</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B24">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C24">
-        <v>0.9370000000000001</v>
+        <v>2.056</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C25">
-        <v>2.183</v>
+        <v>1.112</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B26">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C26">
-        <v>2.891</v>
+        <v>0.515</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C27">
-        <v>3.411</v>
+        <v>0.275</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B28">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C28">
-        <v>3.72</v>
+        <v>0.136</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B29">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C29">
-        <v>3.472</v>
+        <v>0.083</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B30">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C30">
-        <v>3.265</v>
+        <v>0.083</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45919</v>
+        <v>45920</v>
       </c>
       <c r="B31">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C31">
-        <v>3.1</v>
+        <v>0.089</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45919</v>
+        <v>45921</v>
       </c>
       <c r="B32">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <v>1.93</v>
+        <v>0.025</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45919</v>
+        <v>45921</v>
       </c>
       <c r="B33">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C33">
-        <v>1.193</v>
+        <v>0.016</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45919</v>
+        <v>45921</v>
       </c>
       <c r="B34">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C34">
-        <v>0.474</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45919</v>
+        <v>45921</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>0.213</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45919</v>
+        <v>45921</v>
       </c>
       <c r="B36">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C36">
-        <v>0.075</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45919</v>
+        <v>45921</v>
       </c>
       <c r="B37">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>0.022</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45919</v>
+        <v>45921</v>
       </c>
       <c r="B38">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C38">
-        <v>0.027</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45919</v>
+        <v>45921</v>
       </c>
       <c r="B39">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C39">
-        <v>0.027</v>
+        <v>0.392</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C40">
-        <v>0.025</v>
+        <v>0.851</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C41">
-        <v>0.018</v>
+        <v>1.818</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C42">
-        <v>0.018</v>
+        <v>2.683</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>3.668</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B44">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>3.568</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>3.248</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>3.063</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C47">
-        <v>0.392</v>
+        <v>2.509</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B48">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C48">
-        <v>1.108</v>
+        <v>1.874</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B49">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C49">
-        <v>2.107</v>
+        <v>1.018</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B50">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C50">
-        <v>2.799</v>
+        <v>0.42</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C51">
-        <v>3.525</v>
+        <v>0.213</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B52">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C52">
-        <v>3.536</v>
+        <v>0.075</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B53">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C53">
-        <v>3.457</v>
+        <v>0.027</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B54">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C54">
-        <v>3.284</v>
+        <v>0.027</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45920</v>
+        <v>45921</v>
       </c>
       <c r="B55">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C55">
-        <v>3.012</v>
+        <v>0.011</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45920</v>
+        <v>45922</v>
       </c>
       <c r="B56">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>2.279</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45920</v>
+        <v>45922</v>
       </c>
       <c r="B57">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C57">
-        <v>1.193</v>
+        <v>0</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45920</v>
+        <v>45922</v>
       </c>
       <c r="B58">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C58">
-        <v>0.471</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45920</v>
+        <v>45922</v>
       </c>
       <c r="B59">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C59">
-        <v>0.213</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45920</v>
+        <v>45922</v>
       </c>
       <c r="B60">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C60">
-        <v>0.075</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45920</v>
+        <v>45922</v>
       </c>
       <c r="B61">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C61">
-        <v>0.027</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45920</v>
+        <v>45922</v>
       </c>
       <c r="B62">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C62">
-        <v>0.027</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45920</v>
+        <v>45922</v>
       </c>
       <c r="B63">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C63">
-        <v>0.027</v>
+        <v>0.392</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C64">
-        <v>0.025</v>
+        <v>0.886</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C65">
-        <v>0.025</v>
+        <v>1.929</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>2.966</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B67">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>3.67</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B68">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>3.903</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B69">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>3.606</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>3.24</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C71">
-        <v>0.392</v>
+        <v>3.217</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B72">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C72">
-        <v>0.819</v>
+        <v>1.927</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B73">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C73">
-        <v>2.046</v>
+        <v>1.122</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B74">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C74">
-        <v>2.837</v>
+        <v>0.402</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B75">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C75">
-        <v>3.513</v>
+        <v>0.213</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B76">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C76">
-        <v>3.742</v>
+        <v>0.075</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B77">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C77">
-        <v>3.529</v>
+        <v>0.027</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B78">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C78">
-        <v>3.337</v>
+        <v>0.011</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45921</v>
+        <v>45922</v>
       </c>
       <c r="B79">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C79">
-        <v>3.057</v>
+        <v>0.011</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45921</v>
+        <v>45923</v>
       </c>
       <c r="B80">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C80">
-        <v>2.237</v>
+        <v>0</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45921</v>
+        <v>45923</v>
       </c>
       <c r="B81">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C81">
-        <v>1.197</v>
+        <v>0</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45921</v>
+        <v>45923</v>
       </c>
       <c r="B82">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C82">
-        <v>0.436</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45921</v>
+        <v>45923</v>
       </c>
       <c r="B83">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C83">
-        <v>0.213</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45921</v>
+        <v>45923</v>
       </c>
       <c r="B84">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C84">
-        <v>0.075</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45921</v>
+        <v>45923</v>
       </c>
       <c r="B85">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C85">
-        <v>0.027</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45921</v>
+        <v>45923</v>
       </c>
       <c r="B86">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C86">
-        <v>0.027</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45921</v>
+        <v>45923</v>
       </c>
       <c r="B87">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C87">
-        <v>0.018</v>
+        <v>0.387</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C88">
-        <v>0.016</v>
+        <v>0.838</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>1.908</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>2.722</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B91">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>3.661</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B92">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>3.986</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B93">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>3.716</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B94">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>3.388</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B95">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C95">
-        <v>0.392</v>
+        <v>3.09</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B96">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C96">
-        <v>0.826</v>
+        <v>1.927</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B97">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C97">
-        <v>1.869</v>
+        <v>0.963</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B98">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C98">
-        <v>2.523</v>
+        <v>0.297</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B99">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C99">
-        <v>3.668</v>
+        <v>0.213</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B100">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C100">
-        <v>3.749</v>
+        <v>0.075</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B101">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C101">
-        <v>3.481</v>
+        <v>0.027</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B102">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C102">
-        <v>3.384</v>
+        <v>0.027</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45922</v>
+        <v>45923</v>
       </c>
       <c r="B103">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C103">
-        <v>2.994</v>
+        <v>0.011</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45922</v>
+        <v>45924</v>
       </c>
       <c r="B104">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C104">
-        <v>1.946</v>
+        <v>0</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45922</v>
+        <v>45924</v>
       </c>
       <c r="B105">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C105">
-        <v>1.122</v>
+        <v>0</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45922</v>
+        <v>45924</v>
       </c>
       <c r="B106">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C106">
-        <v>0.366</v>
+        <v>0</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45922</v>
+        <v>45924</v>
       </c>
       <c r="B107">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C107">
-        <v>0.213</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45922</v>
+        <v>45924</v>
       </c>
       <c r="B108">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C108">
-        <v>0.075</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45922</v>
+        <v>45924</v>
       </c>
       <c r="B109">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C109">
-        <v>0.022</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45922</v>
+        <v>45924</v>
       </c>
       <c r="B110">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C110">
-        <v>0.027</v>
+        <v>0</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45922</v>
+        <v>45924</v>
       </c>
       <c r="B111">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C111">
-        <v>0.02</v>
+        <v>0.347</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>0.854</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>1.821</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>2.651</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B115">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>3.171</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B116">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>3.612</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B117">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>3.231</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B118">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>3.197</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B119">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C119">
-        <v>0.347</v>
+        <v>2.968</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B120">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C120">
-        <v>0.8179999999999999</v>
+        <v>1.815</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B121">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C121">
-        <v>1.66</v>
+        <v>0.952</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B122">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C122">
-        <v>2.343</v>
+        <v>0.284</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B123">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C123">
-        <v>3.088</v>
+        <v>0.075</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B124">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C124">
-        <v>3.53</v>
+        <v>0.075</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B125">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C125">
-        <v>3.322</v>
+        <v>0.022</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B126">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C126">
-        <v>3.258</v>
+        <v>0.022</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45923</v>
+        <v>45924</v>
       </c>
       <c r="B127">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C127">
-        <v>2.881</v>
+        <v>0.027</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45923</v>
+        <v>45925</v>
       </c>
       <c r="B128">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C128">
-        <v>2.009</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45923</v>
+        <v>45925</v>
       </c>
       <c r="B129">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C129">
-        <v>1.021</v>
+        <v>0.038</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45923</v>
+        <v>45925</v>
       </c>
       <c r="B130">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C130">
-        <v>0.338</v>
+        <v>0.022</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45923</v>
+        <v>45925</v>
       </c>
       <c r="B131">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C131">
-        <v>0.205</v>
+        <v>0.022</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45923</v>
+        <v>45925</v>
       </c>
       <c r="B132">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C132">
-        <v>0.075</v>
+        <v>0.013</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45923</v>
+        <v>45925</v>
       </c>
       <c r="B133">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C133">
-        <v>0.022</v>
+        <v>0.013</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45923</v>
+        <v>45925</v>
       </c>
       <c r="B134">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C134">
-        <v>0.022</v>
+        <v>0.013</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45923</v>
+        <v>45925</v>
       </c>
       <c r="B135">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C135">
-        <v>0.027</v>
+        <v>0.431</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C136">
-        <v>0.025</v>
+        <v>0.437</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B137">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C137">
-        <v>0.016</v>
+        <v>1.017</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B138">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>1.687</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B139">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>2.182</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B140">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>2.451</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B141">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>2.486</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B142">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>2.227</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B143">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C143">
-        <v>0.354</v>
+        <v>1.977</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B144">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C144">
-        <v>0.956</v>
+        <v>1.59</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B145">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C145">
-        <v>2.002</v>
+        <v>0.969</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B146">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C146">
-        <v>2.762</v>
+        <v>0.238</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B147">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C147">
-        <v>3.591</v>
+        <v>0.065</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B148">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C148">
-        <v>3.551</v>
+        <v>0.065</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B149">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C149">
-        <v>3.414</v>
+        <v>0.013</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B150">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C150">
-        <v>3.345</v>
+        <v>0.013</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45924</v>
+        <v>45925</v>
       </c>
       <c r="B151">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C151">
-        <v>2.968</v>
+        <v>0.013</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45924</v>
+        <v>45926</v>
       </c>
       <c r="B152">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C152">
-        <v>1.815</v>
+        <v>0.01</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45924</v>
+        <v>45926</v>
       </c>
       <c r="B153">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C153">
-        <v>1.005</v>
+        <v>0.01</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45924</v>
+        <v>45926</v>
       </c>
       <c r="B154">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C154">
-        <v>0.289</v>
+        <v>0.01</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45924</v>
+        <v>45926</v>
       </c>
       <c r="B155">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C155">
-        <v>0.066</v>
+        <v>0.01</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45924</v>
+        <v>45926</v>
       </c>
       <c r="B156">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C156">
-        <v>0.066</v>
+        <v>0.01</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45924</v>
+        <v>45926</v>
       </c>
       <c r="B157">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C157">
-        <v>0.013</v>
+        <v>0.019</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45924</v>
+        <v>45926</v>
       </c>
       <c r="B158">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C158">
-        <v>0.022</v>
+        <v>0.019</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45924</v>
+        <v>45926</v>
       </c>
       <c r="B159">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C159">
-        <v>0.022</v>
+        <v>0.439</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C160">
-        <v>0.019</v>
+        <v>0.51</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B161">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C161">
-        <v>0.019</v>
+        <v>1.334</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B162">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C162">
-        <v>0.019</v>
+        <v>1.665</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B163">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C163">
-        <v>0.08599999999999999</v>
+        <v>2.36</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B164">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C164">
-        <v>0.029</v>
+        <v>2.521</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B165">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C165">
-        <v>0.013</v>
+        <v>2.681</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B166">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C166">
-        <v>0.013</v>
+        <v>2.794</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B167">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C167">
-        <v>0.525</v>
+        <v>2.101</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B168">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C168">
-        <v>0.594</v>
+        <v>1.729</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B169">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C169">
-        <v>0.951</v>
+        <v>0.741</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45925</v>
+        <v>45926</v>
       </c>
       <c r="B170">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C170">
-        <v>1.731</v>
+        <v>0.238</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding GESS to the forecast portfolio
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>19.09.202519</t>
-  </si>
-  <si>
-    <t>19.09.202520</t>
-  </si>
-  <si>
-    <t>19.09.202521</t>
-  </si>
-  <si>
-    <t>19.09.202522</t>
-  </si>
-  <si>
-    <t>19.09.202523</t>
-  </si>
-  <si>
-    <t>19.09.202524</t>
-  </si>
-  <si>
-    <t>20.09.20251</t>
-  </si>
-  <si>
-    <t>20.09.20252</t>
-  </si>
-  <si>
-    <t>20.09.20253</t>
-  </si>
-  <si>
-    <t>20.09.20254</t>
-  </si>
-  <si>
-    <t>20.09.20255</t>
-  </si>
-  <si>
-    <t>20.09.20256</t>
-  </si>
-  <si>
-    <t>20.09.20257</t>
-  </si>
-  <si>
-    <t>20.09.20258</t>
-  </si>
-  <si>
-    <t>20.09.20259</t>
-  </si>
-  <si>
-    <t>20.09.202510</t>
-  </si>
-  <si>
-    <t>20.09.202511</t>
-  </si>
-  <si>
-    <t>20.09.202512</t>
-  </si>
-  <si>
-    <t>20.09.202513</t>
-  </si>
-  <si>
-    <t>20.09.202514</t>
-  </si>
-  <si>
-    <t>20.09.202515</t>
-  </si>
-  <si>
-    <t>20.09.202516</t>
-  </si>
-  <si>
-    <t>20.09.202517</t>
-  </si>
-  <si>
-    <t>20.09.202518</t>
-  </si>
-  <si>
-    <t>20.09.202519</t>
-  </si>
-  <si>
-    <t>20.09.202520</t>
-  </si>
-  <si>
-    <t>20.09.202521</t>
-  </si>
-  <si>
-    <t>20.09.202522</t>
-  </si>
-  <si>
-    <t>20.09.202523</t>
-  </si>
-  <si>
-    <t>20.09.202524</t>
-  </si>
-  <si>
-    <t>21.09.20251</t>
-  </si>
-  <si>
-    <t>21.09.20252</t>
-  </si>
-  <si>
-    <t>21.09.20253</t>
-  </si>
-  <si>
-    <t>21.09.20254</t>
-  </si>
-  <si>
-    <t>21.09.20255</t>
-  </si>
-  <si>
-    <t>21.09.20256</t>
-  </si>
-  <si>
-    <t>21.09.20257</t>
-  </si>
-  <si>
-    <t>21.09.20258</t>
-  </si>
-  <si>
-    <t>21.09.20259</t>
-  </si>
-  <si>
-    <t>21.09.202510</t>
-  </si>
-  <si>
-    <t>21.09.202511</t>
-  </si>
-  <si>
-    <t>21.09.202512</t>
-  </si>
-  <si>
-    <t>21.09.202513</t>
-  </si>
-  <si>
-    <t>21.09.202514</t>
-  </si>
-  <si>
-    <t>21.09.202515</t>
-  </si>
-  <si>
-    <t>21.09.202516</t>
-  </si>
-  <si>
-    <t>21.09.202517</t>
-  </si>
-  <si>
-    <t>21.09.202518</t>
-  </si>
-  <si>
-    <t>21.09.202519</t>
-  </si>
-  <si>
-    <t>21.09.202520</t>
-  </si>
-  <si>
-    <t>21.09.202521</t>
-  </si>
-  <si>
-    <t>21.09.202522</t>
-  </si>
-  <si>
-    <t>21.09.202523</t>
-  </si>
-  <si>
-    <t>21.09.202524</t>
-  </si>
-  <si>
-    <t>22.09.20251</t>
-  </si>
-  <si>
-    <t>22.09.20252</t>
-  </si>
-  <si>
-    <t>22.09.20253</t>
-  </si>
-  <si>
-    <t>22.09.20254</t>
-  </si>
-  <si>
-    <t>22.09.20255</t>
-  </si>
-  <si>
-    <t>22.09.20256</t>
-  </si>
-  <si>
-    <t>22.09.20257</t>
-  </si>
-  <si>
-    <t>22.09.20258</t>
-  </si>
-  <si>
-    <t>22.09.20259</t>
-  </si>
-  <si>
-    <t>22.09.202510</t>
-  </si>
-  <si>
-    <t>22.09.202511</t>
-  </si>
-  <si>
-    <t>22.09.202512</t>
-  </si>
-  <si>
-    <t>22.09.202513</t>
-  </si>
-  <si>
-    <t>22.09.202514</t>
-  </si>
-  <si>
-    <t>22.09.202515</t>
-  </si>
-  <si>
-    <t>22.09.202516</t>
-  </si>
-  <si>
-    <t>22.09.202517</t>
-  </si>
-  <si>
-    <t>22.09.202518</t>
-  </si>
-  <si>
-    <t>22.09.202519</t>
-  </si>
-  <si>
-    <t>22.09.202520</t>
-  </si>
-  <si>
-    <t>22.09.202521</t>
-  </si>
-  <si>
-    <t>22.09.202522</t>
-  </si>
-  <si>
-    <t>22.09.202523</t>
-  </si>
-  <si>
-    <t>22.09.202524</t>
-  </si>
-  <si>
-    <t>23.09.20251</t>
-  </si>
-  <si>
-    <t>23.09.20252</t>
-  </si>
-  <si>
-    <t>23.09.20253</t>
-  </si>
-  <si>
-    <t>23.09.20254</t>
-  </si>
-  <si>
-    <t>23.09.20255</t>
-  </si>
-  <si>
-    <t>23.09.20256</t>
-  </si>
-  <si>
-    <t>23.09.20257</t>
-  </si>
-  <si>
-    <t>23.09.20258</t>
-  </si>
-  <si>
-    <t>23.09.20259</t>
-  </si>
-  <si>
-    <t>23.09.202510</t>
-  </si>
-  <si>
-    <t>23.09.202511</t>
-  </si>
-  <si>
-    <t>23.09.202512</t>
-  </si>
-  <si>
-    <t>23.09.202513</t>
-  </si>
-  <si>
-    <t>23.09.202514</t>
-  </si>
-  <si>
-    <t>23.09.202515</t>
-  </si>
-  <si>
-    <t>23.09.202516</t>
-  </si>
-  <si>
-    <t>23.09.202517</t>
-  </si>
-  <si>
-    <t>23.09.202518</t>
-  </si>
-  <si>
-    <t>23.09.202519</t>
-  </si>
-  <si>
-    <t>23.09.202520</t>
-  </si>
-  <si>
-    <t>23.09.202521</t>
-  </si>
-  <si>
-    <t>23.09.202522</t>
-  </si>
-  <si>
-    <t>23.09.202523</t>
-  </si>
-  <si>
-    <t>23.09.202524</t>
-  </si>
-  <si>
-    <t>24.09.20251</t>
-  </si>
-  <si>
-    <t>24.09.20252</t>
-  </si>
-  <si>
-    <t>24.09.20253</t>
-  </si>
-  <si>
-    <t>24.09.20254</t>
-  </si>
-  <si>
-    <t>24.09.20255</t>
-  </si>
-  <si>
-    <t>24.09.20256</t>
-  </si>
-  <si>
-    <t>24.09.20257</t>
-  </si>
-  <si>
-    <t>24.09.20258</t>
-  </si>
-  <si>
-    <t>24.09.20259</t>
-  </si>
-  <si>
-    <t>24.09.202510</t>
-  </si>
-  <si>
-    <t>24.09.202511</t>
-  </si>
-  <si>
-    <t>24.09.202512</t>
-  </si>
-  <si>
-    <t>24.09.202513</t>
-  </si>
-  <si>
-    <t>24.09.202514</t>
-  </si>
-  <si>
-    <t>24.09.202515</t>
-  </si>
-  <si>
-    <t>24.09.202516</t>
-  </si>
-  <si>
-    <t>24.09.202517</t>
-  </si>
-  <si>
-    <t>24.09.202518</t>
-  </si>
-  <si>
-    <t>24.09.202519</t>
-  </si>
-  <si>
-    <t>24.09.202520</t>
-  </si>
-  <si>
-    <t>24.09.202521</t>
-  </si>
-  <si>
-    <t>24.09.202522</t>
-  </si>
-  <si>
-    <t>24.09.202523</t>
-  </si>
-  <si>
-    <t>24.09.202524</t>
-  </si>
-  <si>
-    <t>25.09.20251</t>
-  </si>
-  <si>
-    <t>25.09.20252</t>
-  </si>
-  <si>
-    <t>25.09.20253</t>
-  </si>
-  <si>
-    <t>25.09.20254</t>
-  </si>
-  <si>
-    <t>25.09.20255</t>
-  </si>
-  <si>
-    <t>25.09.20256</t>
-  </si>
-  <si>
-    <t>25.09.20257</t>
-  </si>
-  <si>
-    <t>25.09.20258</t>
-  </si>
-  <si>
-    <t>25.09.20259</t>
-  </si>
-  <si>
-    <t>25.09.202510</t>
-  </si>
-  <si>
-    <t>25.09.202511</t>
-  </si>
-  <si>
-    <t>25.09.202512</t>
-  </si>
-  <si>
-    <t>25.09.202513</t>
-  </si>
-  <si>
-    <t>25.09.202514</t>
-  </si>
-  <si>
-    <t>25.09.202515</t>
-  </si>
-  <si>
-    <t>25.09.202516</t>
-  </si>
-  <si>
-    <t>25.09.202517</t>
-  </si>
-  <si>
-    <t>25.09.202518</t>
-  </si>
-  <si>
-    <t>25.09.202519</t>
-  </si>
-  <si>
-    <t>25.09.202520</t>
-  </si>
-  <si>
-    <t>25.09.202521</t>
-  </si>
-  <si>
-    <t>25.09.202522</t>
-  </si>
-  <si>
-    <t>25.09.202523</t>
-  </si>
-  <si>
-    <t>25.09.202524</t>
-  </si>
-  <si>
-    <t>26.09.20251</t>
-  </si>
-  <si>
-    <t>26.09.20252</t>
-  </si>
-  <si>
-    <t>26.09.20253</t>
-  </si>
-  <si>
-    <t>26.09.20254</t>
-  </si>
-  <si>
-    <t>26.09.20255</t>
-  </si>
-  <si>
-    <t>26.09.20256</t>
-  </si>
-  <si>
-    <t>26.09.20257</t>
-  </si>
-  <si>
-    <t>26.09.20258</t>
-  </si>
-  <si>
-    <t>26.09.20259</t>
-  </si>
-  <si>
-    <t>26.09.202510</t>
-  </si>
-  <si>
-    <t>26.09.202511</t>
-  </si>
-  <si>
-    <t>26.09.202512</t>
-  </si>
-  <si>
-    <t>26.09.202513</t>
-  </si>
-  <si>
-    <t>26.09.202514</t>
-  </si>
-  <si>
-    <t>26.09.202515</t>
-  </si>
-  <si>
-    <t>26.09.202516</t>
-  </si>
-  <si>
-    <t>26.09.202517</t>
-  </si>
-  <si>
-    <t>26.09.202518</t>
-  </si>
-  <si>
-    <t>26.09.202519</t>
+    <t>03.10.202511</t>
+  </si>
+  <si>
+    <t>03.10.202512</t>
+  </si>
+  <si>
+    <t>03.10.202513</t>
+  </si>
+  <si>
+    <t>03.10.202514</t>
+  </si>
+  <si>
+    <t>03.10.202515</t>
+  </si>
+  <si>
+    <t>03.10.202516</t>
+  </si>
+  <si>
+    <t>03.10.202517</t>
+  </si>
+  <si>
+    <t>03.10.202518</t>
+  </si>
+  <si>
+    <t>03.10.202519</t>
+  </si>
+  <si>
+    <t>03.10.202520</t>
+  </si>
+  <si>
+    <t>03.10.202521</t>
+  </si>
+  <si>
+    <t>03.10.202522</t>
+  </si>
+  <si>
+    <t>03.10.202523</t>
+  </si>
+  <si>
+    <t>03.10.202524</t>
+  </si>
+  <si>
+    <t>04.10.20251</t>
+  </si>
+  <si>
+    <t>04.10.20252</t>
+  </si>
+  <si>
+    <t>04.10.20253</t>
+  </si>
+  <si>
+    <t>04.10.20254</t>
+  </si>
+  <si>
+    <t>04.10.20255</t>
+  </si>
+  <si>
+    <t>04.10.20256</t>
+  </si>
+  <si>
+    <t>04.10.20257</t>
+  </si>
+  <si>
+    <t>04.10.20258</t>
+  </si>
+  <si>
+    <t>04.10.20259</t>
+  </si>
+  <si>
+    <t>04.10.202510</t>
+  </si>
+  <si>
+    <t>04.10.202511</t>
+  </si>
+  <si>
+    <t>04.10.202512</t>
+  </si>
+  <si>
+    <t>04.10.202513</t>
+  </si>
+  <si>
+    <t>04.10.202514</t>
+  </si>
+  <si>
+    <t>04.10.202515</t>
+  </si>
+  <si>
+    <t>04.10.202516</t>
+  </si>
+  <si>
+    <t>04.10.202517</t>
+  </si>
+  <si>
+    <t>04.10.202518</t>
+  </si>
+  <si>
+    <t>04.10.202519</t>
+  </si>
+  <si>
+    <t>04.10.202520</t>
+  </si>
+  <si>
+    <t>04.10.202521</t>
+  </si>
+  <si>
+    <t>04.10.202522</t>
+  </si>
+  <si>
+    <t>04.10.202523</t>
+  </si>
+  <si>
+    <t>04.10.202524</t>
+  </si>
+  <si>
+    <t>05.10.20251</t>
+  </si>
+  <si>
+    <t>05.10.20252</t>
+  </si>
+  <si>
+    <t>05.10.20253</t>
+  </si>
+  <si>
+    <t>05.10.20254</t>
+  </si>
+  <si>
+    <t>05.10.20255</t>
+  </si>
+  <si>
+    <t>05.10.20256</t>
+  </si>
+  <si>
+    <t>05.10.20257</t>
+  </si>
+  <si>
+    <t>05.10.20258</t>
+  </si>
+  <si>
+    <t>05.10.20259</t>
+  </si>
+  <si>
+    <t>05.10.202510</t>
+  </si>
+  <si>
+    <t>05.10.202511</t>
+  </si>
+  <si>
+    <t>05.10.202512</t>
+  </si>
+  <si>
+    <t>05.10.202513</t>
+  </si>
+  <si>
+    <t>05.10.202514</t>
+  </si>
+  <si>
+    <t>05.10.202515</t>
+  </si>
+  <si>
+    <t>05.10.202516</t>
+  </si>
+  <si>
+    <t>05.10.202517</t>
+  </si>
+  <si>
+    <t>05.10.202518</t>
+  </si>
+  <si>
+    <t>05.10.202519</t>
+  </si>
+  <si>
+    <t>05.10.202520</t>
+  </si>
+  <si>
+    <t>05.10.202521</t>
+  </si>
+  <si>
+    <t>05.10.202522</t>
+  </si>
+  <si>
+    <t>05.10.202523</t>
+  </si>
+  <si>
+    <t>05.10.202524</t>
+  </si>
+  <si>
+    <t>06.10.20251</t>
+  </si>
+  <si>
+    <t>06.10.20252</t>
+  </si>
+  <si>
+    <t>06.10.20253</t>
+  </si>
+  <si>
+    <t>06.10.20254</t>
+  </si>
+  <si>
+    <t>06.10.20255</t>
+  </si>
+  <si>
+    <t>06.10.20256</t>
+  </si>
+  <si>
+    <t>06.10.20257</t>
+  </si>
+  <si>
+    <t>06.10.20258</t>
+  </si>
+  <si>
+    <t>06.10.20259</t>
+  </si>
+  <si>
+    <t>06.10.202510</t>
+  </si>
+  <si>
+    <t>06.10.202511</t>
+  </si>
+  <si>
+    <t>06.10.202512</t>
+  </si>
+  <si>
+    <t>06.10.202513</t>
+  </si>
+  <si>
+    <t>06.10.202514</t>
+  </si>
+  <si>
+    <t>06.10.202515</t>
+  </si>
+  <si>
+    <t>06.10.202516</t>
+  </si>
+  <si>
+    <t>06.10.202517</t>
+  </si>
+  <si>
+    <t>06.10.202518</t>
+  </si>
+  <si>
+    <t>06.10.202519</t>
+  </si>
+  <si>
+    <t>06.10.202520</t>
+  </si>
+  <si>
+    <t>06.10.202521</t>
+  </si>
+  <si>
+    <t>06.10.202522</t>
+  </si>
+  <si>
+    <t>06.10.202523</t>
+  </si>
+  <si>
+    <t>06.10.202524</t>
+  </si>
+  <si>
+    <t>07.10.20251</t>
+  </si>
+  <si>
+    <t>07.10.20252</t>
+  </si>
+  <si>
+    <t>07.10.20253</t>
+  </si>
+  <si>
+    <t>07.10.20254</t>
+  </si>
+  <si>
+    <t>07.10.20255</t>
+  </si>
+  <si>
+    <t>07.10.20256</t>
+  </si>
+  <si>
+    <t>07.10.20257</t>
+  </si>
+  <si>
+    <t>07.10.20258</t>
+  </si>
+  <si>
+    <t>07.10.20259</t>
+  </si>
+  <si>
+    <t>07.10.202510</t>
+  </si>
+  <si>
+    <t>07.10.202511</t>
+  </si>
+  <si>
+    <t>07.10.202512</t>
+  </si>
+  <si>
+    <t>07.10.202513</t>
+  </si>
+  <si>
+    <t>07.10.202514</t>
+  </si>
+  <si>
+    <t>07.10.202515</t>
+  </si>
+  <si>
+    <t>07.10.202516</t>
+  </si>
+  <si>
+    <t>07.10.202517</t>
+  </si>
+  <si>
+    <t>07.10.202518</t>
+  </si>
+  <si>
+    <t>07.10.202519</t>
+  </si>
+  <si>
+    <t>07.10.202520</t>
+  </si>
+  <si>
+    <t>07.10.202521</t>
+  </si>
+  <si>
+    <t>07.10.202522</t>
+  </si>
+  <si>
+    <t>07.10.202523</t>
+  </si>
+  <si>
+    <t>07.10.202524</t>
+  </si>
+  <si>
+    <t>08.10.20251</t>
+  </si>
+  <si>
+    <t>08.10.20252</t>
+  </si>
+  <si>
+    <t>08.10.20253</t>
+  </si>
+  <si>
+    <t>08.10.20254</t>
+  </si>
+  <si>
+    <t>08.10.20255</t>
+  </si>
+  <si>
+    <t>08.10.20256</t>
+  </si>
+  <si>
+    <t>08.10.20257</t>
+  </si>
+  <si>
+    <t>08.10.20258</t>
+  </si>
+  <si>
+    <t>08.10.20259</t>
+  </si>
+  <si>
+    <t>08.10.202510</t>
+  </si>
+  <si>
+    <t>08.10.202511</t>
+  </si>
+  <si>
+    <t>08.10.202512</t>
+  </si>
+  <si>
+    <t>08.10.202513</t>
+  </si>
+  <si>
+    <t>08.10.202514</t>
+  </si>
+  <si>
+    <t>08.10.202515</t>
+  </si>
+  <si>
+    <t>08.10.202516</t>
+  </si>
+  <si>
+    <t>08.10.202517</t>
+  </si>
+  <si>
+    <t>08.10.202518</t>
+  </si>
+  <si>
+    <t>08.10.202519</t>
+  </si>
+  <si>
+    <t>08.10.202520</t>
+  </si>
+  <si>
+    <t>08.10.202521</t>
+  </si>
+  <si>
+    <t>08.10.202522</t>
+  </si>
+  <si>
+    <t>08.10.202523</t>
+  </si>
+  <si>
+    <t>08.10.202524</t>
+  </si>
+  <si>
+    <t>09.10.20251</t>
+  </si>
+  <si>
+    <t>09.10.20252</t>
+  </si>
+  <si>
+    <t>09.10.20253</t>
+  </si>
+  <si>
+    <t>09.10.20254</t>
+  </si>
+  <si>
+    <t>09.10.20255</t>
+  </si>
+  <si>
+    <t>09.10.20256</t>
+  </si>
+  <si>
+    <t>09.10.20257</t>
+  </si>
+  <si>
+    <t>09.10.20258</t>
+  </si>
+  <si>
+    <t>09.10.20259</t>
+  </si>
+  <si>
+    <t>09.10.202510</t>
+  </si>
+  <si>
+    <t>09.10.202511</t>
+  </si>
+  <si>
+    <t>09.10.202512</t>
+  </si>
+  <si>
+    <t>09.10.202513</t>
+  </si>
+  <si>
+    <t>09.10.202514</t>
+  </si>
+  <si>
+    <t>09.10.202515</t>
+  </si>
+  <si>
+    <t>09.10.202516</t>
+  </si>
+  <si>
+    <t>09.10.202517</t>
+  </si>
+  <si>
+    <t>09.10.202518</t>
+  </si>
+  <si>
+    <t>09.10.202519</t>
+  </si>
+  <si>
+    <t>09.10.202520</t>
+  </si>
+  <si>
+    <t>09.10.202521</t>
+  </si>
+  <si>
+    <t>09.10.202522</t>
+  </si>
+  <si>
+    <t>09.10.202523</t>
+  </si>
+  <si>
+    <t>09.10.202524</t>
+  </si>
+  <si>
+    <t>10.10.20251</t>
+  </si>
+  <si>
+    <t>10.10.20252</t>
+  </si>
+  <si>
+    <t>10.10.20253</t>
+  </si>
+  <si>
+    <t>10.10.20254</t>
+  </si>
+  <si>
+    <t>10.10.20255</t>
+  </si>
+  <si>
+    <t>10.10.20256</t>
+  </si>
+  <si>
+    <t>10.10.20257</t>
+  </si>
+  <si>
+    <t>10.10.20258</t>
+  </si>
+  <si>
+    <t>10.10.20259</t>
+  </si>
+  <si>
+    <t>10.10.202510</t>
+  </si>
+  <si>
+    <t>10.10.202511</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45919</v>
+        <v>45933</v>
       </c>
       <c r="B2">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>0.034</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45919</v>
+        <v>45933</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>0.039</v>
+        <v>0.034</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45919</v>
+        <v>45933</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>0.08799999999999999</v>
+        <v>0.513</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45919</v>
+        <v>45933</v>
       </c>
       <c r="B5">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>0.08799999999999999</v>
+        <v>0.408</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45919</v>
+        <v>45933</v>
       </c>
       <c r="B6">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>0.019</v>
+        <v>0.408</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45919</v>
+        <v>45933</v>
       </c>
       <c r="B7">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>0.02</v>
+        <v>0.376</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45920</v>
+        <v>45933</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>0.018</v>
+        <v>0.292</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45920</v>
+        <v>45933</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.246</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45920</v>
+        <v>45933</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.108</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45920</v>
+        <v>45933</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.222</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45920</v>
+        <v>45933</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.209</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45920</v>
+        <v>45933</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.119</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45920</v>
+        <v>45933</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.109</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45920</v>
+        <v>45933</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>0.392</v>
+        <v>0.011</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>1.117</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>1.814</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>2.597</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>3.545</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B20">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>3.468</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B21">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C21">
-        <v>3.254</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B22">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>3.174</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B23">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>2.622</v>
+        <v>0.083</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B24">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C24">
-        <v>2.056</v>
+        <v>0.265</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B25">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C25">
-        <v>1.112</v>
+        <v>0.368</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B26">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C26">
-        <v>0.515</v>
+        <v>0.546</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B27">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C27">
-        <v>0.275</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B28">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C28">
-        <v>0.136</v>
+        <v>0.57</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B29">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C29">
-        <v>0.083</v>
+        <v>0.916</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B30">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C30">
-        <v>0.083</v>
+        <v>0.971</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45920</v>
+        <v>45934</v>
       </c>
       <c r="B31">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C31">
-        <v>0.089</v>
+        <v>1.014</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45921</v>
+        <v>45934</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C32">
-        <v>0.025</v>
+        <v>0.636</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45921</v>
+        <v>45934</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C33">
-        <v>0.016</v>
+        <v>0.297</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45921</v>
+        <v>45934</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>0.165</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45921</v>
+        <v>45934</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45921</v>
+        <v>45934</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45921</v>
+        <v>45934</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45921</v>
+        <v>45934</v>
       </c>
       <c r="B38">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45921</v>
+        <v>45934</v>
       </c>
       <c r="B39">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C39">
-        <v>0.392</v>
+        <v>0.016</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>0.851</v>
+        <v>0.013</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B41">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C41">
-        <v>1.818</v>
+        <v>0.013</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B42">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C42">
-        <v>2.683</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B43">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C43">
-        <v>3.668</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B44">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C44">
-        <v>3.568</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B45">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C45">
-        <v>3.248</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B46">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C46">
-        <v>3.063</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B47">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C47">
-        <v>2.509</v>
+        <v>0.26</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B48">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C48">
-        <v>1.874</v>
+        <v>0.872</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B49">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C49">
-        <v>1.018</v>
+        <v>1.931</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B50">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C50">
-        <v>0.42</v>
+        <v>2.538</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B51">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C51">
-        <v>0.213</v>
+        <v>3.142</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B52">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C52">
-        <v>0.075</v>
+        <v>3.487</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B53">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C53">
-        <v>0.027</v>
+        <v>3.418</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B54">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C54">
-        <v>0.027</v>
+        <v>3.159</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45921</v>
+        <v>45935</v>
       </c>
       <c r="B55">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C55">
-        <v>0.011</v>
+        <v>2.222</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45922</v>
+        <v>45935</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1.686</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45922</v>
+        <v>45935</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>0.881</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45922</v>
+        <v>45935</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>0.236</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45922</v>
+        <v>45935</v>
       </c>
       <c r="B59">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45922</v>
+        <v>45935</v>
       </c>
       <c r="B60">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45922</v>
+        <v>45935</v>
       </c>
       <c r="B61">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45922</v>
+        <v>45935</v>
       </c>
       <c r="B62">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45922</v>
+        <v>45935</v>
       </c>
       <c r="B63">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C63">
-        <v>0.392</v>
+        <v>0.016</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B64">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C64">
-        <v>0.886</v>
+        <v>0.013</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B65">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C65">
-        <v>1.929</v>
+        <v>0.013</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B66">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C66">
-        <v>2.966</v>
+        <v>0.013</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B67">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C67">
-        <v>3.67</v>
+        <v>0.013</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B68">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C68">
-        <v>3.903</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B69">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C69">
-        <v>3.606</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B70">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C70">
-        <v>3.24</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B71">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C71">
-        <v>3.217</v>
+        <v>0.111</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B72">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C72">
-        <v>1.927</v>
+        <v>0.316</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B73">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C73">
-        <v>1.122</v>
+        <v>0.67</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B74">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C74">
-        <v>0.402</v>
+        <v>1.023</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B75">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C75">
-        <v>0.213</v>
+        <v>0.976</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B76">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C76">
-        <v>0.075</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B77">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C77">
-        <v>0.027</v>
+        <v>0.91</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B78">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C78">
-        <v>0.011</v>
+        <v>0.96</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="B79">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C79">
-        <v>0.011</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45923</v>
+        <v>45936</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>0.398</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45923</v>
+        <v>45936</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>0.286</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45923</v>
+        <v>45936</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>0.115</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45923</v>
+        <v>45936</v>
       </c>
       <c r="B83">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>0.068</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45923</v>
+        <v>45936</v>
       </c>
       <c r="B84">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>0.068</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45923</v>
+        <v>45936</v>
       </c>
       <c r="B85">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45923</v>
+        <v>45936</v>
       </c>
       <c r="B86">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45923</v>
+        <v>45936</v>
       </c>
       <c r="B87">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C87">
-        <v>0.387</v>
+        <v>0.011</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B88">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C88">
-        <v>0.838</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B89">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C89">
-        <v>1.908</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B90">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C90">
-        <v>2.722</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B91">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C91">
-        <v>3.661</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B92">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C92">
-        <v>3.986</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B93">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C93">
-        <v>3.716</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B94">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C94">
-        <v>3.388</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B95">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C95">
-        <v>3.09</v>
+        <v>0.392</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B96">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C96">
-        <v>1.927</v>
+        <v>0.637</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B97">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C97">
-        <v>0.963</v>
+        <v>1.161</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B98">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C98">
-        <v>0.297</v>
+        <v>1.855</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B99">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C99">
-        <v>0.213</v>
+        <v>2.459</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B100">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C100">
-        <v>0.075</v>
+        <v>2.509</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B101">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C101">
-        <v>0.027</v>
+        <v>2.364</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B102">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C102">
-        <v>0.027</v>
+        <v>1.655</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="B103">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C103">
-        <v>0.011</v>
+        <v>1.354</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45924</v>
+        <v>45937</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>1.009</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45924</v>
+        <v>45937</v>
       </c>
       <c r="B105">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>0.473</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45924</v>
+        <v>45937</v>
       </c>
       <c r="B106">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>0.426</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45924</v>
+        <v>45937</v>
       </c>
       <c r="B107">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45924</v>
+        <v>45937</v>
       </c>
       <c r="B108">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45924</v>
+        <v>45937</v>
       </c>
       <c r="B109">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45924</v>
+        <v>45937</v>
       </c>
       <c r="B110">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45924</v>
+        <v>45937</v>
       </c>
       <c r="B111">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C111">
-        <v>0.347</v>
+        <v>0.016</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B112">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C112">
-        <v>0.854</v>
+        <v>0</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B113">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C113">
-        <v>1.821</v>
+        <v>0.013</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B114">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C114">
-        <v>2.651</v>
+        <v>0.013</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B115">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C115">
-        <v>3.171</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B116">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C116">
-        <v>3.612</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B117">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C117">
-        <v>3.231</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B118">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C118">
-        <v>3.197</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B119">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C119">
-        <v>2.968</v>
+        <v>0.275</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B120">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C120">
-        <v>1.815</v>
+        <v>0.542</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B121">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C121">
-        <v>0.952</v>
+        <v>1.134</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B122">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C122">
-        <v>0.284</v>
+        <v>2.007</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B123">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C123">
-        <v>0.075</v>
+        <v>2.464</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B124">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C124">
-        <v>0.075</v>
+        <v>2.514</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B125">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C125">
-        <v>0.022</v>
+        <v>2.463</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B126">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C126">
-        <v>0.022</v>
+        <v>1.794</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="B127">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C127">
-        <v>0.027</v>
+        <v>1.959</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45925</v>
+        <v>45938</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C128">
-        <v>0.08599999999999999</v>
+        <v>0.974</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45925</v>
+        <v>45938</v>
       </c>
       <c r="B129">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C129">
-        <v>0.038</v>
+        <v>0.386</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45925</v>
+        <v>45938</v>
       </c>
       <c r="B130">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C130">
-        <v>0.022</v>
+        <v>0.276</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45925</v>
+        <v>45938</v>
       </c>
       <c r="B131">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C131">
-        <v>0.022</v>
+        <v>0.048</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45925</v>
+        <v>45938</v>
       </c>
       <c r="B132">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C132">
-        <v>0.013</v>
+        <v>0.048</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45925</v>
+        <v>45938</v>
       </c>
       <c r="B133">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C133">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45925</v>
+        <v>45938</v>
       </c>
       <c r="B134">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C134">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45925</v>
+        <v>45938</v>
       </c>
       <c r="B135">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C135">
-        <v>0.431</v>
+        <v>0.016</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B136">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C136">
-        <v>0.437</v>
+        <v>0.013</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B137">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C137">
-        <v>1.017</v>
+        <v>0.013</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B138">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C138">
-        <v>1.687</v>
+        <v>0.013</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B139">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C139">
-        <v>2.182</v>
+        <v>0.013</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B140">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C140">
-        <v>2.451</v>
+        <v>0.013</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B141">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C141">
-        <v>2.486</v>
+        <v>0.013</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B142">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C142">
-        <v>2.227</v>
+        <v>0.013</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B143">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C143">
-        <v>1.977</v>
+        <v>0.182</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B144">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C144">
-        <v>1.59</v>
+        <v>0.45</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B145">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C145">
-        <v>0.969</v>
+        <v>1.144</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B146">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C146">
-        <v>0.238</v>
+        <v>1.945</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B147">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C147">
-        <v>0.065</v>
+        <v>2.31</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B148">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C148">
-        <v>0.065</v>
+        <v>2.793</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B149">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C149">
-        <v>0.013</v>
+        <v>2.7</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B150">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C150">
-        <v>0.013</v>
+        <v>2.405</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="B151">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C151">
-        <v>0.013</v>
+        <v>1.81</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45926</v>
+        <v>45939</v>
       </c>
       <c r="B152">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C152">
-        <v>0.01</v>
+        <v>1.181</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45926</v>
+        <v>45939</v>
       </c>
       <c r="B153">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C153">
-        <v>0.01</v>
+        <v>0.637</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45926</v>
+        <v>45939</v>
       </c>
       <c r="B154">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C154">
-        <v>0.01</v>
+        <v>0.411</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45926</v>
+        <v>45939</v>
       </c>
       <c r="B155">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C155">
-        <v>0.01</v>
+        <v>0.064</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45926</v>
+        <v>45939</v>
       </c>
       <c r="B156">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C156">
-        <v>0.01</v>
+        <v>0.064</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45926</v>
+        <v>45939</v>
       </c>
       <c r="B157">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C157">
-        <v>0.019</v>
+        <v>0.011</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45926</v>
+        <v>45939</v>
       </c>
       <c r="B158">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C158">
-        <v>0.019</v>
+        <v>0.011</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45926</v>
+        <v>45939</v>
       </c>
       <c r="B159">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C159">
-        <v>0.439</v>
+        <v>0.011</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B160">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C160">
-        <v>0.51</v>
+        <v>0</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B161">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C161">
-        <v>1.334</v>
+        <v>0</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B162">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C162">
-        <v>1.665</v>
+        <v>0</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B163">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C163">
-        <v>2.36</v>
+        <v>0.013</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B164">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C164">
-        <v>2.521</v>
+        <v>0.013</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B165">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C165">
-        <v>2.681</v>
+        <v>0.013</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B166">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C166">
-        <v>2.794</v>
+        <v>0.013</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B167">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C167">
-        <v>2.101</v>
+        <v>0.267</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B168">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C168">
-        <v>1.729</v>
+        <v>0.518</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B169">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C169">
-        <v>0.741</v>
+        <v>1.065</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="B170">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C170">
-        <v>0.238</v>
+        <v>1.566</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding NRG to the foreecast portfolio
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>03.10.202511</t>
-  </si>
-  <si>
-    <t>03.10.202512</t>
-  </si>
-  <si>
-    <t>03.10.202513</t>
-  </si>
-  <si>
-    <t>03.10.202514</t>
-  </si>
-  <si>
-    <t>03.10.202515</t>
-  </si>
-  <si>
-    <t>03.10.202516</t>
-  </si>
-  <si>
-    <t>03.10.202517</t>
-  </si>
-  <si>
-    <t>03.10.202518</t>
-  </si>
-  <si>
-    <t>03.10.202519</t>
-  </si>
-  <si>
-    <t>03.10.202520</t>
-  </si>
-  <si>
-    <t>03.10.202521</t>
-  </si>
-  <si>
-    <t>03.10.202522</t>
-  </si>
-  <si>
-    <t>03.10.202523</t>
-  </si>
-  <si>
-    <t>03.10.202524</t>
-  </si>
-  <si>
-    <t>04.10.20251</t>
-  </si>
-  <si>
-    <t>04.10.20252</t>
-  </si>
-  <si>
-    <t>04.10.20253</t>
-  </si>
-  <si>
-    <t>04.10.20254</t>
-  </si>
-  <si>
-    <t>04.10.20255</t>
-  </si>
-  <si>
-    <t>04.10.20256</t>
-  </si>
-  <si>
-    <t>04.10.20257</t>
-  </si>
-  <si>
-    <t>04.10.20258</t>
-  </si>
-  <si>
-    <t>04.10.20259</t>
-  </si>
-  <si>
-    <t>04.10.202510</t>
-  </si>
-  <si>
-    <t>04.10.202511</t>
-  </si>
-  <si>
-    <t>04.10.202512</t>
-  </si>
-  <si>
-    <t>04.10.202513</t>
-  </si>
-  <si>
-    <t>04.10.202514</t>
-  </si>
-  <si>
-    <t>04.10.202515</t>
-  </si>
-  <si>
-    <t>04.10.202516</t>
-  </si>
-  <si>
-    <t>04.10.202517</t>
-  </si>
-  <si>
-    <t>04.10.202518</t>
-  </si>
-  <si>
-    <t>04.10.202519</t>
-  </si>
-  <si>
-    <t>04.10.202520</t>
-  </si>
-  <si>
-    <t>04.10.202521</t>
-  </si>
-  <si>
-    <t>04.10.202522</t>
-  </si>
-  <si>
-    <t>04.10.202523</t>
-  </si>
-  <si>
-    <t>04.10.202524</t>
-  </si>
-  <si>
-    <t>05.10.20251</t>
-  </si>
-  <si>
-    <t>05.10.20252</t>
-  </si>
-  <si>
-    <t>05.10.20253</t>
-  </si>
-  <si>
-    <t>05.10.20254</t>
-  </si>
-  <si>
-    <t>05.10.20255</t>
-  </si>
-  <si>
-    <t>05.10.20256</t>
-  </si>
-  <si>
-    <t>05.10.20257</t>
-  </si>
-  <si>
-    <t>05.10.20258</t>
-  </si>
-  <si>
-    <t>05.10.20259</t>
-  </si>
-  <si>
-    <t>05.10.202510</t>
-  </si>
-  <si>
-    <t>05.10.202511</t>
-  </si>
-  <si>
-    <t>05.10.202512</t>
-  </si>
-  <si>
-    <t>05.10.202513</t>
-  </si>
-  <si>
-    <t>05.10.202514</t>
-  </si>
-  <si>
-    <t>05.10.202515</t>
-  </si>
-  <si>
-    <t>05.10.202516</t>
-  </si>
-  <si>
-    <t>05.10.202517</t>
-  </si>
-  <si>
-    <t>05.10.202518</t>
-  </si>
-  <si>
-    <t>05.10.202519</t>
-  </si>
-  <si>
-    <t>05.10.202520</t>
-  </si>
-  <si>
-    <t>05.10.202521</t>
-  </si>
-  <si>
-    <t>05.10.202522</t>
-  </si>
-  <si>
-    <t>05.10.202523</t>
-  </si>
-  <si>
-    <t>05.10.202524</t>
-  </si>
-  <si>
-    <t>06.10.20251</t>
-  </si>
-  <si>
-    <t>06.10.20252</t>
-  </si>
-  <si>
-    <t>06.10.20253</t>
-  </si>
-  <si>
-    <t>06.10.20254</t>
-  </si>
-  <si>
-    <t>06.10.20255</t>
-  </si>
-  <si>
-    <t>06.10.20256</t>
-  </si>
-  <si>
-    <t>06.10.20257</t>
-  </si>
-  <si>
-    <t>06.10.20258</t>
-  </si>
-  <si>
-    <t>06.10.20259</t>
-  </si>
-  <si>
-    <t>06.10.202510</t>
-  </si>
-  <si>
-    <t>06.10.202511</t>
-  </si>
-  <si>
-    <t>06.10.202512</t>
-  </si>
-  <si>
-    <t>06.10.202513</t>
-  </si>
-  <si>
-    <t>06.10.202514</t>
-  </si>
-  <si>
-    <t>06.10.202515</t>
-  </si>
-  <si>
-    <t>06.10.202516</t>
-  </si>
-  <si>
-    <t>06.10.202517</t>
-  </si>
-  <si>
-    <t>06.10.202518</t>
-  </si>
-  <si>
-    <t>06.10.202519</t>
-  </si>
-  <si>
-    <t>06.10.202520</t>
-  </si>
-  <si>
-    <t>06.10.202521</t>
-  </si>
-  <si>
-    <t>06.10.202522</t>
-  </si>
-  <si>
-    <t>06.10.202523</t>
-  </si>
-  <si>
-    <t>06.10.202524</t>
-  </si>
-  <si>
-    <t>07.10.20251</t>
-  </si>
-  <si>
-    <t>07.10.20252</t>
-  </si>
-  <si>
-    <t>07.10.20253</t>
-  </si>
-  <si>
-    <t>07.10.20254</t>
-  </si>
-  <si>
-    <t>07.10.20255</t>
-  </si>
-  <si>
-    <t>07.10.20256</t>
-  </si>
-  <si>
-    <t>07.10.20257</t>
-  </si>
-  <si>
-    <t>07.10.20258</t>
-  </si>
-  <si>
-    <t>07.10.20259</t>
-  </si>
-  <si>
-    <t>07.10.202510</t>
-  </si>
-  <si>
-    <t>07.10.202511</t>
-  </si>
-  <si>
-    <t>07.10.202512</t>
-  </si>
-  <si>
-    <t>07.10.202513</t>
-  </si>
-  <si>
-    <t>07.10.202514</t>
-  </si>
-  <si>
-    <t>07.10.202515</t>
-  </si>
-  <si>
-    <t>07.10.202516</t>
-  </si>
-  <si>
-    <t>07.10.202517</t>
-  </si>
-  <si>
-    <t>07.10.202518</t>
-  </si>
-  <si>
-    <t>07.10.202519</t>
-  </si>
-  <si>
-    <t>07.10.202520</t>
-  </si>
-  <si>
-    <t>07.10.202521</t>
-  </si>
-  <si>
-    <t>07.10.202522</t>
-  </si>
-  <si>
-    <t>07.10.202523</t>
-  </si>
-  <si>
-    <t>07.10.202524</t>
-  </si>
-  <si>
-    <t>08.10.20251</t>
-  </si>
-  <si>
-    <t>08.10.20252</t>
-  </si>
-  <si>
-    <t>08.10.20253</t>
-  </si>
-  <si>
-    <t>08.10.20254</t>
-  </si>
-  <si>
-    <t>08.10.20255</t>
-  </si>
-  <si>
-    <t>08.10.20256</t>
-  </si>
-  <si>
-    <t>08.10.20257</t>
-  </si>
-  <si>
-    <t>08.10.20258</t>
-  </si>
-  <si>
-    <t>08.10.20259</t>
-  </si>
-  <si>
-    <t>08.10.202510</t>
-  </si>
-  <si>
-    <t>08.10.202511</t>
-  </si>
-  <si>
-    <t>08.10.202512</t>
-  </si>
-  <si>
-    <t>08.10.202513</t>
-  </si>
-  <si>
-    <t>08.10.202514</t>
-  </si>
-  <si>
-    <t>08.10.202515</t>
-  </si>
-  <si>
-    <t>08.10.202516</t>
-  </si>
-  <si>
-    <t>08.10.202517</t>
-  </si>
-  <si>
-    <t>08.10.202518</t>
-  </si>
-  <si>
-    <t>08.10.202519</t>
-  </si>
-  <si>
-    <t>08.10.202520</t>
-  </si>
-  <si>
-    <t>08.10.202521</t>
-  </si>
-  <si>
-    <t>08.10.202522</t>
-  </si>
-  <si>
-    <t>08.10.202523</t>
-  </si>
-  <si>
-    <t>08.10.202524</t>
-  </si>
-  <si>
-    <t>09.10.20251</t>
-  </si>
-  <si>
-    <t>09.10.20252</t>
-  </si>
-  <si>
-    <t>09.10.20253</t>
-  </si>
-  <si>
-    <t>09.10.20254</t>
-  </si>
-  <si>
-    <t>09.10.20255</t>
-  </si>
-  <si>
-    <t>09.10.20256</t>
-  </si>
-  <si>
-    <t>09.10.20257</t>
-  </si>
-  <si>
-    <t>09.10.20258</t>
-  </si>
-  <si>
-    <t>09.10.20259</t>
-  </si>
-  <si>
-    <t>09.10.202510</t>
-  </si>
-  <si>
-    <t>09.10.202511</t>
-  </si>
-  <si>
-    <t>09.10.202512</t>
-  </si>
-  <si>
-    <t>09.10.202513</t>
-  </si>
-  <si>
-    <t>09.10.202514</t>
-  </si>
-  <si>
-    <t>09.10.202515</t>
-  </si>
-  <si>
-    <t>09.10.202516</t>
-  </si>
-  <si>
-    <t>09.10.202517</t>
-  </si>
-  <si>
-    <t>09.10.202518</t>
-  </si>
-  <si>
-    <t>09.10.202519</t>
-  </si>
-  <si>
-    <t>09.10.202520</t>
-  </si>
-  <si>
-    <t>09.10.202521</t>
-  </si>
-  <si>
-    <t>09.10.202522</t>
-  </si>
-  <si>
-    <t>09.10.202523</t>
-  </si>
-  <si>
-    <t>09.10.202524</t>
-  </si>
-  <si>
-    <t>10.10.20251</t>
-  </si>
-  <si>
-    <t>10.10.20252</t>
-  </si>
-  <si>
-    <t>10.10.20253</t>
-  </si>
-  <si>
-    <t>10.10.20254</t>
-  </si>
-  <si>
-    <t>10.10.20255</t>
-  </si>
-  <si>
-    <t>10.10.20256</t>
-  </si>
-  <si>
-    <t>10.10.20257</t>
-  </si>
-  <si>
-    <t>10.10.20258</t>
-  </si>
-  <si>
-    <t>10.10.20259</t>
-  </si>
-  <si>
-    <t>10.10.202510</t>
-  </si>
-  <si>
-    <t>10.10.202511</t>
+    <t>16.10.202516</t>
+  </si>
+  <si>
+    <t>16.10.202517</t>
+  </si>
+  <si>
+    <t>16.10.202518</t>
+  </si>
+  <si>
+    <t>16.10.202519</t>
+  </si>
+  <si>
+    <t>16.10.202520</t>
+  </si>
+  <si>
+    <t>16.10.202521</t>
+  </si>
+  <si>
+    <t>16.10.202522</t>
+  </si>
+  <si>
+    <t>16.10.202523</t>
+  </si>
+  <si>
+    <t>16.10.202524</t>
+  </si>
+  <si>
+    <t>17.10.20251</t>
+  </si>
+  <si>
+    <t>17.10.20252</t>
+  </si>
+  <si>
+    <t>17.10.20253</t>
+  </si>
+  <si>
+    <t>17.10.20254</t>
+  </si>
+  <si>
+    <t>17.10.20255</t>
+  </si>
+  <si>
+    <t>17.10.20256</t>
+  </si>
+  <si>
+    <t>17.10.20257</t>
+  </si>
+  <si>
+    <t>17.10.20258</t>
+  </si>
+  <si>
+    <t>17.10.20259</t>
+  </si>
+  <si>
+    <t>17.10.202510</t>
+  </si>
+  <si>
+    <t>17.10.202511</t>
+  </si>
+  <si>
+    <t>17.10.202512</t>
+  </si>
+  <si>
+    <t>17.10.202513</t>
+  </si>
+  <si>
+    <t>17.10.202514</t>
+  </si>
+  <si>
+    <t>17.10.202515</t>
+  </si>
+  <si>
+    <t>17.10.202516</t>
+  </si>
+  <si>
+    <t>17.10.202517</t>
+  </si>
+  <si>
+    <t>17.10.202518</t>
+  </si>
+  <si>
+    <t>17.10.202519</t>
+  </si>
+  <si>
+    <t>17.10.202520</t>
+  </si>
+  <si>
+    <t>17.10.202521</t>
+  </si>
+  <si>
+    <t>17.10.202522</t>
+  </si>
+  <si>
+    <t>17.10.202523</t>
+  </si>
+  <si>
+    <t>17.10.202524</t>
+  </si>
+  <si>
+    <t>18.10.20251</t>
+  </si>
+  <si>
+    <t>18.10.20252</t>
+  </si>
+  <si>
+    <t>18.10.20253</t>
+  </si>
+  <si>
+    <t>18.10.20254</t>
+  </si>
+  <si>
+    <t>18.10.20255</t>
+  </si>
+  <si>
+    <t>18.10.20256</t>
+  </si>
+  <si>
+    <t>18.10.20257</t>
+  </si>
+  <si>
+    <t>18.10.20258</t>
+  </si>
+  <si>
+    <t>18.10.20259</t>
+  </si>
+  <si>
+    <t>18.10.202510</t>
+  </si>
+  <si>
+    <t>18.10.202511</t>
+  </si>
+  <si>
+    <t>18.10.202512</t>
+  </si>
+  <si>
+    <t>18.10.202513</t>
+  </si>
+  <si>
+    <t>18.10.202514</t>
+  </si>
+  <si>
+    <t>18.10.202515</t>
+  </si>
+  <si>
+    <t>18.10.202516</t>
+  </si>
+  <si>
+    <t>18.10.202517</t>
+  </si>
+  <si>
+    <t>18.10.202518</t>
+  </si>
+  <si>
+    <t>18.10.202519</t>
+  </si>
+  <si>
+    <t>18.10.202520</t>
+  </si>
+  <si>
+    <t>18.10.202521</t>
+  </si>
+  <si>
+    <t>18.10.202522</t>
+  </si>
+  <si>
+    <t>18.10.202523</t>
+  </si>
+  <si>
+    <t>18.10.202524</t>
+  </si>
+  <si>
+    <t>19.10.20251</t>
+  </si>
+  <si>
+    <t>19.10.20252</t>
+  </si>
+  <si>
+    <t>19.10.20253</t>
+  </si>
+  <si>
+    <t>19.10.20254</t>
+  </si>
+  <si>
+    <t>19.10.20255</t>
+  </si>
+  <si>
+    <t>19.10.20256</t>
+  </si>
+  <si>
+    <t>19.10.20257</t>
+  </si>
+  <si>
+    <t>19.10.20258</t>
+  </si>
+  <si>
+    <t>19.10.20259</t>
+  </si>
+  <si>
+    <t>19.10.202510</t>
+  </si>
+  <si>
+    <t>19.10.202511</t>
+  </si>
+  <si>
+    <t>19.10.202512</t>
+  </si>
+  <si>
+    <t>19.10.202513</t>
+  </si>
+  <si>
+    <t>19.10.202514</t>
+  </si>
+  <si>
+    <t>19.10.202515</t>
+  </si>
+  <si>
+    <t>19.10.202516</t>
+  </si>
+  <si>
+    <t>19.10.202517</t>
+  </si>
+  <si>
+    <t>19.10.202518</t>
+  </si>
+  <si>
+    <t>19.10.202519</t>
+  </si>
+  <si>
+    <t>19.10.202520</t>
+  </si>
+  <si>
+    <t>19.10.202521</t>
+  </si>
+  <si>
+    <t>19.10.202522</t>
+  </si>
+  <si>
+    <t>19.10.202523</t>
+  </si>
+  <si>
+    <t>19.10.202524</t>
+  </si>
+  <si>
+    <t>20.10.20251</t>
+  </si>
+  <si>
+    <t>20.10.20252</t>
+  </si>
+  <si>
+    <t>20.10.20253</t>
+  </si>
+  <si>
+    <t>20.10.20254</t>
+  </si>
+  <si>
+    <t>20.10.20255</t>
+  </si>
+  <si>
+    <t>20.10.20256</t>
+  </si>
+  <si>
+    <t>20.10.20257</t>
+  </si>
+  <si>
+    <t>20.10.20258</t>
+  </si>
+  <si>
+    <t>20.10.20259</t>
+  </si>
+  <si>
+    <t>20.10.202510</t>
+  </si>
+  <si>
+    <t>20.10.202511</t>
+  </si>
+  <si>
+    <t>20.10.202512</t>
+  </si>
+  <si>
+    <t>20.10.202513</t>
+  </si>
+  <si>
+    <t>20.10.202514</t>
+  </si>
+  <si>
+    <t>20.10.202515</t>
+  </si>
+  <si>
+    <t>20.10.202516</t>
+  </si>
+  <si>
+    <t>20.10.202517</t>
+  </si>
+  <si>
+    <t>20.10.202518</t>
+  </si>
+  <si>
+    <t>20.10.202519</t>
+  </si>
+  <si>
+    <t>20.10.202520</t>
+  </si>
+  <si>
+    <t>20.10.202521</t>
+  </si>
+  <si>
+    <t>20.10.202522</t>
+  </si>
+  <si>
+    <t>20.10.202523</t>
+  </si>
+  <si>
+    <t>20.10.202524</t>
+  </si>
+  <si>
+    <t>21.10.20251</t>
+  </si>
+  <si>
+    <t>21.10.20252</t>
+  </si>
+  <si>
+    <t>21.10.20253</t>
+  </si>
+  <si>
+    <t>21.10.20254</t>
+  </si>
+  <si>
+    <t>21.10.20255</t>
+  </si>
+  <si>
+    <t>21.10.20256</t>
+  </si>
+  <si>
+    <t>21.10.20257</t>
+  </si>
+  <si>
+    <t>21.10.20258</t>
+  </si>
+  <si>
+    <t>21.10.20259</t>
+  </si>
+  <si>
+    <t>21.10.202510</t>
+  </si>
+  <si>
+    <t>21.10.202511</t>
+  </si>
+  <si>
+    <t>21.10.202512</t>
+  </si>
+  <si>
+    <t>21.10.202513</t>
+  </si>
+  <si>
+    <t>21.10.202514</t>
+  </si>
+  <si>
+    <t>21.10.202515</t>
+  </si>
+  <si>
+    <t>21.10.202516</t>
+  </si>
+  <si>
+    <t>21.10.202517</t>
+  </si>
+  <si>
+    <t>21.10.202518</t>
+  </si>
+  <si>
+    <t>21.10.202519</t>
+  </si>
+  <si>
+    <t>21.10.202520</t>
+  </si>
+  <si>
+    <t>21.10.202521</t>
+  </si>
+  <si>
+    <t>21.10.202522</t>
+  </si>
+  <si>
+    <t>21.10.202523</t>
+  </si>
+  <si>
+    <t>21.10.202524</t>
+  </si>
+  <si>
+    <t>22.10.20251</t>
+  </si>
+  <si>
+    <t>22.10.20252</t>
+  </si>
+  <si>
+    <t>22.10.20253</t>
+  </si>
+  <si>
+    <t>22.10.20254</t>
+  </si>
+  <si>
+    <t>22.10.20255</t>
+  </si>
+  <si>
+    <t>22.10.20256</t>
+  </si>
+  <si>
+    <t>22.10.20257</t>
+  </si>
+  <si>
+    <t>22.10.20258</t>
+  </si>
+  <si>
+    <t>22.10.20259</t>
+  </si>
+  <si>
+    <t>22.10.202510</t>
+  </si>
+  <si>
+    <t>22.10.202511</t>
+  </si>
+  <si>
+    <t>22.10.202512</t>
+  </si>
+  <si>
+    <t>22.10.202513</t>
+  </si>
+  <si>
+    <t>22.10.202514</t>
+  </si>
+  <si>
+    <t>22.10.202515</t>
+  </si>
+  <si>
+    <t>22.10.202516</t>
+  </si>
+  <si>
+    <t>22.10.202517</t>
+  </si>
+  <si>
+    <t>22.10.202518</t>
+  </si>
+  <si>
+    <t>22.10.202519</t>
+  </si>
+  <si>
+    <t>22.10.202520</t>
+  </si>
+  <si>
+    <t>22.10.202521</t>
+  </si>
+  <si>
+    <t>22.10.202522</t>
+  </si>
+  <si>
+    <t>22.10.202523</t>
+  </si>
+  <si>
+    <t>22.10.202524</t>
+  </si>
+  <si>
+    <t>23.10.20251</t>
+  </si>
+  <si>
+    <t>23.10.20252</t>
+  </si>
+  <si>
+    <t>23.10.20253</t>
+  </si>
+  <si>
+    <t>23.10.20254</t>
+  </si>
+  <si>
+    <t>23.10.20255</t>
+  </si>
+  <si>
+    <t>23.10.20256</t>
+  </si>
+  <si>
+    <t>23.10.20257</t>
+  </si>
+  <si>
+    <t>23.10.20258</t>
+  </si>
+  <si>
+    <t>23.10.20259</t>
+  </si>
+  <si>
+    <t>23.10.202510</t>
+  </si>
+  <si>
+    <t>23.10.202511</t>
+  </si>
+  <si>
+    <t>23.10.202512</t>
+  </si>
+  <si>
+    <t>23.10.202513</t>
+  </si>
+  <si>
+    <t>23.10.202514</t>
+  </si>
+  <si>
+    <t>23.10.202515</t>
+  </si>
+  <si>
+    <t>23.10.202516</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45933</v>
+        <v>45946</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>0.034</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45933</v>
+        <v>45946</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>0.034</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45933</v>
+        <v>45946</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>0.513</v>
+        <v>0.286</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45933</v>
+        <v>45946</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>0.408</v>
+        <v>0.115</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45933</v>
+        <v>45946</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>0.408</v>
+        <v>0.068</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45933</v>
+        <v>45946</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>0.376</v>
+        <v>0.048</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45933</v>
+        <v>45946</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>0.292</v>
+        <v>0.016</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45933</v>
+        <v>45946</v>
       </c>
       <c r="B9">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C9">
-        <v>0.246</v>
+        <v>0.016</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45933</v>
+        <v>45946</v>
       </c>
       <c r="B10">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>0.108</v>
+        <v>0.016</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45933</v>
+        <v>45947</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0.222</v>
+        <v>0.013</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45933</v>
+        <v>45947</v>
       </c>
       <c r="B12">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>0.209</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45933</v>
+        <v>45947</v>
       </c>
       <c r="B13">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>0.119</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45933</v>
+        <v>45947</v>
       </c>
       <c r="B14">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>0.109</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45933</v>
+        <v>45947</v>
       </c>
       <c r="B15">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.201</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.698</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1.292</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>2.273</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>2.547</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C23">
-        <v>0.083</v>
+        <v>3.069</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B24">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C24">
-        <v>0.265</v>
+        <v>2.766</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C25">
-        <v>0.368</v>
+        <v>2.217</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B26">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C26">
-        <v>0.546</v>
+        <v>1.552</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C27">
-        <v>0.5649999999999999</v>
+        <v>1.001</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B28">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C28">
-        <v>0.57</v>
+        <v>0.423</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B29">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C29">
-        <v>0.916</v>
+        <v>0.115</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B30">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C30">
-        <v>0.971</v>
+        <v>0.068</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B31">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C31">
-        <v>1.014</v>
+        <v>0.068</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B32">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C32">
-        <v>0.636</v>
+        <v>0.016</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B33">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C33">
-        <v>0.297</v>
+        <v>0.016</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45934</v>
+        <v>45947</v>
       </c>
       <c r="B34">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C34">
-        <v>0.165</v>
+        <v>0.016</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45934</v>
+        <v>45948</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>0.048</v>
+        <v>0.013</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45934</v>
+        <v>45948</v>
       </c>
       <c r="B36">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C36">
-        <v>0.048</v>
+        <v>0.013</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45934</v>
+        <v>45948</v>
       </c>
       <c r="B37">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C37">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45934</v>
+        <v>45948</v>
       </c>
       <c r="B38">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C38">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45934</v>
+        <v>45948</v>
       </c>
       <c r="B39">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C39">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C40">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C41">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>0.083</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.255</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B44">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>0.496</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1.048</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1.104</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C47">
-        <v>0.26</v>
+        <v>1.099</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B48">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C48">
-        <v>0.872</v>
+        <v>1.025</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B49">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C49">
-        <v>1.931</v>
+        <v>0.994</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B50">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C50">
-        <v>2.538</v>
+        <v>0.861</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C51">
-        <v>3.142</v>
+        <v>0.454</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B52">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C52">
-        <v>3.487</v>
+        <v>0.236</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B53">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C53">
-        <v>3.418</v>
+        <v>0.106</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B54">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C54">
-        <v>3.159</v>
+        <v>0.063</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B55">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C55">
-        <v>2.222</v>
+        <v>0.063</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B56">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C56">
-        <v>1.686</v>
+        <v>0.011</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B57">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C57">
-        <v>0.881</v>
+        <v>0.011</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45935</v>
+        <v>45948</v>
       </c>
       <c r="B58">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C58">
-        <v>0.236</v>
+        <v>0.011</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45935</v>
+        <v>45949</v>
       </c>
       <c r="B59">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>0.064</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45935</v>
+        <v>45949</v>
       </c>
       <c r="B60">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C60">
-        <v>0.064</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45935</v>
+        <v>45949</v>
       </c>
       <c r="B61">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C61">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45935</v>
+        <v>45949</v>
       </c>
       <c r="B62">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C62">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45935</v>
+        <v>45949</v>
       </c>
       <c r="B63">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C63">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C64">
         <v>0.013</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C65">
         <v>0.013</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C66">
-        <v>0.013</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B67">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C67">
-        <v>0.013</v>
+        <v>0.316</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B68">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B69">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1.065</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1.435</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C71">
-        <v>0.111</v>
+        <v>1.742</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B72">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C72">
-        <v>0.316</v>
+        <v>1.572</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B73">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C73">
-        <v>0.67</v>
+        <v>1.726</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B74">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C74">
-        <v>1.023</v>
+        <v>1.41</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B75">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C75">
-        <v>0.976</v>
+        <v>0.947</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B76">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C76">
-        <v>0.5649999999999999</v>
+        <v>0.406</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B77">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C77">
-        <v>0.91</v>
+        <v>0.091</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B78">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C78">
-        <v>0.96</v>
+        <v>0.044</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B79">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C79">
-        <v>0.9419999999999999</v>
+        <v>0.044</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B80">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C80">
-        <v>0.398</v>
+        <v>0.011</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B81">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C81">
-        <v>0.286</v>
+        <v>0.011</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45936</v>
+        <v>45949</v>
       </c>
       <c r="B82">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C82">
-        <v>0.115</v>
+        <v>0.011</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45936</v>
+        <v>45950</v>
       </c>
       <c r="B83">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C83">
-        <v>0.068</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45936</v>
+        <v>45950</v>
       </c>
       <c r="B84">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C84">
-        <v>0.068</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45936</v>
+        <v>45950</v>
       </c>
       <c r="B85">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C85">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45936</v>
+        <v>45950</v>
       </c>
       <c r="B86">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C86">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45936</v>
+        <v>45950</v>
       </c>
       <c r="B87">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C87">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>0.111</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B91">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>0.497</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B92">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>1.878</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B93">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>2.306</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B94">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>2.902</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B95">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C95">
-        <v>0.392</v>
+        <v>3.31</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B96">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C96">
-        <v>0.637</v>
+        <v>3.289</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B97">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C97">
-        <v>1.161</v>
+        <v>3.04</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B98">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C98">
-        <v>1.855</v>
+        <v>2.069</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B99">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C99">
-        <v>2.459</v>
+        <v>1.724</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B100">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C100">
-        <v>2.509</v>
+        <v>0.483</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B101">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C101">
-        <v>2.364</v>
+        <v>0.1</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B102">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C102">
-        <v>1.655</v>
+        <v>0.055</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B103">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C103">
-        <v>1.354</v>
+        <v>0.044</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B104">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C104">
-        <v>1.009</v>
+        <v>0.011</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B105">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C105">
-        <v>0.473</v>
+        <v>0.011</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45937</v>
+        <v>45950</v>
       </c>
       <c r="B106">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C106">
-        <v>0.426</v>
+        <v>0.011</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45937</v>
+        <v>45951</v>
       </c>
       <c r="B107">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C107">
-        <v>0.048</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45937</v>
+        <v>45951</v>
       </c>
       <c r="B108">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C108">
-        <v>0.048</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45937</v>
+        <v>45951</v>
       </c>
       <c r="B109">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C109">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45937</v>
+        <v>45951</v>
       </c>
       <c r="B110">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C110">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45937</v>
+        <v>45951</v>
       </c>
       <c r="B111">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C111">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C113">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C114">
-        <v>0.013</v>
+        <v>0.083</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B115">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>0.495</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B116">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>1.484</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B117">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>2.032</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B118">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>2.495</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B119">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C119">
-        <v>0.275</v>
+        <v>3.036</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B120">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C120">
-        <v>0.542</v>
+        <v>2.996</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B121">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C121">
-        <v>1.134</v>
+        <v>2.659</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B122">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C122">
-        <v>2.007</v>
+        <v>1.965</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B123">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C123">
-        <v>2.464</v>
+        <v>1.234</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B124">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C124">
-        <v>2.514</v>
+        <v>0.395</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B125">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C125">
-        <v>2.463</v>
+        <v>0.111</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B126">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C126">
-        <v>1.794</v>
+        <v>0.068</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B127">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C127">
-        <v>1.959</v>
+        <v>0.048</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B128">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C128">
-        <v>0.974</v>
+        <v>0.016</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B129">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C129">
-        <v>0.386</v>
+        <v>0.016</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45938</v>
+        <v>45951</v>
       </c>
       <c r="B130">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C130">
-        <v>0.276</v>
+        <v>0.016</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45938</v>
+        <v>45952</v>
       </c>
       <c r="B131">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C131">
-        <v>0.048</v>
+        <v>0.013</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45938</v>
+        <v>45952</v>
       </c>
       <c r="B132">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C132">
-        <v>0.048</v>
+        <v>0.013</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45938</v>
+        <v>45952</v>
       </c>
       <c r="B133">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C133">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45938</v>
+        <v>45952</v>
       </c>
       <c r="B134">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C134">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45938</v>
+        <v>45952</v>
       </c>
       <c r="B135">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C135">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C136">
         <v>0.013</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B137">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C137">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B138">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C138">
-        <v>0.013</v>
+        <v>0.083</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B139">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C139">
-        <v>0.013</v>
+        <v>0.265</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B140">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C140">
-        <v>0.013</v>
+        <v>0.733</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B141">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C141">
-        <v>0.013</v>
+        <v>1.255</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B142">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C142">
-        <v>0.013</v>
+        <v>1.796</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B143">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C143">
-        <v>0.182</v>
+        <v>2.059</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B144">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C144">
-        <v>0.45</v>
+        <v>1.973</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B145">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C145">
-        <v>1.144</v>
+        <v>1.855</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B146">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C146">
-        <v>1.945</v>
+        <v>1.51</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B147">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C147">
-        <v>2.31</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B148">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C148">
-        <v>2.793</v>
+        <v>0.286</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B149">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C149">
-        <v>2.7</v>
+        <v>0.111</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B150">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C150">
-        <v>2.405</v>
+        <v>0.068</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B151">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C151">
-        <v>1.81</v>
+        <v>0.068</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B152">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C152">
-        <v>1.181</v>
+        <v>0.016</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B153">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C153">
-        <v>0.637</v>
+        <v>0.016</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45939</v>
+        <v>45952</v>
       </c>
       <c r="B154">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C154">
-        <v>0.411</v>
+        <v>0.016</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45939</v>
+        <v>45953</v>
       </c>
       <c r="B155">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C155">
-        <v>0.064</v>
+        <v>0.013</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45939</v>
+        <v>45953</v>
       </c>
       <c r="B156">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C156">
-        <v>0.064</v>
+        <v>0.013</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45939</v>
+        <v>45953</v>
       </c>
       <c r="B157">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C157">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45939</v>
+        <v>45953</v>
       </c>
       <c r="B158">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C158">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45939</v>
+        <v>45953</v>
       </c>
       <c r="B159">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C159">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B161">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B162">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B163">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C163">
-        <v>0.013</v>
+        <v>0.41</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B164">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C164">
-        <v>0.013</v>
+        <v>1.134</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B165">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C165">
-        <v>0.013</v>
+        <v>1.742</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B166">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C166">
-        <v>0.013</v>
+        <v>2.017</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B167">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C167">
-        <v>0.267</v>
+        <v>2.251</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B168">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C168">
-        <v>0.518</v>
+        <v>1.994</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B169">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C169">
-        <v>1.065</v>
+        <v>1.835</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45940</v>
+        <v>45953</v>
       </c>
       <c r="B170">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C170">
-        <v>1.566</v>
+        <v>1.792</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Switching to winter DST time
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>16.10.202516</t>
-  </si>
-  <si>
-    <t>16.10.202517</t>
-  </si>
-  <si>
-    <t>16.10.202518</t>
-  </si>
-  <si>
-    <t>16.10.202519</t>
-  </si>
-  <si>
-    <t>16.10.202520</t>
-  </si>
-  <si>
-    <t>16.10.202521</t>
-  </si>
-  <si>
-    <t>16.10.202522</t>
-  </si>
-  <si>
-    <t>16.10.202523</t>
-  </si>
-  <si>
-    <t>16.10.202524</t>
-  </si>
-  <si>
-    <t>17.10.20251</t>
-  </si>
-  <si>
-    <t>17.10.20252</t>
-  </si>
-  <si>
-    <t>17.10.20253</t>
-  </si>
-  <si>
-    <t>17.10.20254</t>
-  </si>
-  <si>
-    <t>17.10.20255</t>
-  </si>
-  <si>
-    <t>17.10.20256</t>
-  </si>
-  <si>
-    <t>17.10.20257</t>
-  </si>
-  <si>
-    <t>17.10.20258</t>
-  </si>
-  <si>
-    <t>17.10.20259</t>
-  </si>
-  <si>
-    <t>17.10.202510</t>
-  </si>
-  <si>
-    <t>17.10.202511</t>
-  </si>
-  <si>
-    <t>17.10.202512</t>
-  </si>
-  <si>
-    <t>17.10.202513</t>
-  </si>
-  <si>
-    <t>17.10.202514</t>
-  </si>
-  <si>
-    <t>17.10.202515</t>
-  </si>
-  <si>
-    <t>17.10.202516</t>
-  </si>
-  <si>
-    <t>17.10.202517</t>
-  </si>
-  <si>
-    <t>17.10.202518</t>
-  </si>
-  <si>
-    <t>17.10.202519</t>
-  </si>
-  <si>
-    <t>17.10.202520</t>
-  </si>
-  <si>
-    <t>17.10.202521</t>
-  </si>
-  <si>
-    <t>17.10.202522</t>
-  </si>
-  <si>
-    <t>17.10.202523</t>
-  </si>
-  <si>
-    <t>17.10.202524</t>
-  </si>
-  <si>
-    <t>18.10.20251</t>
-  </si>
-  <si>
-    <t>18.10.20252</t>
-  </si>
-  <si>
-    <t>18.10.20253</t>
-  </si>
-  <si>
-    <t>18.10.20254</t>
-  </si>
-  <si>
-    <t>18.10.20255</t>
-  </si>
-  <si>
-    <t>18.10.20256</t>
-  </si>
-  <si>
-    <t>18.10.20257</t>
-  </si>
-  <si>
-    <t>18.10.20258</t>
-  </si>
-  <si>
-    <t>18.10.20259</t>
-  </si>
-  <si>
-    <t>18.10.202510</t>
-  </si>
-  <si>
-    <t>18.10.202511</t>
-  </si>
-  <si>
-    <t>18.10.202512</t>
-  </si>
-  <si>
-    <t>18.10.202513</t>
-  </si>
-  <si>
-    <t>18.10.202514</t>
-  </si>
-  <si>
-    <t>18.10.202515</t>
-  </si>
-  <si>
-    <t>18.10.202516</t>
-  </si>
-  <si>
-    <t>18.10.202517</t>
-  </si>
-  <si>
-    <t>18.10.202518</t>
-  </si>
-  <si>
-    <t>18.10.202519</t>
-  </si>
-  <si>
-    <t>18.10.202520</t>
-  </si>
-  <si>
-    <t>18.10.202521</t>
-  </si>
-  <si>
-    <t>18.10.202522</t>
-  </si>
-  <si>
-    <t>18.10.202523</t>
-  </si>
-  <si>
-    <t>18.10.202524</t>
-  </si>
-  <si>
-    <t>19.10.20251</t>
-  </si>
-  <si>
-    <t>19.10.20252</t>
-  </si>
-  <si>
-    <t>19.10.20253</t>
-  </si>
-  <si>
-    <t>19.10.20254</t>
-  </si>
-  <si>
-    <t>19.10.20255</t>
-  </si>
-  <si>
-    <t>19.10.20256</t>
-  </si>
-  <si>
-    <t>19.10.20257</t>
-  </si>
-  <si>
-    <t>19.10.20258</t>
-  </si>
-  <si>
-    <t>19.10.20259</t>
-  </si>
-  <si>
-    <t>19.10.202510</t>
-  </si>
-  <si>
-    <t>19.10.202511</t>
-  </si>
-  <si>
-    <t>19.10.202512</t>
-  </si>
-  <si>
-    <t>19.10.202513</t>
-  </si>
-  <si>
-    <t>19.10.202514</t>
-  </si>
-  <si>
-    <t>19.10.202515</t>
-  </si>
-  <si>
-    <t>19.10.202516</t>
-  </si>
-  <si>
-    <t>19.10.202517</t>
-  </si>
-  <si>
-    <t>19.10.202518</t>
-  </si>
-  <si>
-    <t>19.10.202519</t>
-  </si>
-  <si>
-    <t>19.10.202520</t>
-  </si>
-  <si>
-    <t>19.10.202521</t>
-  </si>
-  <si>
-    <t>19.10.202522</t>
-  </si>
-  <si>
-    <t>19.10.202523</t>
-  </si>
-  <si>
-    <t>19.10.202524</t>
-  </si>
-  <si>
-    <t>20.10.20251</t>
-  </si>
-  <si>
-    <t>20.10.20252</t>
-  </si>
-  <si>
-    <t>20.10.20253</t>
-  </si>
-  <si>
-    <t>20.10.20254</t>
-  </si>
-  <si>
-    <t>20.10.20255</t>
-  </si>
-  <si>
-    <t>20.10.20256</t>
-  </si>
-  <si>
-    <t>20.10.20257</t>
-  </si>
-  <si>
-    <t>20.10.20258</t>
-  </si>
-  <si>
-    <t>20.10.20259</t>
-  </si>
-  <si>
-    <t>20.10.202510</t>
-  </si>
-  <si>
-    <t>20.10.202511</t>
-  </si>
-  <si>
-    <t>20.10.202512</t>
-  </si>
-  <si>
-    <t>20.10.202513</t>
-  </si>
-  <si>
-    <t>20.10.202514</t>
-  </si>
-  <si>
-    <t>20.10.202515</t>
-  </si>
-  <si>
-    <t>20.10.202516</t>
-  </si>
-  <si>
-    <t>20.10.202517</t>
-  </si>
-  <si>
-    <t>20.10.202518</t>
-  </si>
-  <si>
-    <t>20.10.202519</t>
-  </si>
-  <si>
-    <t>20.10.202520</t>
-  </si>
-  <si>
-    <t>20.10.202521</t>
-  </si>
-  <si>
-    <t>20.10.202522</t>
-  </si>
-  <si>
-    <t>20.10.202523</t>
-  </si>
-  <si>
-    <t>20.10.202524</t>
-  </si>
-  <si>
-    <t>21.10.20251</t>
-  </si>
-  <si>
-    <t>21.10.20252</t>
-  </si>
-  <si>
-    <t>21.10.20253</t>
-  </si>
-  <si>
-    <t>21.10.20254</t>
-  </si>
-  <si>
-    <t>21.10.20255</t>
-  </si>
-  <si>
-    <t>21.10.20256</t>
-  </si>
-  <si>
-    <t>21.10.20257</t>
-  </si>
-  <si>
-    <t>21.10.20258</t>
-  </si>
-  <si>
-    <t>21.10.20259</t>
-  </si>
-  <si>
-    <t>21.10.202510</t>
-  </si>
-  <si>
-    <t>21.10.202511</t>
-  </si>
-  <si>
-    <t>21.10.202512</t>
-  </si>
-  <si>
-    <t>21.10.202513</t>
-  </si>
-  <si>
-    <t>21.10.202514</t>
-  </si>
-  <si>
-    <t>21.10.202515</t>
-  </si>
-  <si>
-    <t>21.10.202516</t>
-  </si>
-  <si>
-    <t>21.10.202517</t>
-  </si>
-  <si>
-    <t>21.10.202518</t>
-  </si>
-  <si>
-    <t>21.10.202519</t>
-  </si>
-  <si>
-    <t>21.10.202520</t>
-  </si>
-  <si>
-    <t>21.10.202521</t>
-  </si>
-  <si>
-    <t>21.10.202522</t>
-  </si>
-  <si>
-    <t>21.10.202523</t>
-  </si>
-  <si>
-    <t>21.10.202524</t>
-  </si>
-  <si>
-    <t>22.10.20251</t>
-  </si>
-  <si>
-    <t>22.10.20252</t>
-  </si>
-  <si>
-    <t>22.10.20253</t>
-  </si>
-  <si>
-    <t>22.10.20254</t>
-  </si>
-  <si>
-    <t>22.10.20255</t>
-  </si>
-  <si>
-    <t>22.10.20256</t>
-  </si>
-  <si>
-    <t>22.10.20257</t>
-  </si>
-  <si>
-    <t>22.10.20258</t>
-  </si>
-  <si>
-    <t>22.10.20259</t>
-  </si>
-  <si>
-    <t>22.10.202510</t>
-  </si>
-  <si>
-    <t>22.10.202511</t>
-  </si>
-  <si>
-    <t>22.10.202512</t>
-  </si>
-  <si>
-    <t>22.10.202513</t>
-  </si>
-  <si>
-    <t>22.10.202514</t>
-  </si>
-  <si>
-    <t>22.10.202515</t>
-  </si>
-  <si>
-    <t>22.10.202516</t>
-  </si>
-  <si>
-    <t>22.10.202517</t>
-  </si>
-  <si>
-    <t>22.10.202518</t>
-  </si>
-  <si>
-    <t>22.10.202519</t>
-  </si>
-  <si>
-    <t>22.10.202520</t>
-  </si>
-  <si>
-    <t>22.10.202521</t>
-  </si>
-  <si>
-    <t>22.10.202522</t>
-  </si>
-  <si>
-    <t>22.10.202523</t>
-  </si>
-  <si>
-    <t>22.10.202524</t>
-  </si>
-  <si>
-    <t>23.10.20251</t>
-  </si>
-  <si>
-    <t>23.10.20252</t>
-  </si>
-  <si>
-    <t>23.10.20253</t>
-  </si>
-  <si>
-    <t>23.10.20254</t>
-  </si>
-  <si>
-    <t>23.10.20255</t>
-  </si>
-  <si>
-    <t>23.10.20256</t>
-  </si>
-  <si>
-    <t>23.10.20257</t>
-  </si>
-  <si>
-    <t>23.10.20258</t>
-  </si>
-  <si>
-    <t>23.10.20259</t>
-  </si>
-  <si>
-    <t>23.10.202510</t>
-  </si>
-  <si>
-    <t>23.10.202511</t>
-  </si>
-  <si>
-    <t>23.10.202512</t>
-  </si>
-  <si>
-    <t>23.10.202513</t>
-  </si>
-  <si>
-    <t>23.10.202514</t>
-  </si>
-  <si>
-    <t>23.10.202515</t>
-  </si>
-  <si>
-    <t>23.10.202516</t>
+    <t>25.10.202512</t>
+  </si>
+  <si>
+    <t>25.10.202513</t>
+  </si>
+  <si>
+    <t>25.10.202514</t>
+  </si>
+  <si>
+    <t>25.10.202515</t>
+  </si>
+  <si>
+    <t>25.10.202516</t>
+  </si>
+  <si>
+    <t>25.10.202517</t>
+  </si>
+  <si>
+    <t>25.10.202518</t>
+  </si>
+  <si>
+    <t>25.10.202519</t>
+  </si>
+  <si>
+    <t>25.10.202520</t>
+  </si>
+  <si>
+    <t>25.10.202521</t>
+  </si>
+  <si>
+    <t>25.10.202522</t>
+  </si>
+  <si>
+    <t>25.10.202523</t>
+  </si>
+  <si>
+    <t>25.10.202524</t>
+  </si>
+  <si>
+    <t>26.10.20251</t>
+  </si>
+  <si>
+    <t>26.10.20252</t>
+  </si>
+  <si>
+    <t>26.10.20253</t>
+  </si>
+  <si>
+    <t>26.10.20254</t>
+  </si>
+  <si>
+    <t>26.10.20255</t>
+  </si>
+  <si>
+    <t>26.10.20256</t>
+  </si>
+  <si>
+    <t>26.10.20257</t>
+  </si>
+  <si>
+    <t>26.10.20258</t>
+  </si>
+  <si>
+    <t>26.10.20259</t>
+  </si>
+  <si>
+    <t>26.10.202510</t>
+  </si>
+  <si>
+    <t>26.10.202511</t>
+  </si>
+  <si>
+    <t>26.10.202512</t>
+  </si>
+  <si>
+    <t>26.10.202513</t>
+  </si>
+  <si>
+    <t>26.10.202514</t>
+  </si>
+  <si>
+    <t>26.10.202515</t>
+  </si>
+  <si>
+    <t>26.10.202516</t>
+  </si>
+  <si>
+    <t>26.10.202517</t>
+  </si>
+  <si>
+    <t>26.10.202518</t>
+  </si>
+  <si>
+    <t>26.10.202519</t>
+  </si>
+  <si>
+    <t>26.10.202520</t>
+  </si>
+  <si>
+    <t>26.10.202521</t>
+  </si>
+  <si>
+    <t>26.10.202522</t>
+  </si>
+  <si>
+    <t>26.10.202523</t>
+  </si>
+  <si>
+    <t>26.10.202524</t>
+  </si>
+  <si>
+    <t>27.10.20251</t>
+  </si>
+  <si>
+    <t>27.10.20252</t>
+  </si>
+  <si>
+    <t>27.10.20253</t>
+  </si>
+  <si>
+    <t>27.10.20254</t>
+  </si>
+  <si>
+    <t>27.10.20255</t>
+  </si>
+  <si>
+    <t>27.10.20256</t>
+  </si>
+  <si>
+    <t>27.10.20257</t>
+  </si>
+  <si>
+    <t>27.10.20258</t>
+  </si>
+  <si>
+    <t>27.10.20259</t>
+  </si>
+  <si>
+    <t>27.10.202510</t>
+  </si>
+  <si>
+    <t>27.10.202511</t>
+  </si>
+  <si>
+    <t>27.10.202512</t>
+  </si>
+  <si>
+    <t>27.10.202513</t>
+  </si>
+  <si>
+    <t>27.10.202514</t>
+  </si>
+  <si>
+    <t>27.10.202515</t>
+  </si>
+  <si>
+    <t>27.10.202516</t>
+  </si>
+  <si>
+    <t>27.10.202517</t>
+  </si>
+  <si>
+    <t>27.10.202518</t>
+  </si>
+  <si>
+    <t>27.10.202519</t>
+  </si>
+  <si>
+    <t>27.10.202520</t>
+  </si>
+  <si>
+    <t>27.10.202521</t>
+  </si>
+  <si>
+    <t>27.10.202522</t>
+  </si>
+  <si>
+    <t>27.10.202523</t>
+  </si>
+  <si>
+    <t>27.10.202524</t>
+  </si>
+  <si>
+    <t>28.10.20251</t>
+  </si>
+  <si>
+    <t>28.10.20252</t>
+  </si>
+  <si>
+    <t>28.10.20253</t>
+  </si>
+  <si>
+    <t>28.10.20254</t>
+  </si>
+  <si>
+    <t>28.10.20255</t>
+  </si>
+  <si>
+    <t>28.10.20256</t>
+  </si>
+  <si>
+    <t>28.10.20257</t>
+  </si>
+  <si>
+    <t>28.10.20258</t>
+  </si>
+  <si>
+    <t>28.10.20259</t>
+  </si>
+  <si>
+    <t>28.10.202510</t>
+  </si>
+  <si>
+    <t>28.10.202511</t>
+  </si>
+  <si>
+    <t>28.10.202512</t>
+  </si>
+  <si>
+    <t>28.10.202513</t>
+  </si>
+  <si>
+    <t>28.10.202514</t>
+  </si>
+  <si>
+    <t>28.10.202515</t>
+  </si>
+  <si>
+    <t>28.10.202516</t>
+  </si>
+  <si>
+    <t>28.10.202517</t>
+  </si>
+  <si>
+    <t>28.10.202518</t>
+  </si>
+  <si>
+    <t>28.10.202519</t>
+  </si>
+  <si>
+    <t>28.10.202520</t>
+  </si>
+  <si>
+    <t>28.10.202521</t>
+  </si>
+  <si>
+    <t>28.10.202522</t>
+  </si>
+  <si>
+    <t>28.10.202523</t>
+  </si>
+  <si>
+    <t>28.10.202524</t>
+  </si>
+  <si>
+    <t>29.10.20251</t>
+  </si>
+  <si>
+    <t>29.10.20252</t>
+  </si>
+  <si>
+    <t>29.10.20253</t>
+  </si>
+  <si>
+    <t>29.10.20254</t>
+  </si>
+  <si>
+    <t>29.10.20255</t>
+  </si>
+  <si>
+    <t>29.10.20256</t>
+  </si>
+  <si>
+    <t>29.10.20257</t>
+  </si>
+  <si>
+    <t>29.10.20258</t>
+  </si>
+  <si>
+    <t>29.10.20259</t>
+  </si>
+  <si>
+    <t>29.10.202510</t>
+  </si>
+  <si>
+    <t>29.10.202511</t>
+  </si>
+  <si>
+    <t>29.10.202512</t>
+  </si>
+  <si>
+    <t>29.10.202513</t>
+  </si>
+  <si>
+    <t>29.10.202514</t>
+  </si>
+  <si>
+    <t>29.10.202515</t>
+  </si>
+  <si>
+    <t>29.10.202516</t>
+  </si>
+  <si>
+    <t>29.10.202517</t>
+  </si>
+  <si>
+    <t>29.10.202518</t>
+  </si>
+  <si>
+    <t>29.10.202519</t>
+  </si>
+  <si>
+    <t>29.10.202520</t>
+  </si>
+  <si>
+    <t>29.10.202521</t>
+  </si>
+  <si>
+    <t>29.10.202522</t>
+  </si>
+  <si>
+    <t>29.10.202523</t>
+  </si>
+  <si>
+    <t>29.10.202524</t>
+  </si>
+  <si>
+    <t>30.10.20251</t>
+  </si>
+  <si>
+    <t>30.10.20252</t>
+  </si>
+  <si>
+    <t>30.10.20253</t>
+  </si>
+  <si>
+    <t>30.10.20254</t>
+  </si>
+  <si>
+    <t>30.10.20255</t>
+  </si>
+  <si>
+    <t>30.10.20256</t>
+  </si>
+  <si>
+    <t>30.10.20257</t>
+  </si>
+  <si>
+    <t>30.10.20258</t>
+  </si>
+  <si>
+    <t>30.10.20259</t>
+  </si>
+  <si>
+    <t>30.10.202510</t>
+  </si>
+  <si>
+    <t>30.10.202511</t>
+  </si>
+  <si>
+    <t>30.10.202512</t>
+  </si>
+  <si>
+    <t>30.10.202513</t>
+  </si>
+  <si>
+    <t>30.10.202514</t>
+  </si>
+  <si>
+    <t>30.10.202515</t>
+  </si>
+  <si>
+    <t>30.10.202516</t>
+  </si>
+  <si>
+    <t>30.10.202517</t>
+  </si>
+  <si>
+    <t>30.10.202518</t>
+  </si>
+  <si>
+    <t>30.10.202519</t>
+  </si>
+  <si>
+    <t>30.10.202520</t>
+  </si>
+  <si>
+    <t>30.10.202521</t>
+  </si>
+  <si>
+    <t>30.10.202522</t>
+  </si>
+  <si>
+    <t>30.10.202523</t>
+  </si>
+  <si>
+    <t>30.10.202524</t>
+  </si>
+  <si>
+    <t>31.10.20251</t>
+  </si>
+  <si>
+    <t>31.10.20252</t>
+  </si>
+  <si>
+    <t>31.10.20253</t>
+  </si>
+  <si>
+    <t>31.10.20254</t>
+  </si>
+  <si>
+    <t>31.10.20255</t>
+  </si>
+  <si>
+    <t>31.10.20256</t>
+  </si>
+  <si>
+    <t>31.10.20257</t>
+  </si>
+  <si>
+    <t>31.10.20258</t>
+  </si>
+  <si>
+    <t>31.10.20259</t>
+  </si>
+  <si>
+    <t>31.10.202510</t>
+  </si>
+  <si>
+    <t>31.10.202511</t>
+  </si>
+  <si>
+    <t>31.10.202512</t>
+  </si>
+  <si>
+    <t>31.10.202513</t>
+  </si>
+  <si>
+    <t>31.10.202514</t>
+  </si>
+  <si>
+    <t>31.10.202515</t>
+  </si>
+  <si>
+    <t>31.10.202516</t>
+  </si>
+  <si>
+    <t>31.10.202517</t>
+  </si>
+  <si>
+    <t>31.10.202518</t>
+  </si>
+  <si>
+    <t>31.10.202519</t>
+  </si>
+  <si>
+    <t>31.10.202520</t>
+  </si>
+  <si>
+    <t>31.10.202521</t>
+  </si>
+  <si>
+    <t>31.10.202522</t>
+  </si>
+  <si>
+    <t>31.10.202523</t>
+  </si>
+  <si>
+    <t>31.10.202524</t>
+  </si>
+  <si>
+    <t>01.11.20251</t>
+  </si>
+  <si>
+    <t>01.11.20252</t>
+  </si>
+  <si>
+    <t>01.11.20253</t>
+  </si>
+  <si>
+    <t>01.11.20254</t>
+  </si>
+  <si>
+    <t>01.11.20255</t>
+  </si>
+  <si>
+    <t>01.11.20256</t>
+  </si>
+  <si>
+    <t>01.11.20257</t>
+  </si>
+  <si>
+    <t>01.11.20258</t>
+  </si>
+  <si>
+    <t>01.11.20259</t>
+  </si>
+  <si>
+    <t>01.11.202510</t>
+  </si>
+  <si>
+    <t>01.11.202511</t>
+  </si>
+  <si>
+    <t>01.11.202512</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45946</v>
+        <v>45955</v>
       </c>
       <c r="B2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>0.034</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45946</v>
+        <v>45955</v>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>0.034</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45946</v>
+        <v>45955</v>
       </c>
       <c r="B4">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>0.286</v>
+        <v>3.069</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45946</v>
+        <v>45955</v>
       </c>
       <c r="B5">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>0.115</v>
+        <v>2.379</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45946</v>
+        <v>45955</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>0.068</v>
+        <v>2.02</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45946</v>
+        <v>45955</v>
       </c>
       <c r="B7">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>0.048</v>
+        <v>0.991</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45946</v>
+        <v>45955</v>
       </c>
       <c r="B8">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8">
-        <v>0.016</v>
+        <v>0.429</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45946</v>
+        <v>45955</v>
       </c>
       <c r="B9">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>0.016</v>
+        <v>0.116</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45946</v>
+        <v>45955</v>
       </c>
       <c r="B10">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>0.016</v>
+        <v>0.073</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45947</v>
+        <v>45955</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>0.013</v>
+        <v>0.073</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45947</v>
+        <v>45955</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45947</v>
+        <v>45955</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45947</v>
+        <v>45955</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>0.201</v>
+        <v>0.013</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B19">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>0.698</v>
+        <v>0.013</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>1.292</v>
+        <v>0.013</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B21">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>2.273</v>
+        <v>0.013</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B22">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>2.547</v>
+        <v>0.04</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B23">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>3.069</v>
+        <v>0.265</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B24">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>2.766</v>
+        <v>0.324</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B25">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C25">
-        <v>2.217</v>
+        <v>0.551</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B26">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>1.552</v>
+        <v>0.832</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B27">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <v>1.001</v>
+        <v>0.976</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B28">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C28">
-        <v>0.423</v>
+        <v>1.036</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B29">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C29">
-        <v>0.115</v>
+        <v>0.997</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B30">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C30">
-        <v>0.068</v>
+        <v>0.979</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B31">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <v>0.068</v>
+        <v>0.577</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B32">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C32">
-        <v>0.016</v>
+        <v>0.241</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B33">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C33">
-        <v>0.016</v>
+        <v>0.111</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45947</v>
+        <v>45956</v>
       </c>
       <c r="B34">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C34">
-        <v>0.016</v>
+        <v>0.068</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45948</v>
+        <v>45956</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C35">
-        <v>0.013</v>
+        <v>0.063</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45948</v>
+        <v>45956</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C36">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45948</v>
+        <v>45956</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C37">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45948</v>
+        <v>45956</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C38">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B40">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B41">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B42">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C42">
-        <v>0.083</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B43">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C43">
-        <v>0.255</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B44">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C44">
-        <v>0.496</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B45">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>1.048</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B46">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C46">
-        <v>1.104</v>
+        <v>0.056</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B47">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C47">
-        <v>1.099</v>
+        <v>0.255</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B48">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C48">
-        <v>1.025</v>
+        <v>0.423</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B49">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C49">
-        <v>0.994</v>
+        <v>0.695</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B50">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>0.861</v>
+        <v>0.987</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B51">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C51">
-        <v>0.454</v>
+        <v>1.238</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B52">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C52">
-        <v>0.236</v>
+        <v>1.142</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B53">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C53">
-        <v>0.106</v>
+        <v>1.098</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B54">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C54">
-        <v>0.063</v>
+        <v>0.849</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B55">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C55">
-        <v>0.063</v>
+        <v>0.426</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B56">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C56">
-        <v>0.011</v>
+        <v>0.251</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B57">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C57">
-        <v>0.011</v>
+        <v>0.043</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45948</v>
+        <v>45957</v>
       </c>
       <c r="B58">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C58">
-        <v>0.011</v>
+        <v>0.048</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45949</v>
+        <v>45957</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45949</v>
+        <v>45957</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45949</v>
+        <v>45957</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45949</v>
+        <v>45957</v>
       </c>
       <c r="B62">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B63">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B64">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C64">
         <v>0.013</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B65">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C65">
         <v>0.013</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B66">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C66">
-        <v>0.08799999999999999</v>
+        <v>0.013</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B67">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C67">
-        <v>0.316</v>
+        <v>0.013</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B68">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C68">
-        <v>0.67</v>
+        <v>0.013</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B69">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C69">
-        <v>1.065</v>
+        <v>0.013</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B70">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C70">
-        <v>1.435</v>
+        <v>0.04</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B71">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C71">
-        <v>1.742</v>
+        <v>0.27</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B72">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C72">
-        <v>1.572</v>
+        <v>0.626</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B73">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C73">
-        <v>1.726</v>
+        <v>1.085</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B74">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C74">
-        <v>1.41</v>
+        <v>2.004</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B75">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C75">
-        <v>0.947</v>
+        <v>2.005</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B76">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C76">
-        <v>0.406</v>
+        <v>1.816</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B77">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C77">
-        <v>0.091</v>
+        <v>1.835</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B78">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C78">
-        <v>0.044</v>
+        <v>1.936</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B79">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C79">
-        <v>0.044</v>
+        <v>0.853</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B80">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C80">
-        <v>0.011</v>
+        <v>0.287</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B81">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C81">
-        <v>0.011</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45949</v>
+        <v>45958</v>
       </c>
       <c r="B82">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C82">
-        <v>0.011</v>
+        <v>0.044</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45950</v>
+        <v>45958</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45950</v>
+        <v>45958</v>
       </c>
       <c r="B84">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45950</v>
+        <v>45958</v>
       </c>
       <c r="B85">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45950</v>
+        <v>45958</v>
       </c>
       <c r="B86">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B87">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B88">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C88">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B89">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C89">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B90">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C90">
-        <v>0.111</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B91">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C91">
-        <v>0.497</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B92">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C92">
-        <v>1.878</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B93">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C93">
-        <v>2.306</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B94">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C94">
-        <v>2.902</v>
+        <v>0.036</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B95">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C95">
-        <v>3.31</v>
+        <v>0.313</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B96">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C96">
-        <v>3.289</v>
+        <v>1.025</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B97">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C97">
-        <v>3.04</v>
+        <v>1.849</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B98">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C98">
-        <v>2.069</v>
+        <v>2.289</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B99">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C99">
-        <v>1.724</v>
+        <v>2.841</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B100">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C100">
-        <v>0.483</v>
+        <v>2.73</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B101">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C101">
-        <v>0.1</v>
+        <v>2.261</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B102">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C102">
-        <v>0.055</v>
+        <v>1.843</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B103">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C103">
-        <v>0.044</v>
+        <v>0.862</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B104">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C104">
-        <v>0.011</v>
+        <v>0.291</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B105">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C105">
-        <v>0.011</v>
+        <v>0.068</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45950</v>
+        <v>45959</v>
       </c>
       <c r="B106">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C106">
-        <v>0.011</v>
+        <v>0.044</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45951</v>
+        <v>45959</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45951</v>
+        <v>45959</v>
       </c>
       <c r="B108">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45951</v>
+        <v>45959</v>
       </c>
       <c r="B109">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45951</v>
+        <v>45959</v>
       </c>
       <c r="B110">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B111">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,10 +2456,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B112">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B113">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B114">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C114">
-        <v>0.083</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B115">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C115">
-        <v>0.495</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B116">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C116">
-        <v>1.484</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B117">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C117">
-        <v>2.032</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B118">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C118">
-        <v>2.495</v>
+        <v>0.036</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B119">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C119">
-        <v>3.036</v>
+        <v>0.313</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B120">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C120">
-        <v>2.996</v>
+        <v>0.917</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B121">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C121">
-        <v>2.659</v>
+        <v>1.984</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B122">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C122">
-        <v>1.965</v>
+        <v>2.259</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B123">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C123">
-        <v>1.234</v>
+        <v>2.391</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B124">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C124">
-        <v>0.395</v>
+        <v>2.616</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B125">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C125">
-        <v>0.111</v>
+        <v>2.32</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B126">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C126">
-        <v>0.068</v>
+        <v>1.846</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B127">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C127">
-        <v>0.048</v>
+        <v>0.862</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B128">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C128">
-        <v>0.016</v>
+        <v>0.29</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B129">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C129">
-        <v>0.016</v>
+        <v>0.068</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45951</v>
+        <v>45960</v>
       </c>
       <c r="B130">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C130">
-        <v>0.016</v>
+        <v>0.073</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45952</v>
+        <v>45960</v>
       </c>
       <c r="B131">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C131">
-        <v>0.013</v>
+        <v>0.073</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45952</v>
+        <v>45960</v>
       </c>
       <c r="B132">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C132">
-        <v>0.013</v>
+        <v>0.02</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45952</v>
+        <v>45960</v>
       </c>
       <c r="B133">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C133">
-        <v>0.013</v>
+        <v>0.02</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45952</v>
+        <v>45960</v>
       </c>
       <c r="B134">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C134">
-        <v>0.013</v>
+        <v>0.02</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B135">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C135">
-        <v>0.013</v>
+        <v>0.018</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B136">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C136">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B137">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B138">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C138">
-        <v>0.083</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B139">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C139">
-        <v>0.265</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B140">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C140">
-        <v>0.733</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B141">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C141">
-        <v>1.255</v>
+        <v>0.013</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B142">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C142">
-        <v>1.796</v>
+        <v>0.04</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B143">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C143">
-        <v>2.059</v>
+        <v>0.318</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B144">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C144">
-        <v>1.973</v>
+        <v>0.952</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B145">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C145">
-        <v>1.855</v>
+        <v>2.05</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B146">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C146">
-        <v>1.51</v>
+        <v>2.239</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B147">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C147">
-        <v>0.9389999999999999</v>
+        <v>2.355</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B148">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C148">
-        <v>0.286</v>
+        <v>2.274</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B149">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C149">
-        <v>0.111</v>
+        <v>2.043</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B150">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C150">
-        <v>0.068</v>
+        <v>1.362</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B151">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C151">
-        <v>0.068</v>
+        <v>0.654</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B152">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C152">
-        <v>0.016</v>
+        <v>0.25</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B153">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C153">
-        <v>0.016</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45952</v>
+        <v>45961</v>
       </c>
       <c r="B154">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C154">
-        <v>0.016</v>
+        <v>0.077</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45953</v>
+        <v>45961</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C155">
-        <v>0.013</v>
+        <v>0.077</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45953</v>
+        <v>45961</v>
       </c>
       <c r="B156">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C156">
-        <v>0.013</v>
+        <v>0.025</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45953</v>
+        <v>45961</v>
       </c>
       <c r="B157">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45953</v>
+        <v>45961</v>
       </c>
       <c r="B158">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B159">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>0.022</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B160">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>0.022</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B161">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>0.022</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B162">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C162">
-        <v>0.08799999999999999</v>
+        <v>0.022</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B163">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C163">
-        <v>0.41</v>
+        <v>0.022</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B164">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C164">
-        <v>1.134</v>
+        <v>0.022</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B165">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C165">
-        <v>1.742</v>
+        <v>0.022</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B166">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C166">
-        <v>2.017</v>
+        <v>0.049</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B167">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C167">
-        <v>2.251</v>
+        <v>0.281</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B168">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C168">
-        <v>1.994</v>
+        <v>0.705</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B169">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C169">
-        <v>1.835</v>
+        <v>1.394</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45953</v>
+        <v>45962</v>
       </c>
       <c r="B170">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C170">
-        <v>1.792</v>
+        <v>1.725</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Retraining the 3D Steel, PCSUN and Ulmeni models with the latest available data
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>25.10.202512</t>
-  </si>
-  <si>
-    <t>25.10.202513</t>
-  </si>
-  <si>
-    <t>25.10.202514</t>
-  </si>
-  <si>
-    <t>25.10.202515</t>
-  </si>
-  <si>
-    <t>25.10.202516</t>
-  </si>
-  <si>
-    <t>25.10.202517</t>
-  </si>
-  <si>
-    <t>25.10.202518</t>
-  </si>
-  <si>
-    <t>25.10.202519</t>
-  </si>
-  <si>
-    <t>25.10.202520</t>
-  </si>
-  <si>
-    <t>25.10.202521</t>
-  </si>
-  <si>
-    <t>25.10.202522</t>
-  </si>
-  <si>
-    <t>25.10.202523</t>
-  </si>
-  <si>
-    <t>25.10.202524</t>
-  </si>
-  <si>
-    <t>26.10.20251</t>
-  </si>
-  <si>
-    <t>26.10.20252</t>
-  </si>
-  <si>
-    <t>26.10.20253</t>
-  </si>
-  <si>
-    <t>26.10.20254</t>
-  </si>
-  <si>
-    <t>26.10.20255</t>
-  </si>
-  <si>
-    <t>26.10.20256</t>
-  </si>
-  <si>
-    <t>26.10.20257</t>
-  </si>
-  <si>
-    <t>26.10.20258</t>
-  </si>
-  <si>
-    <t>26.10.20259</t>
-  </si>
-  <si>
-    <t>26.10.202510</t>
-  </si>
-  <si>
-    <t>26.10.202511</t>
-  </si>
-  <si>
-    <t>26.10.202512</t>
-  </si>
-  <si>
-    <t>26.10.202513</t>
-  </si>
-  <si>
-    <t>26.10.202514</t>
-  </si>
-  <si>
-    <t>26.10.202515</t>
-  </si>
-  <si>
-    <t>26.10.202516</t>
-  </si>
-  <si>
-    <t>26.10.202517</t>
-  </si>
-  <si>
-    <t>26.10.202518</t>
-  </si>
-  <si>
-    <t>26.10.202519</t>
-  </si>
-  <si>
-    <t>26.10.202520</t>
-  </si>
-  <si>
-    <t>26.10.202521</t>
-  </si>
-  <si>
-    <t>26.10.202522</t>
-  </si>
-  <si>
-    <t>26.10.202523</t>
-  </si>
-  <si>
-    <t>26.10.202524</t>
-  </si>
-  <si>
-    <t>27.10.20251</t>
-  </si>
-  <si>
-    <t>27.10.20252</t>
-  </si>
-  <si>
-    <t>27.10.20253</t>
-  </si>
-  <si>
-    <t>27.10.20254</t>
-  </si>
-  <si>
-    <t>27.10.20255</t>
-  </si>
-  <si>
-    <t>27.10.20256</t>
-  </si>
-  <si>
-    <t>27.10.20257</t>
-  </si>
-  <si>
-    <t>27.10.20258</t>
-  </si>
-  <si>
-    <t>27.10.20259</t>
-  </si>
-  <si>
-    <t>27.10.202510</t>
-  </si>
-  <si>
-    <t>27.10.202511</t>
-  </si>
-  <si>
-    <t>27.10.202512</t>
-  </si>
-  <si>
-    <t>27.10.202513</t>
-  </si>
-  <si>
-    <t>27.10.202514</t>
-  </si>
-  <si>
-    <t>27.10.202515</t>
-  </si>
-  <si>
-    <t>27.10.202516</t>
-  </si>
-  <si>
-    <t>27.10.202517</t>
-  </si>
-  <si>
-    <t>27.10.202518</t>
-  </si>
-  <si>
-    <t>27.10.202519</t>
-  </si>
-  <si>
-    <t>27.10.202520</t>
-  </si>
-  <si>
-    <t>27.10.202521</t>
-  </si>
-  <si>
-    <t>27.10.202522</t>
-  </si>
-  <si>
-    <t>27.10.202523</t>
-  </si>
-  <si>
-    <t>27.10.202524</t>
-  </si>
-  <si>
-    <t>28.10.20251</t>
-  </si>
-  <si>
-    <t>28.10.20252</t>
-  </si>
-  <si>
-    <t>28.10.20253</t>
-  </si>
-  <si>
-    <t>28.10.20254</t>
-  </si>
-  <si>
-    <t>28.10.20255</t>
-  </si>
-  <si>
-    <t>28.10.20256</t>
-  </si>
-  <si>
-    <t>28.10.20257</t>
-  </si>
-  <si>
-    <t>28.10.20258</t>
-  </si>
-  <si>
-    <t>28.10.20259</t>
-  </si>
-  <si>
-    <t>28.10.202510</t>
-  </si>
-  <si>
-    <t>28.10.202511</t>
-  </si>
-  <si>
-    <t>28.10.202512</t>
-  </si>
-  <si>
-    <t>28.10.202513</t>
-  </si>
-  <si>
-    <t>28.10.202514</t>
-  </si>
-  <si>
-    <t>28.10.202515</t>
-  </si>
-  <si>
-    <t>28.10.202516</t>
-  </si>
-  <si>
-    <t>28.10.202517</t>
-  </si>
-  <si>
-    <t>28.10.202518</t>
-  </si>
-  <si>
-    <t>28.10.202519</t>
-  </si>
-  <si>
-    <t>28.10.202520</t>
-  </si>
-  <si>
-    <t>28.10.202521</t>
-  </si>
-  <si>
-    <t>28.10.202522</t>
-  </si>
-  <si>
-    <t>28.10.202523</t>
-  </si>
-  <si>
-    <t>28.10.202524</t>
-  </si>
-  <si>
-    <t>29.10.20251</t>
-  </si>
-  <si>
-    <t>29.10.20252</t>
-  </si>
-  <si>
-    <t>29.10.20253</t>
-  </si>
-  <si>
-    <t>29.10.20254</t>
-  </si>
-  <si>
-    <t>29.10.20255</t>
-  </si>
-  <si>
-    <t>29.10.20256</t>
-  </si>
-  <si>
-    <t>29.10.20257</t>
-  </si>
-  <si>
-    <t>29.10.20258</t>
-  </si>
-  <si>
-    <t>29.10.20259</t>
-  </si>
-  <si>
-    <t>29.10.202510</t>
-  </si>
-  <si>
-    <t>29.10.202511</t>
-  </si>
-  <si>
-    <t>29.10.202512</t>
-  </si>
-  <si>
-    <t>29.10.202513</t>
-  </si>
-  <si>
-    <t>29.10.202514</t>
-  </si>
-  <si>
-    <t>29.10.202515</t>
-  </si>
-  <si>
-    <t>29.10.202516</t>
-  </si>
-  <si>
-    <t>29.10.202517</t>
-  </si>
-  <si>
-    <t>29.10.202518</t>
-  </si>
-  <si>
-    <t>29.10.202519</t>
-  </si>
-  <si>
-    <t>29.10.202520</t>
-  </si>
-  <si>
-    <t>29.10.202521</t>
-  </si>
-  <si>
-    <t>29.10.202522</t>
-  </si>
-  <si>
-    <t>29.10.202523</t>
-  </si>
-  <si>
-    <t>29.10.202524</t>
-  </si>
-  <si>
-    <t>30.10.20251</t>
-  </si>
-  <si>
-    <t>30.10.20252</t>
-  </si>
-  <si>
-    <t>30.10.20253</t>
-  </si>
-  <si>
-    <t>30.10.20254</t>
-  </si>
-  <si>
-    <t>30.10.20255</t>
-  </si>
-  <si>
-    <t>30.10.20256</t>
-  </si>
-  <si>
-    <t>30.10.20257</t>
-  </si>
-  <si>
-    <t>30.10.20258</t>
-  </si>
-  <si>
-    <t>30.10.20259</t>
-  </si>
-  <si>
-    <t>30.10.202510</t>
-  </si>
-  <si>
-    <t>30.10.202511</t>
-  </si>
-  <si>
-    <t>30.10.202512</t>
-  </si>
-  <si>
-    <t>30.10.202513</t>
-  </si>
-  <si>
-    <t>30.10.202514</t>
-  </si>
-  <si>
-    <t>30.10.202515</t>
-  </si>
-  <si>
-    <t>30.10.202516</t>
-  </si>
-  <si>
-    <t>30.10.202517</t>
-  </si>
-  <si>
-    <t>30.10.202518</t>
-  </si>
-  <si>
-    <t>30.10.202519</t>
-  </si>
-  <si>
-    <t>30.10.202520</t>
-  </si>
-  <si>
-    <t>30.10.202521</t>
-  </si>
-  <si>
-    <t>30.10.202522</t>
-  </si>
-  <si>
-    <t>30.10.202523</t>
-  </si>
-  <si>
-    <t>30.10.202524</t>
-  </si>
-  <si>
-    <t>31.10.20251</t>
-  </si>
-  <si>
-    <t>31.10.20252</t>
-  </si>
-  <si>
-    <t>31.10.20253</t>
-  </si>
-  <si>
-    <t>31.10.20254</t>
-  </si>
-  <si>
-    <t>31.10.20255</t>
-  </si>
-  <si>
-    <t>31.10.20256</t>
-  </si>
-  <si>
-    <t>31.10.20257</t>
-  </si>
-  <si>
-    <t>31.10.20258</t>
-  </si>
-  <si>
-    <t>31.10.20259</t>
-  </si>
-  <si>
-    <t>31.10.202510</t>
-  </si>
-  <si>
-    <t>31.10.202511</t>
-  </si>
-  <si>
-    <t>31.10.202512</t>
-  </si>
-  <si>
-    <t>31.10.202513</t>
-  </si>
-  <si>
-    <t>31.10.202514</t>
-  </si>
-  <si>
-    <t>31.10.202515</t>
-  </si>
-  <si>
-    <t>31.10.202516</t>
-  </si>
-  <si>
-    <t>31.10.202517</t>
-  </si>
-  <si>
-    <t>31.10.202518</t>
-  </si>
-  <si>
-    <t>31.10.202519</t>
-  </si>
-  <si>
-    <t>31.10.202520</t>
-  </si>
-  <si>
-    <t>31.10.202521</t>
-  </si>
-  <si>
-    <t>31.10.202522</t>
-  </si>
-  <si>
-    <t>31.10.202523</t>
-  </si>
-  <si>
-    <t>31.10.202524</t>
-  </si>
-  <si>
-    <t>01.11.20251</t>
-  </si>
-  <si>
-    <t>01.11.20252</t>
-  </si>
-  <si>
-    <t>01.11.20253</t>
-  </si>
-  <si>
-    <t>01.11.20254</t>
-  </si>
-  <si>
-    <t>01.11.20255</t>
-  </si>
-  <si>
-    <t>01.11.20256</t>
-  </si>
-  <si>
-    <t>01.11.20257</t>
-  </si>
-  <si>
-    <t>01.11.20258</t>
-  </si>
-  <si>
-    <t>01.11.20259</t>
-  </si>
-  <si>
-    <t>01.11.202510</t>
-  </si>
-  <si>
-    <t>01.11.202511</t>
-  </si>
-  <si>
-    <t>01.11.202512</t>
+    <t>08.11.202519</t>
+  </si>
+  <si>
+    <t>08.11.202520</t>
+  </si>
+  <si>
+    <t>08.11.202521</t>
+  </si>
+  <si>
+    <t>08.11.202522</t>
+  </si>
+  <si>
+    <t>08.11.202523</t>
+  </si>
+  <si>
+    <t>08.11.202524</t>
+  </si>
+  <si>
+    <t>09.11.20251</t>
+  </si>
+  <si>
+    <t>09.11.20252</t>
+  </si>
+  <si>
+    <t>09.11.20253</t>
+  </si>
+  <si>
+    <t>09.11.20254</t>
+  </si>
+  <si>
+    <t>09.11.20255</t>
+  </si>
+  <si>
+    <t>09.11.20256</t>
+  </si>
+  <si>
+    <t>09.11.20257</t>
+  </si>
+  <si>
+    <t>09.11.20258</t>
+  </si>
+  <si>
+    <t>09.11.20259</t>
+  </si>
+  <si>
+    <t>09.11.202510</t>
+  </si>
+  <si>
+    <t>09.11.202511</t>
+  </si>
+  <si>
+    <t>09.11.202512</t>
+  </si>
+  <si>
+    <t>09.11.202513</t>
+  </si>
+  <si>
+    <t>09.11.202514</t>
+  </si>
+  <si>
+    <t>09.11.202515</t>
+  </si>
+  <si>
+    <t>09.11.202516</t>
+  </si>
+  <si>
+    <t>09.11.202517</t>
+  </si>
+  <si>
+    <t>09.11.202518</t>
+  </si>
+  <si>
+    <t>09.11.202519</t>
+  </si>
+  <si>
+    <t>09.11.202520</t>
+  </si>
+  <si>
+    <t>09.11.202521</t>
+  </si>
+  <si>
+    <t>09.11.202522</t>
+  </si>
+  <si>
+    <t>09.11.202523</t>
+  </si>
+  <si>
+    <t>09.11.202524</t>
+  </si>
+  <si>
+    <t>10.11.20251</t>
+  </si>
+  <si>
+    <t>10.11.20252</t>
+  </si>
+  <si>
+    <t>10.11.20253</t>
+  </si>
+  <si>
+    <t>10.11.20254</t>
+  </si>
+  <si>
+    <t>10.11.20255</t>
+  </si>
+  <si>
+    <t>10.11.20256</t>
+  </si>
+  <si>
+    <t>10.11.20257</t>
+  </si>
+  <si>
+    <t>10.11.20258</t>
+  </si>
+  <si>
+    <t>10.11.20259</t>
+  </si>
+  <si>
+    <t>10.11.202510</t>
+  </si>
+  <si>
+    <t>10.11.202511</t>
+  </si>
+  <si>
+    <t>10.11.202512</t>
+  </si>
+  <si>
+    <t>10.11.202513</t>
+  </si>
+  <si>
+    <t>10.11.202514</t>
+  </si>
+  <si>
+    <t>10.11.202515</t>
+  </si>
+  <si>
+    <t>10.11.202516</t>
+  </si>
+  <si>
+    <t>10.11.202517</t>
+  </si>
+  <si>
+    <t>10.11.202518</t>
+  </si>
+  <si>
+    <t>10.11.202519</t>
+  </si>
+  <si>
+    <t>10.11.202520</t>
+  </si>
+  <si>
+    <t>10.11.202521</t>
+  </si>
+  <si>
+    <t>10.11.202522</t>
+  </si>
+  <si>
+    <t>10.11.202523</t>
+  </si>
+  <si>
+    <t>10.11.202524</t>
+  </si>
+  <si>
+    <t>11.11.20251</t>
+  </si>
+  <si>
+    <t>11.11.20252</t>
+  </si>
+  <si>
+    <t>11.11.20253</t>
+  </si>
+  <si>
+    <t>11.11.20254</t>
+  </si>
+  <si>
+    <t>11.11.20255</t>
+  </si>
+  <si>
+    <t>11.11.20256</t>
+  </si>
+  <si>
+    <t>11.11.20257</t>
+  </si>
+  <si>
+    <t>11.11.20258</t>
+  </si>
+  <si>
+    <t>11.11.20259</t>
+  </si>
+  <si>
+    <t>11.11.202510</t>
+  </si>
+  <si>
+    <t>11.11.202511</t>
+  </si>
+  <si>
+    <t>11.11.202512</t>
+  </si>
+  <si>
+    <t>11.11.202513</t>
+  </si>
+  <si>
+    <t>11.11.202514</t>
+  </si>
+  <si>
+    <t>11.11.202515</t>
+  </si>
+  <si>
+    <t>11.11.202516</t>
+  </si>
+  <si>
+    <t>11.11.202517</t>
+  </si>
+  <si>
+    <t>11.11.202518</t>
+  </si>
+  <si>
+    <t>11.11.202519</t>
+  </si>
+  <si>
+    <t>11.11.202520</t>
+  </si>
+  <si>
+    <t>11.11.202521</t>
+  </si>
+  <si>
+    <t>11.11.202522</t>
+  </si>
+  <si>
+    <t>11.11.202523</t>
+  </si>
+  <si>
+    <t>11.11.202524</t>
+  </si>
+  <si>
+    <t>12.11.20251</t>
+  </si>
+  <si>
+    <t>12.11.20252</t>
+  </si>
+  <si>
+    <t>12.11.20253</t>
+  </si>
+  <si>
+    <t>12.11.20254</t>
+  </si>
+  <si>
+    <t>12.11.20255</t>
+  </si>
+  <si>
+    <t>12.11.20256</t>
+  </si>
+  <si>
+    <t>12.11.20257</t>
+  </si>
+  <si>
+    <t>12.11.20258</t>
+  </si>
+  <si>
+    <t>12.11.20259</t>
+  </si>
+  <si>
+    <t>12.11.202510</t>
+  </si>
+  <si>
+    <t>12.11.202511</t>
+  </si>
+  <si>
+    <t>12.11.202512</t>
+  </si>
+  <si>
+    <t>12.11.202513</t>
+  </si>
+  <si>
+    <t>12.11.202514</t>
+  </si>
+  <si>
+    <t>12.11.202515</t>
+  </si>
+  <si>
+    <t>12.11.202516</t>
+  </si>
+  <si>
+    <t>12.11.202517</t>
+  </si>
+  <si>
+    <t>12.11.202518</t>
+  </si>
+  <si>
+    <t>12.11.202519</t>
+  </si>
+  <si>
+    <t>12.11.202520</t>
+  </si>
+  <si>
+    <t>12.11.202521</t>
+  </si>
+  <si>
+    <t>12.11.202522</t>
+  </si>
+  <si>
+    <t>12.11.202523</t>
+  </si>
+  <si>
+    <t>12.11.202524</t>
+  </si>
+  <si>
+    <t>13.11.20251</t>
+  </si>
+  <si>
+    <t>13.11.20252</t>
+  </si>
+  <si>
+    <t>13.11.20253</t>
+  </si>
+  <si>
+    <t>13.11.20254</t>
+  </si>
+  <si>
+    <t>13.11.20255</t>
+  </si>
+  <si>
+    <t>13.11.20256</t>
+  </si>
+  <si>
+    <t>13.11.20257</t>
+  </si>
+  <si>
+    <t>13.11.20258</t>
+  </si>
+  <si>
+    <t>13.11.20259</t>
+  </si>
+  <si>
+    <t>13.11.202510</t>
+  </si>
+  <si>
+    <t>13.11.202511</t>
+  </si>
+  <si>
+    <t>13.11.202512</t>
+  </si>
+  <si>
+    <t>13.11.202513</t>
+  </si>
+  <si>
+    <t>13.11.202514</t>
+  </si>
+  <si>
+    <t>13.11.202515</t>
+  </si>
+  <si>
+    <t>13.11.202516</t>
+  </si>
+  <si>
+    <t>13.11.202517</t>
+  </si>
+  <si>
+    <t>13.11.202518</t>
+  </si>
+  <si>
+    <t>13.11.202519</t>
+  </si>
+  <si>
+    <t>13.11.202520</t>
+  </si>
+  <si>
+    <t>13.11.202521</t>
+  </si>
+  <si>
+    <t>13.11.202522</t>
+  </si>
+  <si>
+    <t>13.11.202523</t>
+  </si>
+  <si>
+    <t>13.11.202524</t>
+  </si>
+  <si>
+    <t>14.11.20251</t>
+  </si>
+  <si>
+    <t>14.11.20252</t>
+  </si>
+  <si>
+    <t>14.11.20253</t>
+  </si>
+  <si>
+    <t>14.11.20254</t>
+  </si>
+  <si>
+    <t>14.11.20255</t>
+  </si>
+  <si>
+    <t>14.11.20256</t>
+  </si>
+  <si>
+    <t>14.11.20257</t>
+  </si>
+  <si>
+    <t>14.11.20258</t>
+  </si>
+  <si>
+    <t>14.11.20259</t>
+  </si>
+  <si>
+    <t>14.11.202510</t>
+  </si>
+  <si>
+    <t>14.11.202511</t>
+  </si>
+  <si>
+    <t>14.11.202512</t>
+  </si>
+  <si>
+    <t>14.11.202513</t>
+  </si>
+  <si>
+    <t>14.11.202514</t>
+  </si>
+  <si>
+    <t>14.11.202515</t>
+  </si>
+  <si>
+    <t>14.11.202516</t>
+  </si>
+  <si>
+    <t>14.11.202517</t>
+  </si>
+  <si>
+    <t>14.11.202518</t>
+  </si>
+  <si>
+    <t>14.11.202519</t>
+  </si>
+  <si>
+    <t>14.11.202520</t>
+  </si>
+  <si>
+    <t>14.11.202521</t>
+  </si>
+  <si>
+    <t>14.11.202522</t>
+  </si>
+  <si>
+    <t>14.11.202523</t>
+  </si>
+  <si>
+    <t>14.11.202524</t>
+  </si>
+  <si>
+    <t>15.11.20251</t>
+  </si>
+  <si>
+    <t>15.11.20252</t>
+  </si>
+  <si>
+    <t>15.11.20253</t>
+  </si>
+  <si>
+    <t>15.11.20254</t>
+  </si>
+  <si>
+    <t>15.11.20255</t>
+  </si>
+  <si>
+    <t>15.11.20256</t>
+  </si>
+  <si>
+    <t>15.11.20257</t>
+  </si>
+  <si>
+    <t>15.11.20258</t>
+  </si>
+  <si>
+    <t>15.11.20259</t>
+  </si>
+  <si>
+    <t>15.11.202510</t>
+  </si>
+  <si>
+    <t>15.11.202511</t>
+  </si>
+  <si>
+    <t>15.11.202512</t>
+  </si>
+  <si>
+    <t>15.11.202513</t>
+  </si>
+  <si>
+    <t>15.11.202514</t>
+  </si>
+  <si>
+    <t>15.11.202515</t>
+  </si>
+  <si>
+    <t>15.11.202516</t>
+  </si>
+  <si>
+    <t>15.11.202517</t>
+  </si>
+  <si>
+    <t>15.11.202518</t>
+  </si>
+  <si>
+    <t>15.11.202519</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45955</v>
+        <v>45969</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>0.034</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45955</v>
+        <v>45969</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>0.034</v>
+        <v>0.039</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45955</v>
+        <v>45969</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>3.069</v>
+        <v>0.091</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45955</v>
+        <v>45969</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C5">
-        <v>2.379</v>
+        <v>0.011</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45955</v>
+        <v>45969</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C6">
-        <v>2.02</v>
+        <v>0.011</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45955</v>
+        <v>45969</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C7">
-        <v>0.991</v>
+        <v>0.011</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45955</v>
+        <v>45970</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0.429</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45955</v>
+        <v>45970</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>0.116</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45955</v>
+        <v>45970</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>0.073</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45955</v>
+        <v>45970</v>
       </c>
       <c r="B11">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>0.073</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45955</v>
+        <v>45970</v>
       </c>
       <c r="B12">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45955</v>
+        <v>45970</v>
       </c>
       <c r="B13">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45955</v>
+        <v>45970</v>
       </c>
       <c r="B14">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>0.013</v>
+        <v>0.056</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>0.013</v>
+        <v>0.429</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>0.013</v>
+        <v>0.313</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>0.013</v>
+        <v>0.714</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C19">
-        <v>0.013</v>
+        <v>0.963</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C20">
-        <v>0.013</v>
+        <v>1.263</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>0.013</v>
+        <v>1.057</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <v>0.04</v>
+        <v>1.089</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C23">
-        <v>0.265</v>
+        <v>1.022</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C24">
-        <v>0.324</v>
+        <v>0.427</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B25">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C25">
-        <v>0.551</v>
+        <v>0.415</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C26">
-        <v>0.832</v>
+        <v>0.064</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B27">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C27">
-        <v>0.976</v>
+        <v>0.068</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B28">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C28">
-        <v>1.036</v>
+        <v>0.068</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B29">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C29">
-        <v>0.997</v>
+        <v>0.016</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C30">
-        <v>0.979</v>
+        <v>0.016</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="B31">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C31">
-        <v>0.577</v>
+        <v>0.016</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45956</v>
+        <v>45971</v>
       </c>
       <c r="B32">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <v>0.241</v>
+        <v>0.013</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45956</v>
+        <v>45971</v>
       </c>
       <c r="B33">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C33">
-        <v>0.111</v>
+        <v>0.013</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45956</v>
+        <v>45971</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C34">
-        <v>0.068</v>
+        <v>0.013</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45956</v>
+        <v>45971</v>
       </c>
       <c r="B35">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>0.063</v>
+        <v>0.013</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45956</v>
+        <v>45971</v>
       </c>
       <c r="B36">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C36">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45956</v>
+        <v>45971</v>
       </c>
       <c r="B37">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45956</v>
+        <v>45971</v>
       </c>
       <c r="B38">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C38">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>0.306</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>0.305</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>0.602</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.711</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B44">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1.04</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B45">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1.039</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B46">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C46">
-        <v>0.056</v>
+        <v>0.723</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B47">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C47">
-        <v>0.255</v>
+        <v>0.425</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B48">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C48">
-        <v>0.423</v>
+        <v>0.241</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B49">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C49">
-        <v>0.695</v>
+        <v>0.157</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B50">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C50">
-        <v>0.987</v>
+        <v>0.064</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B51">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C51">
-        <v>1.238</v>
+        <v>0.068</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B52">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C52">
-        <v>1.142</v>
+        <v>0.068</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B53">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C53">
-        <v>1.098</v>
+        <v>0.016</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B54">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C54">
-        <v>0.849</v>
+        <v>0.016</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="B55">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C55">
-        <v>0.426</v>
+        <v>0.016</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45957</v>
+        <v>45972</v>
       </c>
       <c r="B56">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>0.251</v>
+        <v>0.013</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45957</v>
+        <v>45972</v>
       </c>
       <c r="B57">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C57">
-        <v>0.043</v>
+        <v>0.013</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45957</v>
+        <v>45972</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C58">
-        <v>0.048</v>
+        <v>0.013</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45957</v>
+        <v>45972</v>
       </c>
       <c r="B59">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C59">
-        <v>0.048</v>
+        <v>0.013</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45957</v>
+        <v>45972</v>
       </c>
       <c r="B60">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C60">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45957</v>
+        <v>45972</v>
       </c>
       <c r="B61">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C61">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45957</v>
+        <v>45972</v>
       </c>
       <c r="B62">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C62">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C63">
-        <v>0.013</v>
+        <v>0.061</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C64">
-        <v>0.013</v>
+        <v>0.173</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C65">
-        <v>0.013</v>
+        <v>0.305</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C66">
-        <v>0.013</v>
+        <v>0.416</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B67">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C67">
-        <v>0.013</v>
+        <v>0.522</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B68">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C68">
-        <v>0.013</v>
+        <v>0.522</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C69">
-        <v>0.013</v>
+        <v>0.517</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B70">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C70">
-        <v>0.04</v>
+        <v>0.393</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B71">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C71">
-        <v>0.27</v>
+        <v>0.276</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C72">
-        <v>0.626</v>
+        <v>0.236</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B73">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C73">
-        <v>1.085</v>
+        <v>0.198</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B74">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C74">
-        <v>2.004</v>
+        <v>0.146</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B75">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C75">
-        <v>2.005</v>
+        <v>0.063</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C76">
-        <v>1.816</v>
+        <v>0.063</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B77">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C77">
-        <v>1.835</v>
+        <v>0.011</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B78">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C78">
-        <v>1.936</v>
+        <v>0.016</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C79">
-        <v>0.853</v>
+        <v>0.016</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45958</v>
+        <v>45973</v>
       </c>
       <c r="B80">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C80">
-        <v>0.287</v>
+        <v>0.013</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45958</v>
+        <v>45973</v>
       </c>
       <c r="B81">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C81">
-        <v>0.08599999999999999</v>
+        <v>0.013</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45958</v>
+        <v>45973</v>
       </c>
       <c r="B82">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C82">
-        <v>0.044</v>
+        <v>0.013</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45958</v>
+        <v>45973</v>
       </c>
       <c r="B83">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C83">
-        <v>0.044</v>
+        <v>0.013</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45958</v>
+        <v>45973</v>
       </c>
       <c r="B84">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C84">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45958</v>
+        <v>45973</v>
       </c>
       <c r="B85">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C85">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45958</v>
+        <v>45973</v>
       </c>
       <c r="B86">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C86">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>0.445</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>0.434</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B90">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>0.733</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B91">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>1.031</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B92">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>1.163</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B93">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>1.321</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B94">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C94">
-        <v>0.036</v>
+        <v>1.147</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B95">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C95">
-        <v>0.313</v>
+        <v>0.995</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B96">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C96">
-        <v>1.025</v>
+        <v>0.399</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B97">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C97">
-        <v>1.849</v>
+        <v>0.426</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B98">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C98">
-        <v>2.289</v>
+        <v>0.043</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B99">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C99">
-        <v>2.841</v>
+        <v>0.048</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B100">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C100">
-        <v>2.73</v>
+        <v>0.048</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B101">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C101">
-        <v>2.261</v>
+        <v>0.016</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B102">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C102">
-        <v>1.843</v>
+        <v>0.016</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="B103">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C103">
-        <v>0.862</v>
+        <v>0.016</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45959</v>
+        <v>45974</v>
       </c>
       <c r="B104">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C104">
-        <v>0.291</v>
+        <v>0.013</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45959</v>
+        <v>45974</v>
       </c>
       <c r="B105">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C105">
-        <v>0.068</v>
+        <v>0.013</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45959</v>
+        <v>45974</v>
       </c>
       <c r="B106">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C106">
-        <v>0.044</v>
+        <v>0</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45959</v>
+        <v>45974</v>
       </c>
       <c r="B107">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C107">
-        <v>0.044</v>
+        <v>0</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45959</v>
+        <v>45974</v>
       </c>
       <c r="B108">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C108">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45959</v>
+        <v>45974</v>
       </c>
       <c r="B109">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C109">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45959</v>
+        <v>45974</v>
       </c>
       <c r="B110">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C110">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B112">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>0.445</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B114">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>1.049</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B115">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>1.248</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B116">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>1.965</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B117">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>1.833</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B118">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C118">
-        <v>0.036</v>
+        <v>1.302</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B119">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C119">
-        <v>0.313</v>
+        <v>0.996</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B120">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C120">
-        <v>0.917</v>
+        <v>0.478</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B121">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C121">
-        <v>1.984</v>
+        <v>0.426</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B122">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C122">
-        <v>2.259</v>
+        <v>0.043</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B123">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C123">
-        <v>2.391</v>
+        <v>0.048</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B124">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C124">
-        <v>2.616</v>
+        <v>0.048</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B125">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C125">
-        <v>2.32</v>
+        <v>0.016</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B126">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C126">
-        <v>1.846</v>
+        <v>0.016</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="B127">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C127">
-        <v>0.862</v>
+        <v>0.016</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45960</v>
+        <v>45975</v>
       </c>
       <c r="B128">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C128">
-        <v>0.29</v>
+        <v>0.013</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45960</v>
+        <v>45975</v>
       </c>
       <c r="B129">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C129">
-        <v>0.068</v>
+        <v>0.013</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45960</v>
+        <v>45975</v>
       </c>
       <c r="B130">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C130">
-        <v>0.073</v>
+        <v>0</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45960</v>
+        <v>45975</v>
       </c>
       <c r="B131">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C131">
-        <v>0.073</v>
+        <v>0</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45960</v>
+        <v>45975</v>
       </c>
       <c r="B132">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C132">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45960</v>
+        <v>45975</v>
       </c>
       <c r="B133">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C133">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45960</v>
+        <v>45975</v>
       </c>
       <c r="B134">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C134">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C135">
-        <v>0.018</v>
+        <v>0.031</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B136">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>0.263</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B137">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B138">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>1.318</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B139">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>1.798</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B140">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>2.27</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B141">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C141">
-        <v>0.013</v>
+        <v>2.129</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B142">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C142">
-        <v>0.04</v>
+        <v>1.673</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B143">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C143">
-        <v>0.318</v>
+        <v>1.883</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B144">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C144">
-        <v>0.952</v>
+        <v>0.649</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B145">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C145">
-        <v>2.05</v>
+        <v>0.247</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B146">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C146">
-        <v>2.239</v>
+        <v>0.039</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B147">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C147">
-        <v>2.355</v>
+        <v>0.044</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B148">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C148">
-        <v>2.274</v>
+        <v>0.044</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B149">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C149">
-        <v>2.043</v>
+        <v>0.011</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B150">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C150">
-        <v>1.362</v>
+        <v>0.011</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="B151">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C151">
-        <v>0.654</v>
+        <v>0.011</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45961</v>
+        <v>45976</v>
       </c>
       <c r="B152">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C152">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45961</v>
+        <v>45976</v>
       </c>
       <c r="B153">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C153">
-        <v>0.07199999999999999</v>
+        <v>0</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45961</v>
+        <v>45976</v>
       </c>
       <c r="B154">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C154">
-        <v>0.077</v>
+        <v>0</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45961</v>
+        <v>45976</v>
       </c>
       <c r="B155">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C155">
-        <v>0.077</v>
+        <v>0</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45961</v>
+        <v>45976</v>
       </c>
       <c r="B156">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C156">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45961</v>
+        <v>45976</v>
       </c>
       <c r="B157">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C157">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45961</v>
+        <v>45976</v>
       </c>
       <c r="B158">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C158">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C159">
-        <v>0.022</v>
+        <v>0.031</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B160">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C160">
-        <v>0.022</v>
+        <v>0.263</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B161">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C161">
-        <v>0.022</v>
+        <v>0.722</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B162">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C162">
-        <v>0.022</v>
+        <v>1.534</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B163">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C163">
-        <v>0.022</v>
+        <v>1.818</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B164">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C164">
-        <v>0.022</v>
+        <v>2.381</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B165">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C165">
-        <v>0.022</v>
+        <v>2.161</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B166">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C166">
-        <v>0.049</v>
+        <v>1.673</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B167">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C167">
-        <v>0.281</v>
+        <v>1.883</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B168">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C168">
-        <v>0.705</v>
+        <v>0.607</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B169">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C169">
-        <v>1.394</v>
+        <v>0.247</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="B170">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C170">
-        <v>1.725</v>
+        <v>0.039</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Issue on PC Sun model and needs retraining
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,45 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>08.11.202519</t>
-  </si>
-  <si>
-    <t>08.11.202520</t>
-  </si>
-  <si>
-    <t>08.11.202521</t>
-  </si>
-  <si>
-    <t>08.11.202522</t>
-  </si>
-  <si>
-    <t>08.11.202523</t>
-  </si>
-  <si>
-    <t>08.11.202524</t>
-  </si>
-  <si>
-    <t>09.11.20251</t>
-  </si>
-  <si>
-    <t>09.11.20252</t>
-  </si>
-  <si>
-    <t>09.11.20253</t>
-  </si>
-  <si>
-    <t>09.11.20254</t>
-  </si>
-  <si>
-    <t>09.11.20255</t>
-  </si>
-  <si>
-    <t>09.11.20256</t>
-  </si>
-  <si>
-    <t>09.11.20257</t>
-  </si>
-  <si>
     <t>09.11.20258</t>
   </si>
   <si>
@@ -533,6 +494,45 @@
   </si>
   <si>
     <t>15.11.202519</t>
+  </si>
+  <si>
+    <t>15.11.202520</t>
+  </si>
+  <si>
+    <t>15.11.202521</t>
+  </si>
+  <si>
+    <t>15.11.202522</t>
+  </si>
+  <si>
+    <t>15.11.202523</t>
+  </si>
+  <si>
+    <t>15.11.202524</t>
+  </si>
+  <si>
+    <t>16.11.20251</t>
+  </si>
+  <si>
+    <t>16.11.20252</t>
+  </si>
+  <si>
+    <t>16.11.20253</t>
+  </si>
+  <si>
+    <t>16.11.20254</t>
+  </si>
+  <si>
+    <t>16.11.20255</t>
+  </si>
+  <si>
+    <t>16.11.20256</t>
+  </si>
+  <si>
+    <t>16.11.20257</t>
+  </si>
+  <si>
+    <t>16.11.20258</t>
   </si>
 </sst>
 </file>
@@ -916,13 +916,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45969</v>
+        <v>45970</v>
       </c>
       <c r="B2">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>0.034</v>
+        <v>0.031</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45969</v>
+        <v>45970</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>0.039</v>
+        <v>0.034</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45969</v>
+        <v>45970</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>0.091</v>
+        <v>0.313</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45969</v>
+        <v>45970</v>
       </c>
       <c r="B5">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>0.011</v>
+        <v>0.597</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45969</v>
+        <v>45970</v>
       </c>
       <c r="B6">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>0.011</v>
+        <v>0.877</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45969</v>
+        <v>45970</v>
       </c>
       <c r="B7">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>0.011</v>
+        <v>1.013</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1003,10 +1003,10 @@
         <v>45970</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1.021</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1017,10 +1017,10 @@
         <v>45970</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1031,10 +1031,10 @@
         <v>45970</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.732</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1045,10 +1045,10 @@
         <v>45970</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.427</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1059,10 +1059,10 @@
         <v>45970</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.415</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1073,10 +1073,10 @@
         <v>45970</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1087,10 +1087,10 @@
         <v>45970</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.068</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1101,10 +1101,10 @@
         <v>45970</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C15">
-        <v>0.056</v>
+        <v>0.068</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1115,10 +1115,10 @@
         <v>45970</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C16">
-        <v>0.429</v>
+        <v>0.016</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1129,10 +1129,10 @@
         <v>45970</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C17">
-        <v>0.313</v>
+        <v>0.016</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1143,10 +1143,10 @@
         <v>45970</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C18">
-        <v>0.714</v>
+        <v>0.011</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>0.963</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B20">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>1.263</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B21">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C21">
-        <v>1.057</v>
+        <v>0.013</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B22">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>1.089</v>
+        <v>0.013</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B23">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C23">
-        <v>1.022</v>
+        <v>0.013</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B24">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C24">
-        <v>0.427</v>
+        <v>0.013</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B25">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C25">
-        <v>0.415</v>
+        <v>0.013</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B26">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C26">
-        <v>0.064</v>
+        <v>0.04</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B27">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C27">
-        <v>0.068</v>
+        <v>0.306</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B28">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C28">
-        <v>0.068</v>
+        <v>0.305</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B29">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C29">
-        <v>0.016</v>
+        <v>0.416</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B30">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C30">
-        <v>0.016</v>
+        <v>0.398</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45970</v>
+        <v>45971</v>
       </c>
       <c r="B31">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C31">
-        <v>0.016</v>
+        <v>0.408</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1339,10 +1339,10 @@
         <v>45971</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C32">
-        <v>0.013</v>
+        <v>0.408</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1353,10 +1353,10 @@
         <v>45971</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C33">
-        <v>0.013</v>
+        <v>0.34</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1367,10 +1367,10 @@
         <v>45971</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C34">
-        <v>0.013</v>
+        <v>0.286</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1381,10 +1381,10 @@
         <v>45971</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C35">
-        <v>0.013</v>
+        <v>0.241</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1395,10 +1395,10 @@
         <v>45971</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C36">
-        <v>0.013</v>
+        <v>0.154</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1409,10 +1409,10 @@
         <v>45971</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C37">
-        <v>0.013</v>
+        <v>0.064</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1423,10 +1423,10 @@
         <v>45971</v>
       </c>
       <c r="B38">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C38">
-        <v>0.013</v>
+        <v>0.068</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1437,10 +1437,10 @@
         <v>45971</v>
       </c>
       <c r="B39">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C39">
-        <v>0.04</v>
+        <v>0.068</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1451,10 +1451,10 @@
         <v>45971</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C40">
-        <v>0.306</v>
+        <v>0.016</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1465,10 +1465,10 @@
         <v>45971</v>
       </c>
       <c r="B41">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C41">
-        <v>0.305</v>
+        <v>0.016</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1479,10 +1479,10 @@
         <v>45971</v>
       </c>
       <c r="B42">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C42">
-        <v>0.602</v>
+        <v>0.011</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B43">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>0.711</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B44">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>1.04</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B45">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C45">
-        <v>1.039</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B46">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C46">
-        <v>0.723</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B47">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C47">
-        <v>0.425</v>
+        <v>0.013</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B48">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C48">
-        <v>0.241</v>
+        <v>0.013</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B49">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C49">
-        <v>0.157</v>
+        <v>0.013</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B50">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C50">
-        <v>0.064</v>
+        <v>0.04</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B51">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C51">
-        <v>0.068</v>
+        <v>0.184</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B52">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C52">
-        <v>0.068</v>
+        <v>0.3</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B53">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C53">
-        <v>0.016</v>
+        <v>0.354</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B54">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C54">
-        <v>0.016</v>
+        <v>0.404</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B55">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C55">
-        <v>0.016</v>
+        <v>0.528</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1675,10 +1675,10 @@
         <v>45972</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C56">
-        <v>0.013</v>
+        <v>0.479</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1689,10 +1689,10 @@
         <v>45972</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C57">
-        <v>0.013</v>
+        <v>0.403</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1703,10 +1703,10 @@
         <v>45972</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C58">
-        <v>0.013</v>
+        <v>0.308</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1717,10 +1717,10 @@
         <v>45972</v>
       </c>
       <c r="B59">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C59">
-        <v>0.013</v>
+        <v>0.246</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1731,10 +1731,10 @@
         <v>45972</v>
       </c>
       <c r="B60">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C60">
-        <v>0.013</v>
+        <v>0.132</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1745,10 +1745,10 @@
         <v>45972</v>
       </c>
       <c r="B61">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C61">
-        <v>0.013</v>
+        <v>0.038</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1759,10 +1759,10 @@
         <v>45972</v>
       </c>
       <c r="B62">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C62">
-        <v>0.013</v>
+        <v>0.043</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1773,10 +1773,10 @@
         <v>45972</v>
       </c>
       <c r="B63">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C63">
-        <v>0.061</v>
+        <v>0.043</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1787,10 +1787,10 @@
         <v>45972</v>
       </c>
       <c r="B64">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C64">
-        <v>0.173</v>
+        <v>0.011</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1801,10 +1801,10 @@
         <v>45972</v>
       </c>
       <c r="B65">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C65">
-        <v>0.305</v>
+        <v>0.011</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1815,10 +1815,10 @@
         <v>45972</v>
       </c>
       <c r="B66">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C66">
-        <v>0.416</v>
+        <v>0.011</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B67">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C67">
-        <v>0.522</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B68">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C68">
-        <v>0.522</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B69">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C69">
-        <v>0.517</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B70">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C70">
-        <v>0.393</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B71">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C71">
-        <v>0.276</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B72">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C72">
-        <v>0.236</v>
+        <v>0</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B73">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C73">
-        <v>0.198</v>
+        <v>0</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B74">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C74">
-        <v>0.146</v>
+        <v>0.035</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B75">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C75">
-        <v>0.063</v>
+        <v>0.184</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B76">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C76">
-        <v>0.063</v>
+        <v>0.316</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B77">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C77">
-        <v>0.011</v>
+        <v>0.602</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B78">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C78">
-        <v>0.016</v>
+        <v>1.012</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="B79">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C79">
-        <v>0.016</v>
+        <v>0.997</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2011,10 +2011,10 @@
         <v>45973</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C80">
-        <v>0.013</v>
+        <v>1.136</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2025,10 +2025,10 @@
         <v>45973</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C81">
-        <v>0.013</v>
+        <v>1.137</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2039,10 +2039,10 @@
         <v>45973</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C82">
-        <v>0.013</v>
+        <v>0.974</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2053,10 +2053,10 @@
         <v>45973</v>
       </c>
       <c r="B83">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C83">
-        <v>0.013</v>
+        <v>0.498</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2067,10 +2067,10 @@
         <v>45973</v>
       </c>
       <c r="B84">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C84">
-        <v>0.013</v>
+        <v>0.415</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2081,10 +2081,10 @@
         <v>45973</v>
       </c>
       <c r="B85">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C85">
-        <v>0.013</v>
+        <v>0.064</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2095,10 +2095,10 @@
         <v>45973</v>
       </c>
       <c r="B86">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C86">
-        <v>0.013</v>
+        <v>0.044</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2109,10 +2109,10 @@
         <v>45973</v>
       </c>
       <c r="B87">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C87">
-        <v>0.04</v>
+        <v>0.039</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2123,10 +2123,10 @@
         <v>45973</v>
       </c>
       <c r="B88">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C88">
-        <v>0.445</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2137,10 +2137,10 @@
         <v>45973</v>
       </c>
       <c r="B89">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C89">
-        <v>0.434</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2151,10 +2151,10 @@
         <v>45973</v>
       </c>
       <c r="B90">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C90">
-        <v>0.733</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B91">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C91">
-        <v>1.031</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B92">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C92">
-        <v>1.163</v>
+        <v>0.013</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B93">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C93">
-        <v>1.321</v>
+        <v>0.013</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B94">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C94">
-        <v>1.147</v>
+        <v>0.013</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B95">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C95">
-        <v>0.995</v>
+        <v>0.013</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B96">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C96">
-        <v>0.399</v>
+        <v>0.013</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B97">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C97">
-        <v>0.426</v>
+        <v>0.013</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B98">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C98">
-        <v>0.043</v>
+        <v>0.04</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B99">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C99">
-        <v>0.048</v>
+        <v>0.447</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B100">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C100">
-        <v>0.048</v>
+        <v>0.518</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B101">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C101">
-        <v>0.016</v>
+        <v>1.029</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B102">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C102">
-        <v>0.016</v>
+        <v>1.606</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="B103">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C103">
-        <v>0.016</v>
+        <v>1.984</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2347,10 +2347,10 @@
         <v>45974</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C104">
-        <v>0.013</v>
+        <v>1.894</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2361,10 +2361,10 @@
         <v>45974</v>
       </c>
       <c r="B105">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C105">
-        <v>0.013</v>
+        <v>1.014</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2375,10 +2375,10 @@
         <v>45974</v>
       </c>
       <c r="B106">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>0.708</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2389,10 +2389,10 @@
         <v>45974</v>
       </c>
       <c r="B107">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.386</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2403,10 +2403,10 @@
         <v>45974</v>
       </c>
       <c r="B108">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C108">
-        <v>0.013</v>
+        <v>0.415</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2417,10 +2417,10 @@
         <v>45974</v>
       </c>
       <c r="B109">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C109">
-        <v>0.013</v>
+        <v>0.064</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2431,10 +2431,10 @@
         <v>45974</v>
       </c>
       <c r="B110">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C110">
-        <v>0.013</v>
+        <v>0.048</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2445,10 +2445,10 @@
         <v>45974</v>
       </c>
       <c r="B111">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C111">
-        <v>0.04</v>
+        <v>0.048</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2459,10 +2459,10 @@
         <v>45974</v>
       </c>
       <c r="B112">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C112">
-        <v>0.445</v>
+        <v>0.016</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2473,10 +2473,10 @@
         <v>45974</v>
       </c>
       <c r="B113">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C113">
-        <v>0.45</v>
+        <v>0.016</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2487,10 +2487,10 @@
         <v>45974</v>
       </c>
       <c r="B114">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C114">
-        <v>1.049</v>
+        <v>0.016</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B115">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C115">
-        <v>1.248</v>
+        <v>0.013</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B116">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C116">
-        <v>1.965</v>
+        <v>0.013</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B117">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C117">
-        <v>1.833</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B118">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C118">
-        <v>1.302</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B119">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C119">
-        <v>0.996</v>
+        <v>0</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B120">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C120">
-        <v>0.478</v>
+        <v>0</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B121">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C121">
-        <v>0.426</v>
+        <v>0</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B122">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C122">
-        <v>0.043</v>
+        <v>0.036</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B123">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C123">
-        <v>0.048</v>
+        <v>0.268</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B124">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C124">
-        <v>0.048</v>
+        <v>0.659</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B125">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C125">
-        <v>0.016</v>
+        <v>1.769</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B126">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C126">
-        <v>0.016</v>
+        <v>1.919</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B127">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C127">
-        <v>0.016</v>
+        <v>2.228</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2683,10 +2683,10 @@
         <v>45975</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C128">
-        <v>0.013</v>
+        <v>2.059</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2697,10 +2697,10 @@
         <v>45975</v>
       </c>
       <c r="B129">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C129">
-        <v>0.013</v>
+        <v>1.818</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2711,10 +2711,10 @@
         <v>45975</v>
       </c>
       <c r="B130">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>1.807</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2725,10 +2725,10 @@
         <v>45975</v>
       </c>
       <c r="B131">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>0.596</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2739,10 +2739,10 @@
         <v>45975</v>
       </c>
       <c r="B132">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>0.236</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2753,10 +2753,10 @@
         <v>45975</v>
       </c>
       <c r="B133">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>0.059</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2767,10 +2767,10 @@
         <v>45975</v>
       </c>
       <c r="B134">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2781,10 +2781,10 @@
         <v>45975</v>
       </c>
       <c r="B135">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C135">
-        <v>0.031</v>
+        <v>0.044</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2795,10 +2795,10 @@
         <v>45975</v>
       </c>
       <c r="B136">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C136">
-        <v>0.263</v>
+        <v>0.011</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2809,10 +2809,10 @@
         <v>45975</v>
       </c>
       <c r="B137">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C137">
-        <v>0.73</v>
+        <v>0.011</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2823,10 +2823,10 @@
         <v>45975</v>
       </c>
       <c r="B138">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C138">
-        <v>1.318</v>
+        <v>0.011</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B139">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C139">
-        <v>1.798</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B140">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C140">
-        <v>2.27</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B141">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C141">
-        <v>2.129</v>
+        <v>0</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B142">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C142">
-        <v>1.673</v>
+        <v>0</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B143">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C143">
-        <v>1.883</v>
+        <v>0</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B144">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C144">
-        <v>0.649</v>
+        <v>0</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B145">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C145">
-        <v>0.247</v>
+        <v>0</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B146">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C146">
-        <v>0.039</v>
+        <v>0.036</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B147">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C147">
-        <v>0.044</v>
+        <v>0.268</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B148">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C148">
-        <v>0.044</v>
+        <v>0.659</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B149">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C149">
-        <v>0.011</v>
+        <v>1.843</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B150">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C150">
-        <v>0.011</v>
+        <v>1.847</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="B151">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C151">
-        <v>0.011</v>
+        <v>2.22</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3019,10 +3019,10 @@
         <v>45976</v>
       </c>
       <c r="B152">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C152">
-        <v>0</v>
+        <v>2.088</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3033,10 +3033,10 @@
         <v>45976</v>
       </c>
       <c r="B153">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>1.827</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3047,10 +3047,10 @@
         <v>45976</v>
       </c>
       <c r="B154">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>1.883</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3061,10 +3061,10 @@
         <v>45976</v>
       </c>
       <c r="B155">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>0.596</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3075,10 +3075,10 @@
         <v>45976</v>
       </c>
       <c r="B156">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>0.236</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3089,10 +3089,10 @@
         <v>45976</v>
       </c>
       <c r="B157">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>0.059</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3103,10 +3103,10 @@
         <v>45976</v>
       </c>
       <c r="B158">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3117,10 +3117,10 @@
         <v>45976</v>
       </c>
       <c r="B159">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C159">
-        <v>0.031</v>
+        <v>0.044</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3131,10 +3131,10 @@
         <v>45976</v>
       </c>
       <c r="B160">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C160">
-        <v>0.263</v>
+        <v>0.011</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3145,10 +3145,10 @@
         <v>45976</v>
       </c>
       <c r="B161">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C161">
-        <v>0.722</v>
+        <v>0.011</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3159,10 +3159,10 @@
         <v>45976</v>
       </c>
       <c r="B162">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C162">
-        <v>1.534</v>
+        <v>0.011</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B163">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C163">
-        <v>1.818</v>
+        <v>0</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B164">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C164">
-        <v>2.381</v>
+        <v>0</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B165">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C165">
-        <v>2.161</v>
+        <v>0</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B166">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C166">
-        <v>1.673</v>
+        <v>0</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B167">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C167">
-        <v>1.883</v>
+        <v>0</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B168">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C168">
-        <v>0.607</v>
+        <v>0</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B169">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C169">
-        <v>0.247</v>
+        <v>0</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45976</v>
+        <v>45977</v>
       </c>
       <c r="B170">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C170">
-        <v>0.039</v>
+        <v>0.036</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Retraining models with the latest data
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,396 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>09.11.20258</t>
-  </si>
-  <si>
-    <t>09.11.20259</t>
-  </si>
-  <si>
-    <t>09.11.202510</t>
-  </si>
-  <si>
-    <t>09.11.202511</t>
-  </si>
-  <si>
-    <t>09.11.202512</t>
-  </si>
-  <si>
-    <t>09.11.202513</t>
-  </si>
-  <si>
-    <t>09.11.202514</t>
-  </si>
-  <si>
-    <t>09.11.202515</t>
-  </si>
-  <si>
-    <t>09.11.202516</t>
-  </si>
-  <si>
-    <t>09.11.202517</t>
-  </si>
-  <si>
-    <t>09.11.202518</t>
-  </si>
-  <si>
-    <t>09.11.202519</t>
-  </si>
-  <si>
-    <t>09.11.202520</t>
-  </si>
-  <si>
-    <t>09.11.202521</t>
-  </si>
-  <si>
-    <t>09.11.202522</t>
-  </si>
-  <si>
-    <t>09.11.202523</t>
-  </si>
-  <si>
-    <t>09.11.202524</t>
-  </si>
-  <si>
-    <t>10.11.20251</t>
-  </si>
-  <si>
-    <t>10.11.20252</t>
-  </si>
-  <si>
-    <t>10.11.20253</t>
-  </si>
-  <si>
-    <t>10.11.20254</t>
-  </si>
-  <si>
-    <t>10.11.20255</t>
-  </si>
-  <si>
-    <t>10.11.20256</t>
-  </si>
-  <si>
-    <t>10.11.20257</t>
-  </si>
-  <si>
-    <t>10.11.20258</t>
-  </si>
-  <si>
-    <t>10.11.20259</t>
-  </si>
-  <si>
-    <t>10.11.202510</t>
-  </si>
-  <si>
-    <t>10.11.202511</t>
-  </si>
-  <si>
-    <t>10.11.202512</t>
-  </si>
-  <si>
-    <t>10.11.202513</t>
-  </si>
-  <si>
-    <t>10.11.202514</t>
-  </si>
-  <si>
-    <t>10.11.202515</t>
-  </si>
-  <si>
-    <t>10.11.202516</t>
-  </si>
-  <si>
-    <t>10.11.202517</t>
-  </si>
-  <si>
-    <t>10.11.202518</t>
-  </si>
-  <si>
-    <t>10.11.202519</t>
-  </si>
-  <si>
-    <t>10.11.202520</t>
-  </si>
-  <si>
-    <t>10.11.202521</t>
-  </si>
-  <si>
-    <t>10.11.202522</t>
-  </si>
-  <si>
-    <t>10.11.202523</t>
-  </si>
-  <si>
-    <t>10.11.202524</t>
-  </si>
-  <si>
-    <t>11.11.20251</t>
-  </si>
-  <si>
-    <t>11.11.20252</t>
-  </si>
-  <si>
-    <t>11.11.20253</t>
-  </si>
-  <si>
-    <t>11.11.20254</t>
-  </si>
-  <si>
-    <t>11.11.20255</t>
-  </si>
-  <si>
-    <t>11.11.20256</t>
-  </si>
-  <si>
-    <t>11.11.20257</t>
-  </si>
-  <si>
-    <t>11.11.20258</t>
-  </si>
-  <si>
-    <t>11.11.20259</t>
-  </si>
-  <si>
-    <t>11.11.202510</t>
-  </si>
-  <si>
-    <t>11.11.202511</t>
-  </si>
-  <si>
-    <t>11.11.202512</t>
-  </si>
-  <si>
-    <t>11.11.202513</t>
-  </si>
-  <si>
-    <t>11.11.202514</t>
-  </si>
-  <si>
-    <t>11.11.202515</t>
-  </si>
-  <si>
-    <t>11.11.202516</t>
-  </si>
-  <si>
-    <t>11.11.202517</t>
-  </si>
-  <si>
-    <t>11.11.202518</t>
-  </si>
-  <si>
-    <t>11.11.202519</t>
-  </si>
-  <si>
-    <t>11.11.202520</t>
-  </si>
-  <si>
-    <t>11.11.202521</t>
-  </si>
-  <si>
-    <t>11.11.202522</t>
-  </si>
-  <si>
-    <t>11.11.202523</t>
-  </si>
-  <si>
-    <t>11.11.202524</t>
-  </si>
-  <si>
-    <t>12.11.20251</t>
-  </si>
-  <si>
-    <t>12.11.20252</t>
-  </si>
-  <si>
-    <t>12.11.20253</t>
-  </si>
-  <si>
-    <t>12.11.20254</t>
-  </si>
-  <si>
-    <t>12.11.20255</t>
-  </si>
-  <si>
-    <t>12.11.20256</t>
-  </si>
-  <si>
-    <t>12.11.20257</t>
-  </si>
-  <si>
-    <t>12.11.20258</t>
-  </si>
-  <si>
-    <t>12.11.20259</t>
-  </si>
-  <si>
-    <t>12.11.202510</t>
-  </si>
-  <si>
-    <t>12.11.202511</t>
-  </si>
-  <si>
-    <t>12.11.202512</t>
-  </si>
-  <si>
-    <t>12.11.202513</t>
-  </si>
-  <si>
-    <t>12.11.202514</t>
-  </si>
-  <si>
-    <t>12.11.202515</t>
-  </si>
-  <si>
-    <t>12.11.202516</t>
-  </si>
-  <si>
-    <t>12.11.202517</t>
-  </si>
-  <si>
-    <t>12.11.202518</t>
-  </si>
-  <si>
-    <t>12.11.202519</t>
-  </si>
-  <si>
-    <t>12.11.202520</t>
-  </si>
-  <si>
-    <t>12.11.202521</t>
-  </si>
-  <si>
-    <t>12.11.202522</t>
-  </si>
-  <si>
-    <t>12.11.202523</t>
-  </si>
-  <si>
-    <t>12.11.202524</t>
-  </si>
-  <si>
-    <t>13.11.20251</t>
-  </si>
-  <si>
-    <t>13.11.20252</t>
-  </si>
-  <si>
-    <t>13.11.20253</t>
-  </si>
-  <si>
-    <t>13.11.20254</t>
-  </si>
-  <si>
-    <t>13.11.20255</t>
-  </si>
-  <si>
-    <t>13.11.20256</t>
-  </si>
-  <si>
-    <t>13.11.20257</t>
-  </si>
-  <si>
-    <t>13.11.20258</t>
-  </si>
-  <si>
-    <t>13.11.20259</t>
-  </si>
-  <si>
-    <t>13.11.202510</t>
-  </si>
-  <si>
-    <t>13.11.202511</t>
-  </si>
-  <si>
-    <t>13.11.202512</t>
-  </si>
-  <si>
-    <t>13.11.202513</t>
-  </si>
-  <si>
-    <t>13.11.202514</t>
-  </si>
-  <si>
-    <t>13.11.202515</t>
-  </si>
-  <si>
-    <t>13.11.202516</t>
-  </si>
-  <si>
-    <t>13.11.202517</t>
-  </si>
-  <si>
-    <t>13.11.202518</t>
-  </si>
-  <si>
-    <t>13.11.202519</t>
-  </si>
-  <si>
-    <t>13.11.202520</t>
-  </si>
-  <si>
-    <t>13.11.202521</t>
-  </si>
-  <si>
-    <t>13.11.202522</t>
-  </si>
-  <si>
-    <t>13.11.202523</t>
-  </si>
-  <si>
-    <t>13.11.202524</t>
-  </si>
-  <si>
-    <t>14.11.20251</t>
-  </si>
-  <si>
-    <t>14.11.20252</t>
-  </si>
-  <si>
-    <t>14.11.20253</t>
-  </si>
-  <si>
-    <t>14.11.20254</t>
-  </si>
-  <si>
-    <t>14.11.20255</t>
-  </si>
-  <si>
-    <t>14.11.20256</t>
-  </si>
-  <si>
-    <t>14.11.20257</t>
-  </si>
-  <si>
-    <t>14.11.20258</t>
-  </si>
-  <si>
-    <t>14.11.20259</t>
-  </si>
-  <si>
-    <t>14.11.202510</t>
-  </si>
-  <si>
-    <t>14.11.202511</t>
-  </si>
-  <si>
-    <t>14.11.202512</t>
-  </si>
-  <si>
-    <t>14.11.202513</t>
-  </si>
-  <si>
-    <t>14.11.202514</t>
-  </si>
-  <si>
-    <t>14.11.202515</t>
-  </si>
-  <si>
-    <t>14.11.202516</t>
-  </si>
-  <si>
-    <t>14.11.202517</t>
-  </si>
-  <si>
     <t>14.11.202518</t>
   </si>
   <si>
@@ -533,6 +143,396 @@
   </si>
   <si>
     <t>16.11.20258</t>
+  </si>
+  <si>
+    <t>16.11.20259</t>
+  </si>
+  <si>
+    <t>16.11.202510</t>
+  </si>
+  <si>
+    <t>16.11.202511</t>
+  </si>
+  <si>
+    <t>16.11.202512</t>
+  </si>
+  <si>
+    <t>16.11.202513</t>
+  </si>
+  <si>
+    <t>16.11.202514</t>
+  </si>
+  <si>
+    <t>16.11.202515</t>
+  </si>
+  <si>
+    <t>16.11.202516</t>
+  </si>
+  <si>
+    <t>16.11.202517</t>
+  </si>
+  <si>
+    <t>16.11.202518</t>
+  </si>
+  <si>
+    <t>16.11.202519</t>
+  </si>
+  <si>
+    <t>16.11.202520</t>
+  </si>
+  <si>
+    <t>16.11.202521</t>
+  </si>
+  <si>
+    <t>16.11.202522</t>
+  </si>
+  <si>
+    <t>16.11.202523</t>
+  </si>
+  <si>
+    <t>16.11.202524</t>
+  </si>
+  <si>
+    <t>17.11.20251</t>
+  </si>
+  <si>
+    <t>17.11.20252</t>
+  </si>
+  <si>
+    <t>17.11.20253</t>
+  </si>
+  <si>
+    <t>17.11.20254</t>
+  </si>
+  <si>
+    <t>17.11.20255</t>
+  </si>
+  <si>
+    <t>17.11.20256</t>
+  </si>
+  <si>
+    <t>17.11.20257</t>
+  </si>
+  <si>
+    <t>17.11.20258</t>
+  </si>
+  <si>
+    <t>17.11.20259</t>
+  </si>
+  <si>
+    <t>17.11.202510</t>
+  </si>
+  <si>
+    <t>17.11.202511</t>
+  </si>
+  <si>
+    <t>17.11.202512</t>
+  </si>
+  <si>
+    <t>17.11.202513</t>
+  </si>
+  <si>
+    <t>17.11.202514</t>
+  </si>
+  <si>
+    <t>17.11.202515</t>
+  </si>
+  <si>
+    <t>17.11.202516</t>
+  </si>
+  <si>
+    <t>17.11.202517</t>
+  </si>
+  <si>
+    <t>17.11.202518</t>
+  </si>
+  <si>
+    <t>17.11.202519</t>
+  </si>
+  <si>
+    <t>17.11.202520</t>
+  </si>
+  <si>
+    <t>17.11.202521</t>
+  </si>
+  <si>
+    <t>17.11.202522</t>
+  </si>
+  <si>
+    <t>17.11.202523</t>
+  </si>
+  <si>
+    <t>17.11.202524</t>
+  </si>
+  <si>
+    <t>18.11.20251</t>
+  </si>
+  <si>
+    <t>18.11.20252</t>
+  </si>
+  <si>
+    <t>18.11.20253</t>
+  </si>
+  <si>
+    <t>18.11.20254</t>
+  </si>
+  <si>
+    <t>18.11.20255</t>
+  </si>
+  <si>
+    <t>18.11.20256</t>
+  </si>
+  <si>
+    <t>18.11.20257</t>
+  </si>
+  <si>
+    <t>18.11.20258</t>
+  </si>
+  <si>
+    <t>18.11.20259</t>
+  </si>
+  <si>
+    <t>18.11.202510</t>
+  </si>
+  <si>
+    <t>18.11.202511</t>
+  </si>
+  <si>
+    <t>18.11.202512</t>
+  </si>
+  <si>
+    <t>18.11.202513</t>
+  </si>
+  <si>
+    <t>18.11.202514</t>
+  </si>
+  <si>
+    <t>18.11.202515</t>
+  </si>
+  <si>
+    <t>18.11.202516</t>
+  </si>
+  <si>
+    <t>18.11.202517</t>
+  </si>
+  <si>
+    <t>18.11.202518</t>
+  </si>
+  <si>
+    <t>18.11.202519</t>
+  </si>
+  <si>
+    <t>18.11.202520</t>
+  </si>
+  <si>
+    <t>18.11.202521</t>
+  </si>
+  <si>
+    <t>18.11.202522</t>
+  </si>
+  <si>
+    <t>18.11.202523</t>
+  </si>
+  <si>
+    <t>18.11.202524</t>
+  </si>
+  <si>
+    <t>19.11.20251</t>
+  </si>
+  <si>
+    <t>19.11.20252</t>
+  </si>
+  <si>
+    <t>19.11.20253</t>
+  </si>
+  <si>
+    <t>19.11.20254</t>
+  </si>
+  <si>
+    <t>19.11.20255</t>
+  </si>
+  <si>
+    <t>19.11.20256</t>
+  </si>
+  <si>
+    <t>19.11.20257</t>
+  </si>
+  <si>
+    <t>19.11.20258</t>
+  </si>
+  <si>
+    <t>19.11.20259</t>
+  </si>
+  <si>
+    <t>19.11.202510</t>
+  </si>
+  <si>
+    <t>19.11.202511</t>
+  </si>
+  <si>
+    <t>19.11.202512</t>
+  </si>
+  <si>
+    <t>19.11.202513</t>
+  </si>
+  <si>
+    <t>19.11.202514</t>
+  </si>
+  <si>
+    <t>19.11.202515</t>
+  </si>
+  <si>
+    <t>19.11.202516</t>
+  </si>
+  <si>
+    <t>19.11.202517</t>
+  </si>
+  <si>
+    <t>19.11.202518</t>
+  </si>
+  <si>
+    <t>19.11.202519</t>
+  </si>
+  <si>
+    <t>19.11.202520</t>
+  </si>
+  <si>
+    <t>19.11.202521</t>
+  </si>
+  <si>
+    <t>19.11.202522</t>
+  </si>
+  <si>
+    <t>19.11.202523</t>
+  </si>
+  <si>
+    <t>19.11.202524</t>
+  </si>
+  <si>
+    <t>20.11.20251</t>
+  </si>
+  <si>
+    <t>20.11.20252</t>
+  </si>
+  <si>
+    <t>20.11.20253</t>
+  </si>
+  <si>
+    <t>20.11.20254</t>
+  </si>
+  <si>
+    <t>20.11.20255</t>
+  </si>
+  <si>
+    <t>20.11.20256</t>
+  </si>
+  <si>
+    <t>20.11.20257</t>
+  </si>
+  <si>
+    <t>20.11.20258</t>
+  </si>
+  <si>
+    <t>20.11.20259</t>
+  </si>
+  <si>
+    <t>20.11.202510</t>
+  </si>
+  <si>
+    <t>20.11.202511</t>
+  </si>
+  <si>
+    <t>20.11.202512</t>
+  </si>
+  <si>
+    <t>20.11.202513</t>
+  </si>
+  <si>
+    <t>20.11.202514</t>
+  </si>
+  <si>
+    <t>20.11.202515</t>
+  </si>
+  <si>
+    <t>20.11.202516</t>
+  </si>
+  <si>
+    <t>20.11.202517</t>
+  </si>
+  <si>
+    <t>20.11.202518</t>
+  </si>
+  <si>
+    <t>20.11.202519</t>
+  </si>
+  <si>
+    <t>20.11.202520</t>
+  </si>
+  <si>
+    <t>20.11.202521</t>
+  </si>
+  <si>
+    <t>20.11.202522</t>
+  </si>
+  <si>
+    <t>20.11.202523</t>
+  </si>
+  <si>
+    <t>20.11.202524</t>
+  </si>
+  <si>
+    <t>21.11.20251</t>
+  </si>
+  <si>
+    <t>21.11.20252</t>
+  </si>
+  <si>
+    <t>21.11.20253</t>
+  </si>
+  <si>
+    <t>21.11.20254</t>
+  </si>
+  <si>
+    <t>21.11.20255</t>
+  </si>
+  <si>
+    <t>21.11.20256</t>
+  </si>
+  <si>
+    <t>21.11.20257</t>
+  </si>
+  <si>
+    <t>21.11.20258</t>
+  </si>
+  <si>
+    <t>21.11.20259</t>
+  </si>
+  <si>
+    <t>21.11.202510</t>
+  </si>
+  <si>
+    <t>21.11.202511</t>
+  </si>
+  <si>
+    <t>21.11.202512</t>
+  </si>
+  <si>
+    <t>21.11.202513</t>
+  </si>
+  <si>
+    <t>21.11.202514</t>
+  </si>
+  <si>
+    <t>21.11.202515</t>
+  </si>
+  <si>
+    <t>21.11.202516</t>
+  </si>
+  <si>
+    <t>21.11.202517</t>
+  </si>
+  <si>
+    <t>21.11.202518</t>
   </si>
 </sst>
 </file>
@@ -916,13 +916,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45970</v>
+        <v>45975</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C2">
-        <v>0.031</v>
+        <v>0.034</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45970</v>
+        <v>45975</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>0.034</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45970</v>
+        <v>45975</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>0.313</v>
+        <v>0.044</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45970</v>
+        <v>45975</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C5">
-        <v>0.597</v>
+        <v>0.044</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45970</v>
+        <v>45975</v>
       </c>
       <c r="B6">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C6">
-        <v>0.877</v>
+        <v>0.016</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45970</v>
+        <v>45975</v>
       </c>
       <c r="B7">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>1.013</v>
+        <v>0.016</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45970</v>
+        <v>45975</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C8">
-        <v>1.021</v>
+        <v>0.016</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.925</v>
+        <v>0.013</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>0.732</v>
+        <v>0.013</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B11">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>0.427</v>
+        <v>0.013</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B12">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>0.415</v>
+        <v>0.013</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B13">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>0.064</v>
+        <v>0.013</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B14">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>0.068</v>
+        <v>0.013</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B15">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C15">
-        <v>0.068</v>
+        <v>0.013</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B16">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C16">
-        <v>0.016</v>
+        <v>0.04</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B17">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>0.016</v>
+        <v>0.184</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45970</v>
+        <v>45976</v>
       </c>
       <c r="B18">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C18">
-        <v>0.011</v>
+        <v>0.316</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.613</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>0.912</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C21">
-        <v>0.013</v>
+        <v>1.098</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C22">
-        <v>0.013</v>
+        <v>1.278</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C23">
-        <v>0.013</v>
+        <v>1.092</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C24">
-        <v>0.013</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C25">
-        <v>0.013</v>
+        <v>0.526</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B26">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C26">
-        <v>0.04</v>
+        <v>0.415</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C27">
-        <v>0.306</v>
+        <v>0.059</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C28">
-        <v>0.305</v>
+        <v>0.044</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B29">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C29">
-        <v>0.416</v>
+        <v>0.044</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B30">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C30">
-        <v>0.398</v>
+        <v>0.011</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B31">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C31">
-        <v>0.408</v>
+        <v>0.011</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45971</v>
+        <v>45976</v>
       </c>
       <c r="B32">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C32">
-        <v>0.408</v>
+        <v>0.011</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45971</v>
+        <v>45977</v>
       </c>
       <c r="B33">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>0.34</v>
+        <v>0.013</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45971</v>
+        <v>45977</v>
       </c>
       <c r="B34">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>0.286</v>
+        <v>0.013</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45971</v>
+        <v>45977</v>
       </c>
       <c r="B35">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>0.241</v>
+        <v>0.013</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45971</v>
+        <v>45977</v>
       </c>
       <c r="B36">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C36">
-        <v>0.154</v>
+        <v>0.013</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45971</v>
+        <v>45977</v>
       </c>
       <c r="B37">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C37">
-        <v>0.064</v>
+        <v>0.013</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45971</v>
+        <v>45977</v>
       </c>
       <c r="B38">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C38">
-        <v>0.068</v>
+        <v>0.013</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45971</v>
+        <v>45977</v>
       </c>
       <c r="B39">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C39">
-        <v>0.068</v>
+        <v>0.013</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45971</v>
+        <v>45977</v>
       </c>
       <c r="B40">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C40">
-        <v>0.016</v>
+        <v>0.04</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45971</v>
+        <v>45977</v>
       </c>
       <c r="B41">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C41">
-        <v>0.016</v>
+        <v>0.306</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45971</v>
+        <v>45977</v>
       </c>
       <c r="B42">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C42">
-        <v>0.011</v>
+        <v>0.329</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.878</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1.102</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1.52</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1.334</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B47">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C47">
-        <v>0.013</v>
+        <v>0.999</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B48">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C48">
-        <v>0.013</v>
+        <v>0.963</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B49">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C49">
-        <v>0.013</v>
+        <v>0.476</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B50">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C50">
-        <v>0.04</v>
+        <v>0.415</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B51">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C51">
-        <v>0.184</v>
+        <v>0.064</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B52">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C52">
-        <v>0.3</v>
+        <v>0.048</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B53">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C53">
-        <v>0.354</v>
+        <v>0.048</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B54">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C54">
-        <v>0.404</v>
+        <v>0.016</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B55">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C55">
-        <v>0.528</v>
+        <v>0.016</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45972</v>
+        <v>45977</v>
       </c>
       <c r="B56">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C56">
-        <v>0.479</v>
+        <v>0.016</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B57">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C57">
-        <v>0.403</v>
+        <v>0.013</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B58">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C58">
-        <v>0.308</v>
+        <v>0.013</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B59">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C59">
-        <v>0.246</v>
+        <v>0.013</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B60">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C60">
-        <v>0.132</v>
+        <v>0.013</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B61">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C61">
-        <v>0.038</v>
+        <v>0.013</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B62">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C62">
-        <v>0.043</v>
+        <v>0.013</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B63">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C63">
-        <v>0.043</v>
+        <v>0.013</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B64">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C64">
-        <v>0.011</v>
+        <v>0.04</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B65">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C65">
-        <v>0.011</v>
+        <v>0.447</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45972</v>
+        <v>45978</v>
       </c>
       <c r="B66">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C66">
-        <v>0.011</v>
+        <v>0.549</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1.026</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>1.524</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1.839</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B70">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1.826</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B71">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1.438</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B72">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>0.972</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B73">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>0.531</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B74">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C74">
-        <v>0.035</v>
+        <v>0.424</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B75">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C75">
-        <v>0.184</v>
+        <v>0.064</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B76">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C76">
-        <v>0.316</v>
+        <v>0.068</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B77">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C77">
-        <v>0.602</v>
+        <v>0.068</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B78">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C78">
-        <v>1.012</v>
+        <v>0.016</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B79">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C79">
-        <v>0.997</v>
+        <v>0.011</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45973</v>
+        <v>45978</v>
       </c>
       <c r="B80">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C80">
-        <v>1.136</v>
+        <v>0.016</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B81">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C81">
-        <v>1.137</v>
+        <v>0.013</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B82">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C82">
-        <v>0.974</v>
+        <v>0.013</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B83">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C83">
-        <v>0.498</v>
+        <v>0.013</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B84">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C84">
-        <v>0.415</v>
+        <v>0.013</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B85">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C85">
-        <v>0.064</v>
+        <v>0.013</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B86">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C86">
-        <v>0.044</v>
+        <v>0.013</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B87">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C87">
-        <v>0.039</v>
+        <v>0.013</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B88">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B89">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>0.156</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45973</v>
+        <v>45979</v>
       </c>
       <c r="B90">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>0.305</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>0.652</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C92">
-        <v>0.013</v>
+        <v>1.03</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C93">
-        <v>0.013</v>
+        <v>1.038</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B94">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C94">
-        <v>0.013</v>
+        <v>0.994</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B95">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C95">
-        <v>0.013</v>
+        <v>0.95</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B96">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C96">
-        <v>0.013</v>
+        <v>0.543</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B97">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C97">
-        <v>0.013</v>
+        <v>0.286</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B98">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C98">
-        <v>0.04</v>
+        <v>0.157</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B99">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C99">
-        <v>0.447</v>
+        <v>0.064</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B100">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C100">
-        <v>0.518</v>
+        <v>0.068</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B101">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C101">
-        <v>1.029</v>
+        <v>0.068</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B102">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C102">
-        <v>1.606</v>
+        <v>0.016</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B103">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C103">
-        <v>1.984</v>
+        <v>0.016</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45974</v>
+        <v>45979</v>
       </c>
       <c r="B104">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C104">
-        <v>1.894</v>
+        <v>0.016</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B105">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C105">
-        <v>1.014</v>
+        <v>0.013</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B106">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C106">
-        <v>0.708</v>
+        <v>0.013</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B107">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C107">
-        <v>0.386</v>
+        <v>0.013</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B108">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C108">
-        <v>0.415</v>
+        <v>0.013</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B109">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C109">
-        <v>0.064</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B110">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C110">
-        <v>0.048</v>
+        <v>0</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B111">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C111">
-        <v>0.048</v>
+        <v>0</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B112">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C112">
-        <v>0.016</v>
+        <v>0.035</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B113">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C113">
-        <v>0.016</v>
+        <v>0.242</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45974</v>
+        <v>45980</v>
       </c>
       <c r="B114">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C114">
-        <v>0.016</v>
+        <v>0.47</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B115">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C115">
-        <v>0.013</v>
+        <v>0.305</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B116">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C116">
-        <v>0.013</v>
+        <v>0.404</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B117">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>0.404</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B118">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>0.403</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B119">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>0.403</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B120">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>0.292</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B121">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>0.251</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B122">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C122">
-        <v>0.036</v>
+        <v>0.095</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B123">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C123">
-        <v>0.268</v>
+        <v>0.043</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B124">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C124">
-        <v>0.659</v>
+        <v>0.048</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B125">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C125">
-        <v>1.769</v>
+        <v>0.048</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B126">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C126">
-        <v>1.919</v>
+        <v>0.016</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B127">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C127">
-        <v>2.228</v>
+        <v>0.016</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45975</v>
+        <v>45980</v>
       </c>
       <c r="B128">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C128">
-        <v>2.059</v>
+        <v>0.016</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45975</v>
+        <v>45981</v>
       </c>
       <c r="B129">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C129">
-        <v>1.818</v>
+        <v>0.013</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45975</v>
+        <v>45981</v>
       </c>
       <c r="B130">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C130">
-        <v>1.807</v>
+        <v>0.013</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45975</v>
+        <v>45981</v>
       </c>
       <c r="B131">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C131">
-        <v>0.596</v>
+        <v>0</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45975</v>
+        <v>45981</v>
       </c>
       <c r="B132">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C132">
-        <v>0.236</v>
+        <v>0</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45975</v>
+        <v>45981</v>
       </c>
       <c r="B133">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C133">
-        <v>0.059</v>
+        <v>0</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45975</v>
+        <v>45981</v>
       </c>
       <c r="B134">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C134">
-        <v>0.044</v>
+        <v>0</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45975</v>
+        <v>45981</v>
       </c>
       <c r="B135">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C135">
-        <v>0.044</v>
+        <v>0</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45975</v>
+        <v>45981</v>
       </c>
       <c r="B136">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C136">
-        <v>0.011</v>
+        <v>0.031</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45975</v>
+        <v>45981</v>
       </c>
       <c r="B137">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C137">
-        <v>0.011</v>
+        <v>0.438</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45975</v>
+        <v>45981</v>
       </c>
       <c r="B138">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C138">
-        <v>0.011</v>
+        <v>0.601</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B139">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>1.003</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B140">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>1.873</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B141">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>1.914</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B142">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>1.832</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B143">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>1.579</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B144">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>1.011</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B145">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>0.505</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B146">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C146">
-        <v>0.036</v>
+        <v>0.421</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B147">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C147">
-        <v>0.268</v>
+        <v>0.039</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B148">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C148">
-        <v>0.659</v>
+        <v>0.044</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B149">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C149">
-        <v>1.843</v>
+        <v>0.044</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B150">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C150">
-        <v>1.847</v>
+        <v>0.011</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B151">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C151">
-        <v>2.22</v>
+        <v>0.011</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45976</v>
+        <v>45981</v>
       </c>
       <c r="B152">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C152">
-        <v>2.088</v>
+        <v>0.011</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B153">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C153">
-        <v>1.827</v>
+        <v>0</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B154">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C154">
-        <v>1.883</v>
+        <v>0</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B155">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C155">
-        <v>0.596</v>
+        <v>0</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B156">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C156">
-        <v>0.236</v>
+        <v>0.013</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B157">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C157">
-        <v>0.059</v>
+        <v>0.013</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B158">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C158">
-        <v>0.044</v>
+        <v>0</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B159">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C159">
-        <v>0.044</v>
+        <v>0</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B160">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C160">
-        <v>0.011</v>
+        <v>0.035</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B161">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C161">
-        <v>0.011</v>
+        <v>0.156</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B162">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C162">
-        <v>0.011</v>
+        <v>0.316</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45977</v>
+        <v>45982</v>
       </c>
       <c r="B163">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>0.663</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45977</v>
+        <v>45982</v>
       </c>
       <c r="B164">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C164">
-        <v>0</v>
+        <v>1.023</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45977</v>
+        <v>45982</v>
       </c>
       <c r="B165">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>1.163</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45977</v>
+        <v>45982</v>
       </c>
       <c r="B166">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>1.162</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45977</v>
+        <v>45982</v>
       </c>
       <c r="B167">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>1.021</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45977</v>
+        <v>45982</v>
       </c>
       <c r="B168">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C168">
-        <v>0</v>
+        <v>0.704</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45977</v>
+        <v>45982</v>
       </c>
       <c r="B169">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>0.292</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45977</v>
+        <v>45982</v>
       </c>
       <c r="B170">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C170">
-        <v>0.036</v>
+        <v>0.165</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Retraining the models for ELnet and NRG
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,486 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>14.11.202523</t>
-  </si>
-  <si>
-    <t>14.11.202524</t>
-  </si>
-  <si>
-    <t>15.11.20251</t>
-  </si>
-  <si>
-    <t>15.11.20252</t>
-  </si>
-  <si>
-    <t>15.11.20253</t>
-  </si>
-  <si>
-    <t>15.11.20254</t>
-  </si>
-  <si>
-    <t>15.11.20255</t>
-  </si>
-  <si>
-    <t>15.11.20256</t>
-  </si>
-  <si>
-    <t>15.11.20257</t>
-  </si>
-  <si>
-    <t>15.11.20258</t>
-  </si>
-  <si>
-    <t>15.11.20259</t>
-  </si>
-  <si>
-    <t>15.11.202510</t>
-  </si>
-  <si>
-    <t>15.11.202511</t>
-  </si>
-  <si>
-    <t>15.11.202512</t>
-  </si>
-  <si>
-    <t>15.11.202513</t>
-  </si>
-  <si>
-    <t>15.11.202514</t>
-  </si>
-  <si>
-    <t>15.11.202515</t>
-  </si>
-  <si>
-    <t>15.11.202516</t>
-  </si>
-  <si>
-    <t>15.11.202517</t>
-  </si>
-  <si>
-    <t>15.11.202518</t>
-  </si>
-  <si>
-    <t>15.11.202519</t>
-  </si>
-  <si>
-    <t>15.11.202520</t>
-  </si>
-  <si>
-    <t>15.11.202521</t>
-  </si>
-  <si>
-    <t>15.11.202522</t>
-  </si>
-  <si>
-    <t>15.11.202523</t>
-  </si>
-  <si>
-    <t>15.11.202524</t>
-  </si>
-  <si>
-    <t>16.11.20251</t>
-  </si>
-  <si>
-    <t>16.11.20252</t>
-  </si>
-  <si>
-    <t>16.11.20253</t>
-  </si>
-  <si>
-    <t>16.11.20254</t>
-  </si>
-  <si>
-    <t>16.11.20255</t>
-  </si>
-  <si>
-    <t>16.11.20256</t>
-  </si>
-  <si>
-    <t>16.11.20257</t>
-  </si>
-  <si>
-    <t>16.11.20258</t>
-  </si>
-  <si>
-    <t>16.11.20259</t>
-  </si>
-  <si>
-    <t>16.11.202510</t>
-  </si>
-  <si>
-    <t>16.11.202511</t>
-  </si>
-  <si>
-    <t>16.11.202512</t>
-  </si>
-  <si>
-    <t>16.11.202513</t>
-  </si>
-  <si>
-    <t>16.11.202514</t>
-  </si>
-  <si>
-    <t>16.11.202515</t>
-  </si>
-  <si>
-    <t>16.11.202516</t>
-  </si>
-  <si>
-    <t>16.11.202517</t>
-  </si>
-  <si>
-    <t>16.11.202518</t>
-  </si>
-  <si>
-    <t>16.11.202519</t>
-  </si>
-  <si>
-    <t>16.11.202520</t>
-  </si>
-  <si>
-    <t>16.11.202521</t>
-  </si>
-  <si>
-    <t>16.11.202522</t>
-  </si>
-  <si>
-    <t>16.11.202523</t>
-  </si>
-  <si>
-    <t>16.11.202524</t>
-  </si>
-  <si>
-    <t>17.11.20251</t>
-  </si>
-  <si>
-    <t>17.11.20252</t>
-  </si>
-  <si>
-    <t>17.11.20253</t>
-  </si>
-  <si>
-    <t>17.11.20254</t>
-  </si>
-  <si>
-    <t>17.11.20255</t>
-  </si>
-  <si>
-    <t>17.11.20256</t>
-  </si>
-  <si>
-    <t>17.11.20257</t>
-  </si>
-  <si>
-    <t>17.11.20258</t>
-  </si>
-  <si>
-    <t>17.11.20259</t>
-  </si>
-  <si>
-    <t>17.11.202510</t>
-  </si>
-  <si>
-    <t>17.11.202511</t>
-  </si>
-  <si>
-    <t>17.11.202512</t>
-  </si>
-  <si>
-    <t>17.11.202513</t>
-  </si>
-  <si>
-    <t>17.11.202514</t>
-  </si>
-  <si>
-    <t>17.11.202515</t>
-  </si>
-  <si>
-    <t>17.11.202516</t>
-  </si>
-  <si>
-    <t>17.11.202517</t>
-  </si>
-  <si>
-    <t>17.11.202518</t>
-  </si>
-  <si>
-    <t>17.11.202519</t>
-  </si>
-  <si>
-    <t>17.11.202520</t>
-  </si>
-  <si>
-    <t>17.11.202521</t>
-  </si>
-  <si>
-    <t>17.11.202522</t>
-  </si>
-  <si>
-    <t>17.11.202523</t>
-  </si>
-  <si>
-    <t>17.11.202524</t>
-  </si>
-  <si>
-    <t>18.11.20251</t>
-  </si>
-  <si>
-    <t>18.11.20252</t>
-  </si>
-  <si>
-    <t>18.11.20253</t>
-  </si>
-  <si>
-    <t>18.11.20254</t>
-  </si>
-  <si>
-    <t>18.11.20255</t>
-  </si>
-  <si>
-    <t>18.11.20256</t>
-  </si>
-  <si>
-    <t>18.11.20257</t>
-  </si>
-  <si>
-    <t>18.11.20258</t>
-  </si>
-  <si>
-    <t>18.11.20259</t>
-  </si>
-  <si>
-    <t>18.11.202510</t>
-  </si>
-  <si>
-    <t>18.11.202511</t>
-  </si>
-  <si>
-    <t>18.11.202512</t>
-  </si>
-  <si>
-    <t>18.11.202513</t>
-  </si>
-  <si>
-    <t>18.11.202514</t>
-  </si>
-  <si>
-    <t>18.11.202515</t>
-  </si>
-  <si>
-    <t>18.11.202516</t>
-  </si>
-  <si>
-    <t>18.11.202517</t>
-  </si>
-  <si>
-    <t>18.11.202518</t>
-  </si>
-  <si>
-    <t>18.11.202519</t>
-  </si>
-  <si>
-    <t>18.11.202520</t>
-  </si>
-  <si>
-    <t>18.11.202521</t>
-  </si>
-  <si>
-    <t>18.11.202522</t>
-  </si>
-  <si>
-    <t>18.11.202523</t>
-  </si>
-  <si>
-    <t>18.11.202524</t>
-  </si>
-  <si>
-    <t>19.11.20251</t>
-  </si>
-  <si>
-    <t>19.11.20252</t>
-  </si>
-  <si>
-    <t>19.11.20253</t>
-  </si>
-  <si>
-    <t>19.11.20254</t>
-  </si>
-  <si>
-    <t>19.11.20255</t>
-  </si>
-  <si>
-    <t>19.11.20256</t>
-  </si>
-  <si>
-    <t>19.11.20257</t>
-  </si>
-  <si>
-    <t>19.11.20258</t>
-  </si>
-  <si>
-    <t>19.11.20259</t>
-  </si>
-  <si>
-    <t>19.11.202510</t>
-  </si>
-  <si>
-    <t>19.11.202511</t>
-  </si>
-  <si>
-    <t>19.11.202512</t>
-  </si>
-  <si>
-    <t>19.11.202513</t>
-  </si>
-  <si>
-    <t>19.11.202514</t>
-  </si>
-  <si>
-    <t>19.11.202515</t>
-  </si>
-  <si>
-    <t>19.11.202516</t>
-  </si>
-  <si>
-    <t>19.11.202517</t>
-  </si>
-  <si>
-    <t>19.11.202518</t>
-  </si>
-  <si>
-    <t>19.11.202519</t>
-  </si>
-  <si>
-    <t>19.11.202520</t>
-  </si>
-  <si>
-    <t>19.11.202521</t>
-  </si>
-  <si>
-    <t>19.11.202522</t>
-  </si>
-  <si>
-    <t>19.11.202523</t>
-  </si>
-  <si>
-    <t>19.11.202524</t>
-  </si>
-  <si>
-    <t>20.11.20251</t>
-  </si>
-  <si>
-    <t>20.11.20252</t>
-  </si>
-  <si>
-    <t>20.11.20253</t>
-  </si>
-  <si>
-    <t>20.11.20254</t>
-  </si>
-  <si>
-    <t>20.11.20255</t>
-  </si>
-  <si>
-    <t>20.11.20256</t>
-  </si>
-  <si>
-    <t>20.11.20257</t>
-  </si>
-  <si>
-    <t>20.11.20258</t>
-  </si>
-  <si>
-    <t>20.11.20259</t>
-  </si>
-  <si>
-    <t>20.11.202510</t>
-  </si>
-  <si>
-    <t>20.11.202511</t>
-  </si>
-  <si>
-    <t>20.11.202512</t>
-  </si>
-  <si>
-    <t>20.11.202513</t>
-  </si>
-  <si>
-    <t>20.11.202514</t>
-  </si>
-  <si>
-    <t>20.11.202515</t>
-  </si>
-  <si>
-    <t>20.11.202516</t>
-  </si>
-  <si>
-    <t>20.11.202517</t>
-  </si>
-  <si>
-    <t>20.11.202518</t>
-  </si>
-  <si>
-    <t>20.11.202519</t>
-  </si>
-  <si>
-    <t>20.11.202520</t>
-  </si>
-  <si>
-    <t>20.11.202521</t>
-  </si>
-  <si>
-    <t>20.11.202522</t>
-  </si>
-  <si>
-    <t>20.11.202523</t>
-  </si>
-  <si>
-    <t>20.11.202524</t>
-  </si>
-  <si>
-    <t>21.11.20251</t>
-  </si>
-  <si>
-    <t>21.11.20252</t>
-  </si>
-  <si>
-    <t>21.11.20253</t>
-  </si>
-  <si>
-    <t>21.11.20254</t>
-  </si>
-  <si>
-    <t>21.11.20255</t>
-  </si>
-  <si>
-    <t>21.11.20256</t>
-  </si>
-  <si>
-    <t>21.11.20257</t>
-  </si>
-  <si>
-    <t>21.11.20258</t>
-  </si>
-  <si>
-    <t>21.11.20259</t>
-  </si>
-  <si>
-    <t>21.11.202510</t>
-  </si>
-  <si>
-    <t>21.11.202511</t>
-  </si>
-  <si>
-    <t>21.11.202512</t>
-  </si>
-  <si>
-    <t>21.11.202513</t>
-  </si>
-  <si>
-    <t>21.11.202514</t>
-  </si>
-  <si>
     <t>21.11.202515</t>
   </si>
   <si>
@@ -533,6 +53,486 @@
   </si>
   <si>
     <t>21.11.202523</t>
+  </si>
+  <si>
+    <t>21.11.202524</t>
+  </si>
+  <si>
+    <t>22.11.20251</t>
+  </si>
+  <si>
+    <t>22.11.20252</t>
+  </si>
+  <si>
+    <t>22.11.20253</t>
+  </si>
+  <si>
+    <t>22.11.20254</t>
+  </si>
+  <si>
+    <t>22.11.20255</t>
+  </si>
+  <si>
+    <t>22.11.20256</t>
+  </si>
+  <si>
+    <t>22.11.20257</t>
+  </si>
+  <si>
+    <t>22.11.20258</t>
+  </si>
+  <si>
+    <t>22.11.20259</t>
+  </si>
+  <si>
+    <t>22.11.202510</t>
+  </si>
+  <si>
+    <t>22.11.202511</t>
+  </si>
+  <si>
+    <t>22.11.202512</t>
+  </si>
+  <si>
+    <t>22.11.202513</t>
+  </si>
+  <si>
+    <t>22.11.202514</t>
+  </si>
+  <si>
+    <t>22.11.202515</t>
+  </si>
+  <si>
+    <t>22.11.202516</t>
+  </si>
+  <si>
+    <t>22.11.202517</t>
+  </si>
+  <si>
+    <t>22.11.202518</t>
+  </si>
+  <si>
+    <t>22.11.202519</t>
+  </si>
+  <si>
+    <t>22.11.202520</t>
+  </si>
+  <si>
+    <t>22.11.202521</t>
+  </si>
+  <si>
+    <t>22.11.202522</t>
+  </si>
+  <si>
+    <t>22.11.202523</t>
+  </si>
+  <si>
+    <t>22.11.202524</t>
+  </si>
+  <si>
+    <t>23.11.20251</t>
+  </si>
+  <si>
+    <t>23.11.20252</t>
+  </si>
+  <si>
+    <t>23.11.20253</t>
+  </si>
+  <si>
+    <t>23.11.20254</t>
+  </si>
+  <si>
+    <t>23.11.20255</t>
+  </si>
+  <si>
+    <t>23.11.20256</t>
+  </si>
+  <si>
+    <t>23.11.20257</t>
+  </si>
+  <si>
+    <t>23.11.20258</t>
+  </si>
+  <si>
+    <t>23.11.20259</t>
+  </si>
+  <si>
+    <t>23.11.202510</t>
+  </si>
+  <si>
+    <t>23.11.202511</t>
+  </si>
+  <si>
+    <t>23.11.202512</t>
+  </si>
+  <si>
+    <t>23.11.202513</t>
+  </si>
+  <si>
+    <t>23.11.202514</t>
+  </si>
+  <si>
+    <t>23.11.202515</t>
+  </si>
+  <si>
+    <t>23.11.202516</t>
+  </si>
+  <si>
+    <t>23.11.202517</t>
+  </si>
+  <si>
+    <t>23.11.202518</t>
+  </si>
+  <si>
+    <t>23.11.202519</t>
+  </si>
+  <si>
+    <t>23.11.202520</t>
+  </si>
+  <si>
+    <t>23.11.202521</t>
+  </si>
+  <si>
+    <t>23.11.202522</t>
+  </si>
+  <si>
+    <t>23.11.202523</t>
+  </si>
+  <si>
+    <t>23.11.202524</t>
+  </si>
+  <si>
+    <t>24.11.20251</t>
+  </si>
+  <si>
+    <t>24.11.20252</t>
+  </si>
+  <si>
+    <t>24.11.20253</t>
+  </si>
+  <si>
+    <t>24.11.20254</t>
+  </si>
+  <si>
+    <t>24.11.20255</t>
+  </si>
+  <si>
+    <t>24.11.20256</t>
+  </si>
+  <si>
+    <t>24.11.20257</t>
+  </si>
+  <si>
+    <t>24.11.20258</t>
+  </si>
+  <si>
+    <t>24.11.20259</t>
+  </si>
+  <si>
+    <t>24.11.202510</t>
+  </si>
+  <si>
+    <t>24.11.202511</t>
+  </si>
+  <si>
+    <t>24.11.202512</t>
+  </si>
+  <si>
+    <t>24.11.202513</t>
+  </si>
+  <si>
+    <t>24.11.202514</t>
+  </si>
+  <si>
+    <t>24.11.202515</t>
+  </si>
+  <si>
+    <t>24.11.202516</t>
+  </si>
+  <si>
+    <t>24.11.202517</t>
+  </si>
+  <si>
+    <t>24.11.202518</t>
+  </si>
+  <si>
+    <t>24.11.202519</t>
+  </si>
+  <si>
+    <t>24.11.202520</t>
+  </si>
+  <si>
+    <t>24.11.202521</t>
+  </si>
+  <si>
+    <t>24.11.202522</t>
+  </si>
+  <si>
+    <t>24.11.202523</t>
+  </si>
+  <si>
+    <t>24.11.202524</t>
+  </si>
+  <si>
+    <t>25.11.20251</t>
+  </si>
+  <si>
+    <t>25.11.20252</t>
+  </si>
+  <si>
+    <t>25.11.20253</t>
+  </si>
+  <si>
+    <t>25.11.20254</t>
+  </si>
+  <si>
+    <t>25.11.20255</t>
+  </si>
+  <si>
+    <t>25.11.20256</t>
+  </si>
+  <si>
+    <t>25.11.20257</t>
+  </si>
+  <si>
+    <t>25.11.20258</t>
+  </si>
+  <si>
+    <t>25.11.20259</t>
+  </si>
+  <si>
+    <t>25.11.202510</t>
+  </si>
+  <si>
+    <t>25.11.202511</t>
+  </si>
+  <si>
+    <t>25.11.202512</t>
+  </si>
+  <si>
+    <t>25.11.202513</t>
+  </si>
+  <si>
+    <t>25.11.202514</t>
+  </si>
+  <si>
+    <t>25.11.202515</t>
+  </si>
+  <si>
+    <t>25.11.202516</t>
+  </si>
+  <si>
+    <t>25.11.202517</t>
+  </si>
+  <si>
+    <t>25.11.202518</t>
+  </si>
+  <si>
+    <t>25.11.202519</t>
+  </si>
+  <si>
+    <t>25.11.202520</t>
+  </si>
+  <si>
+    <t>25.11.202521</t>
+  </si>
+  <si>
+    <t>25.11.202522</t>
+  </si>
+  <si>
+    <t>25.11.202523</t>
+  </si>
+  <si>
+    <t>25.11.202524</t>
+  </si>
+  <si>
+    <t>26.11.20251</t>
+  </si>
+  <si>
+    <t>26.11.20252</t>
+  </si>
+  <si>
+    <t>26.11.20253</t>
+  </si>
+  <si>
+    <t>26.11.20254</t>
+  </si>
+  <si>
+    <t>26.11.20255</t>
+  </si>
+  <si>
+    <t>26.11.20256</t>
+  </si>
+  <si>
+    <t>26.11.20257</t>
+  </si>
+  <si>
+    <t>26.11.20258</t>
+  </si>
+  <si>
+    <t>26.11.20259</t>
+  </si>
+  <si>
+    <t>26.11.202510</t>
+  </si>
+  <si>
+    <t>26.11.202511</t>
+  </si>
+  <si>
+    <t>26.11.202512</t>
+  </si>
+  <si>
+    <t>26.11.202513</t>
+  </si>
+  <si>
+    <t>26.11.202514</t>
+  </si>
+  <si>
+    <t>26.11.202515</t>
+  </si>
+  <si>
+    <t>26.11.202516</t>
+  </si>
+  <si>
+    <t>26.11.202517</t>
+  </si>
+  <si>
+    <t>26.11.202518</t>
+  </si>
+  <si>
+    <t>26.11.202519</t>
+  </si>
+  <si>
+    <t>26.11.202520</t>
+  </si>
+  <si>
+    <t>26.11.202521</t>
+  </si>
+  <si>
+    <t>26.11.202522</t>
+  </si>
+  <si>
+    <t>26.11.202523</t>
+  </si>
+  <si>
+    <t>26.11.202524</t>
+  </si>
+  <si>
+    <t>27.11.20251</t>
+  </si>
+  <si>
+    <t>27.11.20252</t>
+  </si>
+  <si>
+    <t>27.11.20253</t>
+  </si>
+  <si>
+    <t>27.11.20254</t>
+  </si>
+  <si>
+    <t>27.11.20255</t>
+  </si>
+  <si>
+    <t>27.11.20256</t>
+  </si>
+  <si>
+    <t>27.11.20257</t>
+  </si>
+  <si>
+    <t>27.11.20258</t>
+  </si>
+  <si>
+    <t>27.11.20259</t>
+  </si>
+  <si>
+    <t>27.11.202510</t>
+  </si>
+  <si>
+    <t>27.11.202511</t>
+  </si>
+  <si>
+    <t>27.11.202512</t>
+  </si>
+  <si>
+    <t>27.11.202513</t>
+  </si>
+  <si>
+    <t>27.11.202514</t>
+  </si>
+  <si>
+    <t>27.11.202515</t>
+  </si>
+  <si>
+    <t>27.11.202516</t>
+  </si>
+  <si>
+    <t>27.11.202517</t>
+  </si>
+  <si>
+    <t>27.11.202518</t>
+  </si>
+  <si>
+    <t>27.11.202519</t>
+  </si>
+  <si>
+    <t>27.11.202520</t>
+  </si>
+  <si>
+    <t>27.11.202521</t>
+  </si>
+  <si>
+    <t>27.11.202522</t>
+  </si>
+  <si>
+    <t>27.11.202523</t>
+  </si>
+  <si>
+    <t>27.11.202524</t>
+  </si>
+  <si>
+    <t>28.11.20251</t>
+  </si>
+  <si>
+    <t>28.11.20252</t>
+  </si>
+  <si>
+    <t>28.11.20253</t>
+  </si>
+  <si>
+    <t>28.11.20254</t>
+  </si>
+  <si>
+    <t>28.11.20255</t>
+  </si>
+  <si>
+    <t>28.11.20256</t>
+  </si>
+  <si>
+    <t>28.11.20257</t>
+  </si>
+  <si>
+    <t>28.11.20258</t>
+  </si>
+  <si>
+    <t>28.11.20259</t>
+  </si>
+  <si>
+    <t>28.11.202510</t>
+  </si>
+  <si>
+    <t>28.11.202511</t>
+  </si>
+  <si>
+    <t>28.11.202512</t>
+  </si>
+  <si>
+    <t>28.11.202513</t>
+  </si>
+  <si>
+    <t>28.11.202514</t>
+  </si>
+  <si>
+    <t>28.11.202515</t>
   </si>
 </sst>
 </file>
@@ -916,13 +916,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45975</v>
+        <v>45982</v>
       </c>
       <c r="B2">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.034</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -930,13 +930,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45975</v>
+        <v>45982</v>
       </c>
       <c r="B3">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.034</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>0.013</v>
+        <v>0.157</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>0.013</v>
+        <v>0.064</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>0.013</v>
+        <v>0.068</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C8">
-        <v>0.013</v>
+        <v>0.068</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C10">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45976</v>
+        <v>45982</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C11">
-        <v>0.04</v>
+        <v>0.011</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0.184</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>0.316</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B14">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>0.613</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>0.868</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B16">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>1.993</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B17">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C17">
-        <v>1.415</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B18">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>1.442</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B19">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>1.002</v>
+        <v>0.035</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B20">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>0.635</v>
+        <v>0.245</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B21">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>0.236</v>
+        <v>0.418</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B22">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C22">
-        <v>0.059</v>
+        <v>0.853</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B23">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>0.044</v>
+        <v>1.11</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B24">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>0.044</v>
+        <v>1.152</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B25">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C25">
-        <v>0.011</v>
+        <v>1.041</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B26">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C26">
-        <v>0.011</v>
+        <v>0.865</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="B27">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C27">
-        <v>0.011</v>
+        <v>0.732</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45977</v>
+        <v>45983</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C28">
-        <v>0.013</v>
+        <v>0.308</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45977</v>
+        <v>45983</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C29">
-        <v>0.013</v>
+        <v>0.276</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45977</v>
+        <v>45983</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C30">
-        <v>0.013</v>
+        <v>0.054</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45977</v>
+        <v>45983</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C31">
-        <v>0.013</v>
+        <v>0.059</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45977</v>
+        <v>45983</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C32">
-        <v>0.013</v>
+        <v>0.059</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45977</v>
+        <v>45983</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C33">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45977</v>
+        <v>45983</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C34">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45977</v>
+        <v>45983</v>
       </c>
       <c r="B35">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C35">
-        <v>0.04</v>
+        <v>0.011</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B36">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>0.447</v>
+        <v>0.013</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B37">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C37">
-        <v>0.436</v>
+        <v>0.013</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B38">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C38">
-        <v>1.049</v>
+        <v>0.013</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B39">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C39">
-        <v>1.055</v>
+        <v>0.013</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B40">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C40">
-        <v>1.993</v>
+        <v>0.013</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B41">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C41">
-        <v>1.535</v>
+        <v>0.013</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B42">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>1.258</v>
+        <v>0.013</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B43">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C43">
-        <v>0.9429999999999999</v>
+        <v>0.04</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B44">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>0.476</v>
+        <v>0.25</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B45">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C45">
-        <v>0.415</v>
+        <v>0.311</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B46">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C46">
-        <v>0.064</v>
+        <v>0.349</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B47">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C47">
-        <v>0.048</v>
+        <v>0.404</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B48">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C48">
-        <v>0.048</v>
+        <v>0.533</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B49">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C49">
-        <v>0.016</v>
+        <v>0.59</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B50">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C50">
-        <v>0.016</v>
+        <v>0.469</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="B51">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>0.016</v>
+        <v>0.408</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45978</v>
+        <v>45984</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C52">
-        <v>0.013</v>
+        <v>0.297</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45978</v>
+        <v>45984</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C53">
-        <v>0.013</v>
+        <v>0.095</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45978</v>
+        <v>45984</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C54">
-        <v>0.013</v>
+        <v>0.043</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45978</v>
+        <v>45984</v>
       </c>
       <c r="B55">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C55">
-        <v>0.013</v>
+        <v>0.048</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45978</v>
+        <v>45984</v>
       </c>
       <c r="B56">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C56">
-        <v>0.013</v>
+        <v>0.048</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45978</v>
+        <v>45984</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C57">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45978</v>
+        <v>45984</v>
       </c>
       <c r="B58">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C58">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45978</v>
+        <v>45984</v>
       </c>
       <c r="B59">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C59">
-        <v>0.04</v>
+        <v>0.016</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B60">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C60">
-        <v>0.447</v>
+        <v>0.013</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B61">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C61">
-        <v>0.549</v>
+        <v>0.013</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B62">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>1.026</v>
+        <v>0.011</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B63">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C63">
-        <v>1.614</v>
+        <v>0.011</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B64">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C64">
-        <v>1.839</v>
+        <v>0.011</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B65">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C65">
-        <v>1.683</v>
+        <v>0.011</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B66">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C66">
-        <v>1.388</v>
+        <v>0.011</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B67">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C67">
-        <v>0.9429999999999999</v>
+        <v>0.038</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B68">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C68">
-        <v>0.471</v>
+        <v>0.445</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B69">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C69">
-        <v>0.415</v>
+        <v>0.67</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B70">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C70">
-        <v>0.064</v>
+        <v>1.299</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B71">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C71">
-        <v>0.068</v>
+        <v>2.053</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B72">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C72">
-        <v>0.068</v>
+        <v>2.356</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B73">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C73">
-        <v>0.016</v>
+        <v>2.284</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B74">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C74">
-        <v>0.011</v>
+        <v>1.933</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="B75">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C75">
-        <v>0.011</v>
+        <v>1.559</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45979</v>
+        <v>45985</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C76">
-        <v>0.013</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45979</v>
+        <v>45985</v>
       </c>
       <c r="B77">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C77">
-        <v>0.013</v>
+        <v>0.421</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45979</v>
+        <v>45985</v>
       </c>
       <c r="B78">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C78">
-        <v>0.013</v>
+        <v>0.039</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45979</v>
+        <v>45985</v>
       </c>
       <c r="B79">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C79">
-        <v>0.013</v>
+        <v>0.044</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45979</v>
+        <v>45985</v>
       </c>
       <c r="B80">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C80">
-        <v>0.013</v>
+        <v>0.044</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45979</v>
+        <v>45985</v>
       </c>
       <c r="B81">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C81">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45979</v>
+        <v>45985</v>
       </c>
       <c r="B82">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C82">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45979</v>
+        <v>45985</v>
       </c>
       <c r="B83">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C83">
-        <v>0.04</v>
+        <v>0.011</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B84">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C84">
-        <v>0.156</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B85">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C85">
-        <v>0.305</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B86">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C86">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B87">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C87">
-        <v>1.026</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B88">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C88">
-        <v>1.23</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B89">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C89">
-        <v>1.076</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B90">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C90">
-        <v>0.988</v>
+        <v>0.013</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B91">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C91">
-        <v>0.543</v>
+        <v>0.04</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B92">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C92">
-        <v>0.286</v>
+        <v>0.181</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B93">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C93">
-        <v>0.157</v>
+        <v>0.544</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B94">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C94">
-        <v>0.064</v>
+        <v>1.033</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B95">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C95">
-        <v>0.068</v>
+        <v>1.897</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B96">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C96">
-        <v>0.068</v>
+        <v>1.932</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B97">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C97">
-        <v>0.016</v>
+        <v>2.042</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B98">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C98">
-        <v>0.016</v>
+        <v>1.692</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="B99">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C99">
-        <v>0.016</v>
+        <v>1.033</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45980</v>
+        <v>45986</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C100">
-        <v>0.013</v>
+        <v>0.518</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45980</v>
+        <v>45986</v>
       </c>
       <c r="B101">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C101">
-        <v>0.013</v>
+        <v>0.426</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45980</v>
+        <v>45986</v>
       </c>
       <c r="B102">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C102">
-        <v>0.013</v>
+        <v>0.039</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45980</v>
+        <v>45986</v>
       </c>
       <c r="B103">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C103">
-        <v>0.013</v>
+        <v>0.044</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45980</v>
+        <v>45986</v>
       </c>
       <c r="B104">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C104">
-        <v>0.013</v>
+        <v>0.044</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45980</v>
+        <v>45986</v>
       </c>
       <c r="B105">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C105">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45980</v>
+        <v>45986</v>
       </c>
       <c r="B106">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C106">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45980</v>
+        <v>45986</v>
       </c>
       <c r="B107">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C107">
-        <v>0.04</v>
+        <v>0.011</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B108">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C108">
-        <v>0.091</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B109">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C109">
-        <v>0.27</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B110">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C110">
-        <v>0.354</v>
+        <v>0</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B111">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C111">
-        <v>0.409</v>
+        <v>0</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B112">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C112">
-        <v>0.404</v>
+        <v>0.013</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B113">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C113">
-        <v>0.403</v>
+        <v>0.013</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B114">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C114">
-        <v>0.335</v>
+        <v>0.013</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B115">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C115">
-        <v>0.287</v>
+        <v>0.036</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B116">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C116">
-        <v>0.246</v>
+        <v>0.153</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B117">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C117">
-        <v>0.09</v>
+        <v>0.45</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B118">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C118">
-        <v>0.038</v>
+        <v>1.025</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B119">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C119">
-        <v>0.043</v>
+        <v>1.761</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B120">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C120">
-        <v>0.043</v>
+        <v>1.806</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B121">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C121">
-        <v>0.011</v>
+        <v>1.894</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B122">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C122">
-        <v>0.011</v>
+        <v>1.084</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45980</v>
+        <v>45987</v>
       </c>
       <c r="B123">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C123">
-        <v>0.011</v>
+        <v>0.652</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45981</v>
+        <v>45987</v>
       </c>
       <c r="B124">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>0.286</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45981</v>
+        <v>45987</v>
       </c>
       <c r="B125">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>0.157</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45981</v>
+        <v>45987</v>
       </c>
       <c r="B126">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>0.043</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45981</v>
+        <v>45987</v>
       </c>
       <c r="B127">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45981</v>
+        <v>45987</v>
       </c>
       <c r="B128">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45981</v>
+        <v>45987</v>
       </c>
       <c r="B129">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45981</v>
+        <v>45987</v>
       </c>
       <c r="B130">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45981</v>
+        <v>45987</v>
       </c>
       <c r="B131">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C131">
-        <v>0.031</v>
+        <v>0.016</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B132">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C132">
-        <v>0.438</v>
+        <v>0.013</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B133">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C133">
-        <v>0.657</v>
+        <v>0.013</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B134">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C134">
-        <v>1.073</v>
+        <v>0.013</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B135">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C135">
-        <v>1.76</v>
+        <v>0.013</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B136">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C136">
-        <v>2.139</v>
+        <v>0.013</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B137">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C137">
-        <v>1.931</v>
+        <v>0.013</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B138">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C138">
-        <v>1.764</v>
+        <v>0.013</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B139">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C139">
-        <v>1.218</v>
+        <v>0.04</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B140">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C140">
-        <v>0.614</v>
+        <v>0.091</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B141">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C141">
-        <v>0.411</v>
+        <v>0.27</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B142">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C142">
-        <v>0.039</v>
+        <v>0.488</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B143">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C143">
-        <v>0.044</v>
+        <v>0.594</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B144">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C144">
-        <v>0.044</v>
+        <v>0.641</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B145">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C145">
-        <v>0.011</v>
+        <v>0.522</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B146">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C146">
-        <v>0.011</v>
+        <v>0.398</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="B147">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C147">
-        <v>0.011</v>
+        <v>0.286</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45982</v>
+        <v>45988</v>
       </c>
       <c r="B148">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C148">
-        <v>0</v>
+        <v>0.241</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45982</v>
+        <v>45988</v>
       </c>
       <c r="B149">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>0.091</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45982</v>
+        <v>45988</v>
       </c>
       <c r="B150">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C150">
-        <v>0</v>
+        <v>0.043</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45982</v>
+        <v>45988</v>
       </c>
       <c r="B151">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45982</v>
+        <v>45988</v>
       </c>
       <c r="B152">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C152">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45982</v>
+        <v>45988</v>
       </c>
       <c r="B153">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45982</v>
+        <v>45988</v>
       </c>
       <c r="B154">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45982</v>
+        <v>45988</v>
       </c>
       <c r="B155">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C155">
-        <v>0.035</v>
+        <v>0.016</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B156">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C156">
-        <v>0.151</v>
+        <v>0.013</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B157">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C157">
-        <v>0.311</v>
+        <v>0.013</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B158">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C158">
-        <v>0.722</v>
+        <v>0.013</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B159">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C159">
-        <v>1.105</v>
+        <v>0.013</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B160">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C160">
-        <v>1.267</v>
+        <v>0.013</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B161">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C161">
-        <v>1.23</v>
+        <v>0.013</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B162">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C162">
-        <v>0.961</v>
+        <v>0.013</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B163">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C163">
-        <v>0.979</v>
+        <v>0.04</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B164">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C164">
-        <v>0.281</v>
+        <v>0.091</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B165">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C165">
-        <v>0.154</v>
+        <v>0.27</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B166">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C166">
-        <v>0.064</v>
+        <v>0.42</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B167">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C167">
-        <v>0.068</v>
+        <v>0.545</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B168">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C168">
-        <v>0.063</v>
+        <v>0.652</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B169">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C169">
-        <v>0.011</v>
+        <v>0.601</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B170">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C170">
-        <v>0.011</v>
+        <v>0.469</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Adding Sun Grow Lucia to the Portfolio Forecast
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>21.11.202515</t>
-  </si>
-  <si>
-    <t>21.11.202516</t>
-  </si>
-  <si>
-    <t>21.11.202517</t>
-  </si>
-  <si>
-    <t>21.11.202518</t>
-  </si>
-  <si>
-    <t>21.11.202519</t>
-  </si>
-  <si>
-    <t>21.11.202520</t>
-  </si>
-  <si>
-    <t>21.11.202521</t>
-  </si>
-  <si>
-    <t>21.11.202522</t>
-  </si>
-  <si>
-    <t>21.11.202523</t>
-  </si>
-  <si>
-    <t>21.11.202524</t>
-  </si>
-  <si>
-    <t>22.11.20251</t>
-  </si>
-  <si>
-    <t>22.11.20252</t>
-  </si>
-  <si>
-    <t>22.11.20253</t>
-  </si>
-  <si>
-    <t>22.11.20254</t>
-  </si>
-  <si>
-    <t>22.11.20255</t>
-  </si>
-  <si>
-    <t>22.11.20256</t>
-  </si>
-  <si>
-    <t>22.11.20257</t>
-  </si>
-  <si>
-    <t>22.11.20258</t>
-  </si>
-  <si>
-    <t>22.11.20259</t>
-  </si>
-  <si>
-    <t>22.11.202510</t>
-  </si>
-  <si>
-    <t>22.11.202511</t>
-  </si>
-  <si>
-    <t>22.11.202512</t>
-  </si>
-  <si>
-    <t>22.11.202513</t>
-  </si>
-  <si>
-    <t>22.11.202514</t>
-  </si>
-  <si>
-    <t>22.11.202515</t>
-  </si>
-  <si>
-    <t>22.11.202516</t>
-  </si>
-  <si>
-    <t>22.11.202517</t>
-  </si>
-  <si>
-    <t>22.11.202518</t>
-  </si>
-  <si>
-    <t>22.11.202519</t>
-  </si>
-  <si>
-    <t>22.11.202520</t>
-  </si>
-  <si>
-    <t>22.11.202521</t>
-  </si>
-  <si>
-    <t>22.11.202522</t>
-  </si>
-  <si>
-    <t>22.11.202523</t>
-  </si>
-  <si>
-    <t>22.11.202524</t>
-  </si>
-  <si>
-    <t>23.11.20251</t>
-  </si>
-  <si>
-    <t>23.11.20252</t>
-  </si>
-  <si>
-    <t>23.11.20253</t>
-  </si>
-  <si>
-    <t>23.11.20254</t>
-  </si>
-  <si>
-    <t>23.11.20255</t>
-  </si>
-  <si>
-    <t>23.11.20256</t>
-  </si>
-  <si>
-    <t>23.11.20257</t>
-  </si>
-  <si>
-    <t>23.11.20258</t>
-  </si>
-  <si>
-    <t>23.11.20259</t>
-  </si>
-  <si>
-    <t>23.11.202510</t>
-  </si>
-  <si>
-    <t>23.11.202511</t>
-  </si>
-  <si>
-    <t>23.11.202512</t>
-  </si>
-  <si>
-    <t>23.11.202513</t>
-  </si>
-  <si>
-    <t>23.11.202514</t>
-  </si>
-  <si>
-    <t>23.11.202515</t>
-  </si>
-  <si>
-    <t>23.11.202516</t>
-  </si>
-  <si>
-    <t>23.11.202517</t>
-  </si>
-  <si>
-    <t>23.11.202518</t>
-  </si>
-  <si>
-    <t>23.11.202519</t>
-  </si>
-  <si>
-    <t>23.11.202520</t>
-  </si>
-  <si>
-    <t>23.11.202521</t>
-  </si>
-  <si>
-    <t>23.11.202522</t>
-  </si>
-  <si>
-    <t>23.11.202523</t>
-  </si>
-  <si>
-    <t>23.11.202524</t>
-  </si>
-  <si>
-    <t>24.11.20251</t>
-  </si>
-  <si>
-    <t>24.11.20252</t>
-  </si>
-  <si>
-    <t>24.11.20253</t>
-  </si>
-  <si>
-    <t>24.11.20254</t>
-  </si>
-  <si>
-    <t>24.11.20255</t>
-  </si>
-  <si>
-    <t>24.11.20256</t>
-  </si>
-  <si>
-    <t>24.11.20257</t>
-  </si>
-  <si>
-    <t>24.11.20258</t>
-  </si>
-  <si>
-    <t>24.11.20259</t>
-  </si>
-  <si>
-    <t>24.11.202510</t>
-  </si>
-  <si>
-    <t>24.11.202511</t>
-  </si>
-  <si>
-    <t>24.11.202512</t>
-  </si>
-  <si>
-    <t>24.11.202513</t>
-  </si>
-  <si>
-    <t>24.11.202514</t>
-  </si>
-  <si>
-    <t>24.11.202515</t>
-  </si>
-  <si>
-    <t>24.11.202516</t>
-  </si>
-  <si>
-    <t>24.11.202517</t>
-  </si>
-  <si>
-    <t>24.11.202518</t>
-  </si>
-  <si>
-    <t>24.11.202519</t>
-  </si>
-  <si>
-    <t>24.11.202520</t>
-  </si>
-  <si>
-    <t>24.11.202521</t>
-  </si>
-  <si>
-    <t>24.11.202522</t>
-  </si>
-  <si>
-    <t>24.11.202523</t>
-  </si>
-  <si>
-    <t>24.11.202524</t>
-  </si>
-  <si>
-    <t>25.11.20251</t>
-  </si>
-  <si>
-    <t>25.11.20252</t>
-  </si>
-  <si>
-    <t>25.11.20253</t>
-  </si>
-  <si>
-    <t>25.11.20254</t>
-  </si>
-  <si>
-    <t>25.11.20255</t>
-  </si>
-  <si>
-    <t>25.11.20256</t>
-  </si>
-  <si>
-    <t>25.11.20257</t>
-  </si>
-  <si>
-    <t>25.11.20258</t>
-  </si>
-  <si>
-    <t>25.11.20259</t>
-  </si>
-  <si>
-    <t>25.11.202510</t>
-  </si>
-  <si>
-    <t>25.11.202511</t>
-  </si>
-  <si>
-    <t>25.11.202512</t>
-  </si>
-  <si>
-    <t>25.11.202513</t>
-  </si>
-  <si>
-    <t>25.11.202514</t>
-  </si>
-  <si>
-    <t>25.11.202515</t>
-  </si>
-  <si>
-    <t>25.11.202516</t>
-  </si>
-  <si>
-    <t>25.11.202517</t>
-  </si>
-  <si>
-    <t>25.11.202518</t>
-  </si>
-  <si>
-    <t>25.11.202519</t>
-  </si>
-  <si>
-    <t>25.11.202520</t>
-  </si>
-  <si>
-    <t>25.11.202521</t>
-  </si>
-  <si>
-    <t>25.11.202522</t>
-  </si>
-  <si>
-    <t>25.11.202523</t>
-  </si>
-  <si>
-    <t>25.11.202524</t>
-  </si>
-  <si>
-    <t>26.11.20251</t>
-  </si>
-  <si>
-    <t>26.11.20252</t>
-  </si>
-  <si>
-    <t>26.11.20253</t>
-  </si>
-  <si>
-    <t>26.11.20254</t>
-  </si>
-  <si>
-    <t>26.11.20255</t>
-  </si>
-  <si>
-    <t>26.11.20256</t>
-  </si>
-  <si>
-    <t>26.11.20257</t>
-  </si>
-  <si>
-    <t>26.11.20258</t>
-  </si>
-  <si>
-    <t>26.11.20259</t>
-  </si>
-  <si>
-    <t>26.11.202510</t>
-  </si>
-  <si>
-    <t>26.11.202511</t>
-  </si>
-  <si>
-    <t>26.11.202512</t>
-  </si>
-  <si>
-    <t>26.11.202513</t>
-  </si>
-  <si>
-    <t>26.11.202514</t>
-  </si>
-  <si>
-    <t>26.11.202515</t>
-  </si>
-  <si>
-    <t>26.11.202516</t>
-  </si>
-  <si>
-    <t>26.11.202517</t>
-  </si>
-  <si>
-    <t>26.11.202518</t>
-  </si>
-  <si>
-    <t>26.11.202519</t>
-  </si>
-  <si>
-    <t>26.11.202520</t>
-  </si>
-  <si>
-    <t>26.11.202521</t>
-  </si>
-  <si>
-    <t>26.11.202522</t>
-  </si>
-  <si>
-    <t>26.11.202523</t>
-  </si>
-  <si>
-    <t>26.11.202524</t>
-  </si>
-  <si>
-    <t>27.11.20251</t>
-  </si>
-  <si>
-    <t>27.11.20252</t>
-  </si>
-  <si>
-    <t>27.11.20253</t>
-  </si>
-  <si>
-    <t>27.11.20254</t>
-  </si>
-  <si>
-    <t>27.11.20255</t>
-  </si>
-  <si>
-    <t>27.11.20256</t>
-  </si>
-  <si>
-    <t>27.11.20257</t>
-  </si>
-  <si>
-    <t>27.11.20258</t>
-  </si>
-  <si>
-    <t>27.11.20259</t>
-  </si>
-  <si>
-    <t>27.11.202510</t>
-  </si>
-  <si>
-    <t>27.11.202511</t>
-  </si>
-  <si>
-    <t>27.11.202512</t>
-  </si>
-  <si>
-    <t>27.11.202513</t>
-  </si>
-  <si>
-    <t>27.11.202514</t>
-  </si>
-  <si>
-    <t>27.11.202515</t>
-  </si>
-  <si>
-    <t>27.11.202516</t>
-  </si>
-  <si>
-    <t>27.11.202517</t>
-  </si>
-  <si>
-    <t>27.11.202518</t>
-  </si>
-  <si>
-    <t>27.11.202519</t>
-  </si>
-  <si>
-    <t>27.11.202520</t>
-  </si>
-  <si>
-    <t>27.11.202521</t>
-  </si>
-  <si>
-    <t>27.11.202522</t>
-  </si>
-  <si>
-    <t>27.11.202523</t>
-  </si>
-  <si>
-    <t>27.11.202524</t>
-  </si>
-  <si>
-    <t>28.11.20251</t>
-  </si>
-  <si>
-    <t>28.11.20252</t>
-  </si>
-  <si>
-    <t>28.11.20253</t>
-  </si>
-  <si>
-    <t>28.11.20254</t>
-  </si>
-  <si>
-    <t>28.11.20255</t>
-  </si>
-  <si>
-    <t>28.11.20256</t>
-  </si>
-  <si>
-    <t>28.11.20257</t>
-  </si>
-  <si>
-    <t>28.11.20258</t>
-  </si>
-  <si>
-    <t>28.11.20259</t>
-  </si>
-  <si>
-    <t>28.11.202510</t>
-  </si>
-  <si>
-    <t>28.11.202511</t>
-  </si>
-  <si>
-    <t>28.11.202512</t>
-  </si>
-  <si>
-    <t>28.11.202513</t>
-  </si>
-  <si>
-    <t>28.11.202514</t>
-  </si>
-  <si>
-    <t>28.11.202515</t>
+    <t>30.11.202514</t>
+  </si>
+  <si>
+    <t>30.11.202515</t>
+  </si>
+  <si>
+    <t>30.11.202516</t>
+  </si>
+  <si>
+    <t>30.11.202517</t>
+  </si>
+  <si>
+    <t>30.11.202518</t>
+  </si>
+  <si>
+    <t>30.11.202519</t>
+  </si>
+  <si>
+    <t>30.11.202520</t>
+  </si>
+  <si>
+    <t>30.11.202521</t>
+  </si>
+  <si>
+    <t>30.11.202522</t>
+  </si>
+  <si>
+    <t>30.11.202523</t>
+  </si>
+  <si>
+    <t>30.11.202524</t>
+  </si>
+  <si>
+    <t>01.12.20251</t>
+  </si>
+  <si>
+    <t>01.12.20252</t>
+  </si>
+  <si>
+    <t>01.12.20253</t>
+  </si>
+  <si>
+    <t>01.12.20254</t>
+  </si>
+  <si>
+    <t>01.12.20255</t>
+  </si>
+  <si>
+    <t>01.12.20256</t>
+  </si>
+  <si>
+    <t>01.12.20257</t>
+  </si>
+  <si>
+    <t>01.12.20258</t>
+  </si>
+  <si>
+    <t>01.12.20259</t>
+  </si>
+  <si>
+    <t>01.12.202510</t>
+  </si>
+  <si>
+    <t>01.12.202511</t>
+  </si>
+  <si>
+    <t>01.12.202512</t>
+  </si>
+  <si>
+    <t>01.12.202513</t>
+  </si>
+  <si>
+    <t>01.12.202514</t>
+  </si>
+  <si>
+    <t>01.12.202515</t>
+  </si>
+  <si>
+    <t>01.12.202516</t>
+  </si>
+  <si>
+    <t>01.12.202517</t>
+  </si>
+  <si>
+    <t>01.12.202518</t>
+  </si>
+  <si>
+    <t>01.12.202519</t>
+  </si>
+  <si>
+    <t>01.12.202520</t>
+  </si>
+  <si>
+    <t>01.12.202521</t>
+  </si>
+  <si>
+    <t>01.12.202522</t>
+  </si>
+  <si>
+    <t>01.12.202523</t>
+  </si>
+  <si>
+    <t>01.12.202524</t>
+  </si>
+  <si>
+    <t>02.12.20251</t>
+  </si>
+  <si>
+    <t>02.12.20252</t>
+  </si>
+  <si>
+    <t>02.12.20253</t>
+  </si>
+  <si>
+    <t>02.12.20254</t>
+  </si>
+  <si>
+    <t>02.12.20255</t>
+  </si>
+  <si>
+    <t>02.12.20256</t>
+  </si>
+  <si>
+    <t>02.12.20257</t>
+  </si>
+  <si>
+    <t>02.12.20258</t>
+  </si>
+  <si>
+    <t>02.12.20259</t>
+  </si>
+  <si>
+    <t>02.12.202510</t>
+  </si>
+  <si>
+    <t>02.12.202511</t>
+  </si>
+  <si>
+    <t>02.12.202512</t>
+  </si>
+  <si>
+    <t>02.12.202513</t>
+  </si>
+  <si>
+    <t>02.12.202514</t>
+  </si>
+  <si>
+    <t>02.12.202515</t>
+  </si>
+  <si>
+    <t>02.12.202516</t>
+  </si>
+  <si>
+    <t>02.12.202517</t>
+  </si>
+  <si>
+    <t>02.12.202518</t>
+  </si>
+  <si>
+    <t>02.12.202519</t>
+  </si>
+  <si>
+    <t>02.12.202520</t>
+  </si>
+  <si>
+    <t>02.12.202521</t>
+  </si>
+  <si>
+    <t>02.12.202522</t>
+  </si>
+  <si>
+    <t>02.12.202523</t>
+  </si>
+  <si>
+    <t>02.12.202524</t>
+  </si>
+  <si>
+    <t>03.12.20251</t>
+  </si>
+  <si>
+    <t>03.12.20252</t>
+  </si>
+  <si>
+    <t>03.12.20253</t>
+  </si>
+  <si>
+    <t>03.12.20254</t>
+  </si>
+  <si>
+    <t>03.12.20255</t>
+  </si>
+  <si>
+    <t>03.12.20256</t>
+  </si>
+  <si>
+    <t>03.12.20257</t>
+  </si>
+  <si>
+    <t>03.12.20258</t>
+  </si>
+  <si>
+    <t>03.12.20259</t>
+  </si>
+  <si>
+    <t>03.12.202510</t>
+  </si>
+  <si>
+    <t>03.12.202511</t>
+  </si>
+  <si>
+    <t>03.12.202512</t>
+  </si>
+  <si>
+    <t>03.12.202513</t>
+  </si>
+  <si>
+    <t>03.12.202514</t>
+  </si>
+  <si>
+    <t>03.12.202515</t>
+  </si>
+  <si>
+    <t>03.12.202516</t>
+  </si>
+  <si>
+    <t>03.12.202517</t>
+  </si>
+  <si>
+    <t>03.12.202518</t>
+  </si>
+  <si>
+    <t>03.12.202519</t>
+  </si>
+  <si>
+    <t>03.12.202520</t>
+  </si>
+  <si>
+    <t>03.12.202521</t>
+  </si>
+  <si>
+    <t>03.12.202522</t>
+  </si>
+  <si>
+    <t>03.12.202523</t>
+  </si>
+  <si>
+    <t>03.12.202524</t>
+  </si>
+  <si>
+    <t>04.12.20251</t>
+  </si>
+  <si>
+    <t>04.12.20252</t>
+  </si>
+  <si>
+    <t>04.12.20253</t>
+  </si>
+  <si>
+    <t>04.12.20254</t>
+  </si>
+  <si>
+    <t>04.12.20255</t>
+  </si>
+  <si>
+    <t>04.12.20256</t>
+  </si>
+  <si>
+    <t>04.12.20257</t>
+  </si>
+  <si>
+    <t>04.12.20258</t>
+  </si>
+  <si>
+    <t>04.12.20259</t>
+  </si>
+  <si>
+    <t>04.12.202510</t>
+  </si>
+  <si>
+    <t>04.12.202511</t>
+  </si>
+  <si>
+    <t>04.12.202512</t>
+  </si>
+  <si>
+    <t>04.12.202513</t>
+  </si>
+  <si>
+    <t>04.12.202514</t>
+  </si>
+  <si>
+    <t>04.12.202515</t>
+  </si>
+  <si>
+    <t>04.12.202516</t>
+  </si>
+  <si>
+    <t>04.12.202517</t>
+  </si>
+  <si>
+    <t>04.12.202518</t>
+  </si>
+  <si>
+    <t>04.12.202519</t>
+  </si>
+  <si>
+    <t>04.12.202520</t>
+  </si>
+  <si>
+    <t>04.12.202521</t>
+  </si>
+  <si>
+    <t>04.12.202522</t>
+  </si>
+  <si>
+    <t>04.12.202523</t>
+  </si>
+  <si>
+    <t>04.12.202524</t>
+  </si>
+  <si>
+    <t>05.12.20251</t>
+  </si>
+  <si>
+    <t>05.12.20252</t>
+  </si>
+  <si>
+    <t>05.12.20253</t>
+  </si>
+  <si>
+    <t>05.12.20254</t>
+  </si>
+  <si>
+    <t>05.12.20255</t>
+  </si>
+  <si>
+    <t>05.12.20256</t>
+  </si>
+  <si>
+    <t>05.12.20257</t>
+  </si>
+  <si>
+    <t>05.12.20258</t>
+  </si>
+  <si>
+    <t>05.12.20259</t>
+  </si>
+  <si>
+    <t>05.12.202510</t>
+  </si>
+  <si>
+    <t>05.12.202511</t>
+  </si>
+  <si>
+    <t>05.12.202512</t>
+  </si>
+  <si>
+    <t>05.12.202513</t>
+  </si>
+  <si>
+    <t>05.12.202514</t>
+  </si>
+  <si>
+    <t>05.12.202515</t>
+  </si>
+  <si>
+    <t>05.12.202516</t>
+  </si>
+  <si>
+    <t>05.12.202517</t>
+  </si>
+  <si>
+    <t>05.12.202518</t>
+  </si>
+  <si>
+    <t>05.12.202519</t>
+  </si>
+  <si>
+    <t>05.12.202520</t>
+  </si>
+  <si>
+    <t>05.12.202521</t>
+  </si>
+  <si>
+    <t>05.12.202522</t>
+  </si>
+  <si>
+    <t>05.12.202523</t>
+  </si>
+  <si>
+    <t>05.12.202524</t>
+  </si>
+  <si>
+    <t>06.12.20251</t>
+  </si>
+  <si>
+    <t>06.12.20252</t>
+  </si>
+  <si>
+    <t>06.12.20253</t>
+  </si>
+  <si>
+    <t>06.12.20254</t>
+  </si>
+  <si>
+    <t>06.12.20255</t>
+  </si>
+  <si>
+    <t>06.12.20256</t>
+  </si>
+  <si>
+    <t>06.12.20257</t>
+  </si>
+  <si>
+    <t>06.12.20258</t>
+  </si>
+  <si>
+    <t>06.12.20259</t>
+  </si>
+  <si>
+    <t>06.12.202510</t>
+  </si>
+  <si>
+    <t>06.12.202511</t>
+  </si>
+  <si>
+    <t>06.12.202512</t>
+  </si>
+  <si>
+    <t>06.12.202513</t>
+  </si>
+  <si>
+    <t>06.12.202514</t>
+  </si>
+  <si>
+    <t>06.12.202515</t>
+  </si>
+  <si>
+    <t>06.12.202516</t>
+  </si>
+  <si>
+    <t>06.12.202517</t>
+  </si>
+  <si>
+    <t>06.12.202518</t>
+  </si>
+  <si>
+    <t>06.12.202519</t>
+  </si>
+  <si>
+    <t>06.12.202520</t>
+  </si>
+  <si>
+    <t>06.12.202521</t>
+  </si>
+  <si>
+    <t>06.12.202522</t>
+  </si>
+  <si>
+    <t>06.12.202523</t>
+  </si>
+  <si>
+    <t>06.12.202524</t>
+  </si>
+  <si>
+    <t>07.12.20251</t>
+  </si>
+  <si>
+    <t>07.12.20252</t>
+  </si>
+  <si>
+    <t>07.12.20253</t>
+  </si>
+  <si>
+    <t>07.12.20254</t>
+  </si>
+  <si>
+    <t>07.12.20255</t>
+  </si>
+  <si>
+    <t>07.12.20256</t>
+  </si>
+  <si>
+    <t>07.12.20257</t>
+  </si>
+  <si>
+    <t>07.12.20258</t>
+  </si>
+  <si>
+    <t>07.12.20259</t>
+  </si>
+  <si>
+    <t>07.12.202510</t>
+  </si>
+  <si>
+    <t>07.12.202511</t>
+  </si>
+  <si>
+    <t>07.12.202512</t>
+  </si>
+  <si>
+    <t>07.12.202513</t>
+  </si>
+  <si>
+    <t>07.12.202514</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45982</v>
+        <v>45991</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>0.034</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45982</v>
+        <v>45991</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>0.034</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45982</v>
+        <v>45991</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>0.5600000000000001</v>
+        <v>0.269</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45982</v>
+        <v>45991</v>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <v>0.157</v>
+        <v>0.154</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45982</v>
+        <v>45991</v>
       </c>
       <c r="B6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>0.064</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45982</v>
+        <v>45991</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7">
-        <v>0.068</v>
+        <v>0.038</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45982</v>
+        <v>45991</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>0.068</v>
+        <v>0.043</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45982</v>
+        <v>45991</v>
       </c>
       <c r="B9">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9">
-        <v>0.011</v>
+        <v>0.043</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,10 +1028,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45982</v>
+        <v>45991</v>
       </c>
       <c r="B10">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>0.011</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45982</v>
+        <v>45991</v>
       </c>
       <c r="B11">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>0.011</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45983</v>
+        <v>45991</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>0.035</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>0.245</v>
+        <v>0.035</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>0.418</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B22">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>0.853</v>
+        <v>0.265</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23">
-        <v>1.11</v>
+        <v>0.305</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B24">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24">
-        <v>1.152</v>
+        <v>0.409</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B25">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25">
-        <v>1.041</v>
+        <v>0.652</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B26">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26">
-        <v>0.865</v>
+        <v>0.721</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B27">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27">
-        <v>0.732</v>
+        <v>0.636</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B28">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28">
-        <v>0.308</v>
+        <v>0.47</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B29">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29">
-        <v>0.276</v>
+        <v>0.251</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B30">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30">
-        <v>0.054</v>
+        <v>0.095</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B31">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31">
-        <v>0.059</v>
+        <v>0.038</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B32">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C32">
-        <v>0.059</v>
+        <v>0.043</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B33">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>0.043</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,10 +1364,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B34">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>0.011</v>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="B35">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35">
         <v>0.011</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45984</v>
+        <v>45992</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C36">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B43">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B44">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C44">
-        <v>0.25</v>
+        <v>0.035</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B45">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C45">
-        <v>0.311</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B46">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C46">
-        <v>0.349</v>
+        <v>0.318</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B47">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C47">
-        <v>0.404</v>
+        <v>0.497</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B48">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C48">
-        <v>0.533</v>
+        <v>0.714</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B49">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C49">
-        <v>0.59</v>
+        <v>1.014</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B50">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C50">
-        <v>0.469</v>
+        <v>1.022</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B51">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C51">
-        <v>0.408</v>
+        <v>1.014</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B52">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C52">
-        <v>0.297</v>
+        <v>0.587</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B53">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C53">
-        <v>0.095</v>
+        <v>0.251</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B54">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C54">
-        <v>0.043</v>
+        <v>0.091</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B55">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C55">
-        <v>0.048</v>
+        <v>0.043</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,10 +1672,10 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B56">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C56">
         <v>0.048</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B57">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C57">
-        <v>0.016</v>
+        <v>0.048</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,10 +1700,10 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B58">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C58">
         <v>0.016</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45984</v>
+        <v>45993</v>
       </c>
       <c r="B59">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C59">
-        <v>0.016</v>
+        <v>0.011</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45985</v>
+        <v>45993</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C60">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C64">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B65">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C65">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B66">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C66">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B67">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C67">
-        <v>0.038</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B68">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C68">
-        <v>0.445</v>
+        <v>0.035</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B69">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C69">
-        <v>0.67</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B70">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C70">
-        <v>1.299</v>
+        <v>0.265</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B71">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C71">
-        <v>2.053</v>
+        <v>0.451</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B72">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C72">
-        <v>2.356</v>
+        <v>0.647</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B73">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C73">
-        <v>2.284</v>
+        <v>0.969</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B74">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C74">
-        <v>1.933</v>
+        <v>0.977</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B75">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C75">
-        <v>1.559</v>
+        <v>0.978</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B76">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C76">
-        <v>0.5679999999999999</v>
+        <v>0.47</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B77">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C77">
-        <v>0.421</v>
+        <v>0.251</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B78">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C78">
-        <v>0.039</v>
+        <v>0.091</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B79">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C79">
-        <v>0.044</v>
+        <v>0.043</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B80">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C80">
-        <v>0.044</v>
+        <v>0.043</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B81">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C81">
-        <v>0.011</v>
+        <v>0.043</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,10 +2036,10 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B82">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C82">
         <v>0.011</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45985</v>
+        <v>45994</v>
       </c>
       <c r="B83">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C83">
         <v>0.011</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45986</v>
+        <v>45994</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,10 +2078,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B86">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B87">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B88">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B89">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B90">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C90">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B91">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C91">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B92">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C92">
-        <v>0.181</v>
+        <v>0.192</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B93">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C93">
-        <v>0.544</v>
+        <v>0.242</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B94">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C94">
-        <v>1.033</v>
+        <v>0.484</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B95">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C95">
-        <v>1.897</v>
+        <v>0.524</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B96">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C96">
-        <v>1.932</v>
+        <v>0.501</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B97">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C97">
-        <v>2.042</v>
+        <v>0.597</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B98">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C98">
-        <v>1.692</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B99">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C99">
-        <v>1.033</v>
+        <v>0.511</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B100">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C100">
-        <v>0.518</v>
+        <v>0.331</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B101">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C101">
-        <v>0.426</v>
+        <v>0.246</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B102">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C102">
-        <v>0.039</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B103">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C103">
-        <v>0.044</v>
+        <v>0.038</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B104">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C104">
-        <v>0.044</v>
+        <v>0.043</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B105">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C105">
-        <v>0.011</v>
+        <v>0.043</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,10 +2372,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B106">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C106">
         <v>0.011</v>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45986</v>
+        <v>45995</v>
       </c>
       <c r="B107">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C107">
         <v>0.011</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45987</v>
+        <v>45995</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,10 +2414,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B111">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B112">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C112">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B113">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C113">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B114">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C114">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B115">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C115">
-        <v>0.036</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B116">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C116">
-        <v>0.153</v>
+        <v>0.035</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B117">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C117">
-        <v>0.45</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B118">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C118">
-        <v>1.025</v>
+        <v>0.265</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B119">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C119">
-        <v>1.761</v>
+        <v>0.292</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B120">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C120">
-        <v>1.806</v>
+        <v>0.331</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B121">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C121">
-        <v>1.894</v>
+        <v>0.404</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B122">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C122">
-        <v>1.084</v>
+        <v>0.484</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B123">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C123">
-        <v>0.652</v>
+        <v>0.408</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B124">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C124">
-        <v>0.286</v>
+        <v>0.292</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B125">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C125">
-        <v>0.157</v>
+        <v>0.251</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B126">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C126">
-        <v>0.043</v>
+        <v>0.091</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B127">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C127">
-        <v>0.048</v>
+        <v>0.043</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,10 +2680,10 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B128">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C128">
         <v>0.048</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B129">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C129">
-        <v>0.016</v>
+        <v>0.048</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,10 +2708,10 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B130">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C130">
         <v>0.016</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45987</v>
+        <v>45996</v>
       </c>
       <c r="B131">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C131">
         <v>0.016</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45988</v>
+        <v>45996</v>
       </c>
       <c r="B132">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C132">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,10 +2750,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C133">
         <v>0.013</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B134">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C134">
         <v>0.013</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B135">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C135">
         <v>0.013</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B136">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C136">
         <v>0.013</v>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B137">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C137">
         <v>0.013</v>
@@ -2820,10 +2820,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B138">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C138">
         <v>0.013</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B139">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C139">
-        <v>0.04</v>
+        <v>0.013</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B140">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C140">
-        <v>0.091</v>
+        <v>0.04</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B141">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C141">
-        <v>0.27</v>
+        <v>0.091</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B142">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C142">
-        <v>0.488</v>
+        <v>0.27</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B143">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C143">
-        <v>0.594</v>
+        <v>0.42</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B144">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C144">
-        <v>0.641</v>
+        <v>0.594</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B145">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C145">
-        <v>0.522</v>
+        <v>0.722</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B146">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C146">
-        <v>0.398</v>
+        <v>1.021</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B147">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C147">
-        <v>0.286</v>
+        <v>0.706</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B148">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C148">
-        <v>0.241</v>
+        <v>0.47</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B149">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C149">
-        <v>0.091</v>
+        <v>0.251</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B150">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C150">
-        <v>0.043</v>
+        <v>0.091</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B151">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C151">
-        <v>0.048</v>
+        <v>0.043</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,10 +3016,10 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B152">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C152">
         <v>0.048</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B153">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C153">
-        <v>0.016</v>
+        <v>0.048</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,10 +3044,10 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B154">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C154">
         <v>0.016</v>
@@ -3058,10 +3058,10 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="B155">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C155">
         <v>0.016</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45989</v>
+        <v>45997</v>
       </c>
       <c r="B156">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C156">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,10 +3086,10 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B157">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C157">
         <v>0.013</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B158">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C158">
         <v>0.013</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B159">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C159">
         <v>0.013</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B160">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C160">
         <v>0.013</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B161">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C161">
         <v>0.013</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B162">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C162">
         <v>0.013</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B163">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C163">
-        <v>0.04</v>
+        <v>0.013</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B164">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C164">
-        <v>0.091</v>
+        <v>0.04</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B165">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C165">
-        <v>0.27</v>
+        <v>0.091</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B166">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C166">
-        <v>0.42</v>
+        <v>0.27</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B167">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C167">
-        <v>0.545</v>
+        <v>0.31</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B168">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C168">
-        <v>0.652</v>
+        <v>0.419</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B169">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C169">
-        <v>0.601</v>
+        <v>0.652</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45989</v>
+        <v>45998</v>
       </c>
       <c r="B170">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C170">
-        <v>0.469</v>
+        <v>0.721</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Fixing some issues on the SGL productuion forecast
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,147 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>30.11.202514</t>
-  </si>
-  <si>
-    <t>30.11.202515</t>
-  </si>
-  <si>
-    <t>30.11.202516</t>
-  </si>
-  <si>
-    <t>30.11.202517</t>
-  </si>
-  <si>
-    <t>30.11.202518</t>
-  </si>
-  <si>
-    <t>30.11.202519</t>
-  </si>
-  <si>
-    <t>30.11.202520</t>
-  </si>
-  <si>
-    <t>30.11.202521</t>
-  </si>
-  <si>
-    <t>30.11.202522</t>
-  </si>
-  <si>
-    <t>30.11.202523</t>
-  </si>
-  <si>
-    <t>30.11.202524</t>
-  </si>
-  <si>
-    <t>01.12.20251</t>
-  </si>
-  <si>
-    <t>01.12.20252</t>
-  </si>
-  <si>
-    <t>01.12.20253</t>
-  </si>
-  <si>
-    <t>01.12.20254</t>
-  </si>
-  <si>
-    <t>01.12.20255</t>
-  </si>
-  <si>
-    <t>01.12.20256</t>
-  </si>
-  <si>
-    <t>01.12.20257</t>
-  </si>
-  <si>
-    <t>01.12.20258</t>
-  </si>
-  <si>
-    <t>01.12.20259</t>
-  </si>
-  <si>
-    <t>01.12.202510</t>
-  </si>
-  <si>
-    <t>01.12.202511</t>
-  </si>
-  <si>
-    <t>01.12.202512</t>
-  </si>
-  <si>
-    <t>01.12.202513</t>
-  </si>
-  <si>
-    <t>01.12.202514</t>
-  </si>
-  <si>
-    <t>01.12.202515</t>
-  </si>
-  <si>
-    <t>01.12.202516</t>
-  </si>
-  <si>
-    <t>01.12.202517</t>
-  </si>
-  <si>
-    <t>01.12.202518</t>
-  </si>
-  <si>
-    <t>01.12.202519</t>
-  </si>
-  <si>
-    <t>01.12.202520</t>
-  </si>
-  <si>
-    <t>01.12.202521</t>
-  </si>
-  <si>
-    <t>01.12.202522</t>
-  </si>
-  <si>
-    <t>01.12.202523</t>
-  </si>
-  <si>
-    <t>01.12.202524</t>
-  </si>
-  <si>
-    <t>02.12.20251</t>
-  </si>
-  <si>
-    <t>02.12.20252</t>
-  </si>
-  <si>
-    <t>02.12.20253</t>
-  </si>
-  <si>
-    <t>02.12.20254</t>
-  </si>
-  <si>
-    <t>02.12.20255</t>
-  </si>
-  <si>
-    <t>02.12.20256</t>
-  </si>
-  <si>
-    <t>02.12.20257</t>
-  </si>
-  <si>
-    <t>02.12.20258</t>
-  </si>
-  <si>
-    <t>02.12.20259</t>
-  </si>
-  <si>
-    <t>02.12.202510</t>
-  </si>
-  <si>
-    <t>02.12.202511</t>
-  </si>
-  <si>
-    <t>02.12.202512</t>
-  </si>
-  <si>
     <t>02.12.202513</t>
   </si>
   <si>
@@ -533,6 +392,147 @@
   </si>
   <si>
     <t>07.12.202514</t>
+  </si>
+  <si>
+    <t>07.12.202515</t>
+  </si>
+  <si>
+    <t>07.12.202516</t>
+  </si>
+  <si>
+    <t>07.12.202517</t>
+  </si>
+  <si>
+    <t>07.12.202518</t>
+  </si>
+  <si>
+    <t>07.12.202519</t>
+  </si>
+  <si>
+    <t>07.12.202520</t>
+  </si>
+  <si>
+    <t>07.12.202521</t>
+  </si>
+  <si>
+    <t>07.12.202522</t>
+  </si>
+  <si>
+    <t>07.12.202523</t>
+  </si>
+  <si>
+    <t>07.12.202524</t>
+  </si>
+  <si>
+    <t>08.12.20251</t>
+  </si>
+  <si>
+    <t>08.12.20252</t>
+  </si>
+  <si>
+    <t>08.12.20253</t>
+  </si>
+  <si>
+    <t>08.12.20254</t>
+  </si>
+  <si>
+    <t>08.12.20255</t>
+  </si>
+  <si>
+    <t>08.12.20256</t>
+  </si>
+  <si>
+    <t>08.12.20257</t>
+  </si>
+  <si>
+    <t>08.12.20258</t>
+  </si>
+  <si>
+    <t>08.12.20259</t>
+  </si>
+  <si>
+    <t>08.12.202510</t>
+  </si>
+  <si>
+    <t>08.12.202511</t>
+  </si>
+  <si>
+    <t>08.12.202512</t>
+  </si>
+  <si>
+    <t>08.12.202513</t>
+  </si>
+  <si>
+    <t>08.12.202514</t>
+  </si>
+  <si>
+    <t>08.12.202515</t>
+  </si>
+  <si>
+    <t>08.12.202516</t>
+  </si>
+  <si>
+    <t>08.12.202517</t>
+  </si>
+  <si>
+    <t>08.12.202518</t>
+  </si>
+  <si>
+    <t>08.12.202519</t>
+  </si>
+  <si>
+    <t>08.12.202520</t>
+  </si>
+  <si>
+    <t>08.12.202521</t>
+  </si>
+  <si>
+    <t>08.12.202522</t>
+  </si>
+  <si>
+    <t>08.12.202523</t>
+  </si>
+  <si>
+    <t>08.12.202524</t>
+  </si>
+  <si>
+    <t>09.12.20251</t>
+  </si>
+  <si>
+    <t>09.12.20252</t>
+  </si>
+  <si>
+    <t>09.12.20253</t>
+  </si>
+  <si>
+    <t>09.12.20254</t>
+  </si>
+  <si>
+    <t>09.12.20255</t>
+  </si>
+  <si>
+    <t>09.12.20256</t>
+  </si>
+  <si>
+    <t>09.12.20257</t>
+  </si>
+  <si>
+    <t>09.12.20258</t>
+  </si>
+  <si>
+    <t>09.12.20259</t>
+  </si>
+  <si>
+    <t>09.12.202510</t>
+  </si>
+  <si>
+    <t>09.12.202511</t>
+  </si>
+  <si>
+    <t>09.12.202512</t>
+  </si>
+  <si>
+    <t>09.12.202513</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>0.034</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>0.034</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>0.269</v>
+        <v>0.408</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>0.154</v>
+        <v>0.47</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>0.08599999999999999</v>
+        <v>0.251</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>0.038</v>
+        <v>0.09</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>0.043</v>
+        <v>0.038</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,10 +1014,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B9">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>0.043</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B10">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>0.011</v>
+        <v>0.043</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B11">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>0.011</v>
@@ -1056,10 +1056,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45991</v>
+        <v>45993</v>
       </c>
       <c r="B12">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>0.011</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20">
-        <v>0.035</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>0.08599999999999999</v>
+        <v>0.123</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>0.265</v>
+        <v>0.173</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>0.305</v>
+        <v>0.265</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>0.409</v>
+        <v>0.483</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>0.652</v>
+        <v>0.647</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B26">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>0.721</v>
+        <v>0.722</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B27">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>0.636</v>
+        <v>0.984</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B28">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>0.47</v>
+        <v>0.706</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B29">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>0.251</v>
+        <v>0.47</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B30">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>0.095</v>
+        <v>0.246</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B31">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31">
-        <v>0.038</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32">
-        <v>0.043</v>
+        <v>0.038</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,10 +1350,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C33">
         <v>0.043</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B34">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C34">
-        <v>0.011</v>
+        <v>0.043</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B35">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35">
         <v>0.011</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45992</v>
+        <v>45994</v>
       </c>
       <c r="B36">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36">
         <v>0.011</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>0.035</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B45">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45">
-        <v>0.08599999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B46">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C46">
-        <v>0.318</v>
+        <v>0.242</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B47">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C47">
-        <v>0.497</v>
+        <v>0.484</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C48">
-        <v>0.714</v>
+        <v>0.609</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B49">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>1.014</v>
+        <v>0.465</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B50">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C50">
-        <v>1.022</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B51">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C51">
-        <v>1.014</v>
+        <v>1.023</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B52">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C52">
-        <v>0.587</v>
+        <v>0.897</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B53">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C53">
-        <v>0.251</v>
+        <v>0.47</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B54">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C54">
-        <v>0.091</v>
+        <v>0.251</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B55">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C55">
-        <v>0.043</v>
+        <v>0.091</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B56">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C56">
-        <v>0.048</v>
+        <v>0.043</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,10 +1686,10 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B57">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C57">
         <v>0.048</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B58">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C58">
-        <v>0.016</v>
+        <v>0.048</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B59">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C59">
-        <v>0.011</v>
+        <v>0.016</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B60">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C60">
         <v>0.011</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.109</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1770,10 +1770,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B64">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B66">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B68">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C68">
-        <v>0.035</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B69">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C69">
-        <v>0.08599999999999999</v>
+        <v>0.035</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B70">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C70">
-        <v>0.265</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B71">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C71">
-        <v>0.451</v>
+        <v>0.265</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C72">
-        <v>0.647</v>
+        <v>0.305</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B73">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C73">
-        <v>0.969</v>
+        <v>0.404</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B74">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C74">
-        <v>0.977</v>
+        <v>0.528</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B75">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C75">
-        <v>0.978</v>
+        <v>0.651</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B76">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C76">
-        <v>0.47</v>
+        <v>0.636</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B77">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C77">
-        <v>0.251</v>
+        <v>0.47</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B78">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C78">
-        <v>0.091</v>
+        <v>0.251</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B79">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C79">
-        <v>0.043</v>
+        <v>0.091</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,10 +2008,10 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B80">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C80">
         <v>0.043</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B81">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C81">
-        <v>0.043</v>
+        <v>0.048</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B82">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C82">
-        <v>0.011</v>
+        <v>0.048</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B83">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C83">
-        <v>0.011</v>
+        <v>0.016</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B84">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C84">
-        <v>0.011</v>
+        <v>0.016</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2106,10 +2106,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B88">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B89">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B90">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B91">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B92">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C92">
-        <v>0.192</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B93">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C93">
-        <v>0.242</v>
+        <v>0.035</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B94">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C94">
-        <v>0.484</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B95">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C95">
-        <v>0.524</v>
+        <v>0.265</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B96">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C96">
-        <v>0.501</v>
+        <v>0.488</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B97">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C97">
-        <v>0.597</v>
+        <v>0.706</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B98">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C98">
-        <v>0.6860000000000001</v>
+        <v>1.021</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B99">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C99">
-        <v>0.511</v>
+        <v>0.721</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B100">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C100">
-        <v>0.331</v>
+        <v>0.636</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B101">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C101">
-        <v>0.246</v>
+        <v>0.402</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B102">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C102">
-        <v>0.08599999999999999</v>
+        <v>0.251</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B103">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C103">
-        <v>0.038</v>
+        <v>0.091</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,10 +2344,10 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B104">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C104">
         <v>0.043</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B105">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C105">
-        <v>0.043</v>
+        <v>0.048</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B106">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C106">
-        <v>0.011</v>
+        <v>0.048</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B107">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C107">
-        <v>0.011</v>
+        <v>0.016</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B108">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C108">
-        <v>0.011</v>
+        <v>0.016</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B110">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B111">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B112">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B113">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B114">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B115">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B116">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C116">
-        <v>0.035</v>
+        <v>0.013</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B117">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C117">
-        <v>0.08599999999999999</v>
+        <v>0.04</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B118">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C118">
-        <v>0.265</v>
+        <v>0.091</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B119">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C119">
-        <v>0.292</v>
+        <v>0.27</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B120">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C120">
-        <v>0.331</v>
+        <v>0.31</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B121">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C121">
-        <v>0.404</v>
+        <v>0.409</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B122">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C122">
-        <v>0.484</v>
+        <v>0.533</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B123">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C123">
-        <v>0.408</v>
+        <v>0.59</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B124">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C124">
-        <v>0.292</v>
+        <v>0.469</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B125">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C125">
-        <v>0.251</v>
+        <v>0.336</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B126">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C126">
-        <v>0.091</v>
+        <v>0.251</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B127">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C127">
-        <v>0.043</v>
+        <v>0.091</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B128">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C128">
-        <v>0.048</v>
+        <v>0.043</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,10 +2694,10 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B129">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C129">
         <v>0.048</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B130">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C130">
-        <v>0.016</v>
+        <v>0.048</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B131">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C131">
         <v>0.016</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B132">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C132">
         <v>0.016</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45997</v>
+        <v>45998</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C133">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B134">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C134">
         <v>0.013</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B135">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C135">
         <v>0.013</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B136">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C136">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B137">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C137">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B138">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C138">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B139">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C139">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B140">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C140">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B141">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C141">
-        <v>0.091</v>
+        <v>0.035</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B142">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C142">
-        <v>0.27</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B143">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C143">
-        <v>0.42</v>
+        <v>0.265</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B144">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C144">
-        <v>0.594</v>
+        <v>0.497</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B145">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C145">
-        <v>0.722</v>
+        <v>1.014</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B146">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C146">
-        <v>1.021</v>
+        <v>1.022</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B147">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C147">
-        <v>0.706</v>
+        <v>1.031</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B148">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C148">
-        <v>0.47</v>
+        <v>1.014</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B149">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C149">
-        <v>0.251</v>
+        <v>0.587</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B150">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C150">
-        <v>0.091</v>
+        <v>0.297</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B151">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C151">
-        <v>0.043</v>
+        <v>0.095</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B152">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C152">
-        <v>0.048</v>
+        <v>0.043</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,10 +3030,10 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B153">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C153">
         <v>0.048</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B154">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C154">
-        <v>0.016</v>
+        <v>0.048</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,10 +3058,10 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B155">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C155">
         <v>0.016</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B156">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C156">
         <v>0.016</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45998</v>
+        <v>45999</v>
       </c>
       <c r="B157">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C157">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B158">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C158">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B159">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C159">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B160">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C160">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B161">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C161">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B162">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C162">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B163">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C163">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B164">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C164">
-        <v>0.04</v>
+        <v>0.013</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B165">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C165">
-        <v>0.091</v>
+        <v>0.043</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B166">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C166">
-        <v>0.27</v>
+        <v>0.093</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B167">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C167">
-        <v>0.31</v>
+        <v>0.273</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B168">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C168">
-        <v>0.419</v>
+        <v>0.418</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B169">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C169">
-        <v>0.652</v>
+        <v>0.654</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B170">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C170">
-        <v>0.721</v>
+        <v>1.023</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Retrainin the forecast model for Dragosel Laslea
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,162 +28,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>02.12.202513</t>
-  </si>
-  <si>
-    <t>02.12.202514</t>
-  </si>
-  <si>
-    <t>02.12.202515</t>
-  </si>
-  <si>
-    <t>02.12.202516</t>
-  </si>
-  <si>
-    <t>02.12.202517</t>
-  </si>
-  <si>
-    <t>02.12.202518</t>
-  </si>
-  <si>
-    <t>02.12.202519</t>
-  </si>
-  <si>
-    <t>02.12.202520</t>
-  </si>
-  <si>
-    <t>02.12.202521</t>
-  </si>
-  <si>
-    <t>02.12.202522</t>
-  </si>
-  <si>
-    <t>02.12.202523</t>
-  </si>
-  <si>
-    <t>02.12.202524</t>
-  </si>
-  <si>
-    <t>03.12.20251</t>
-  </si>
-  <si>
-    <t>03.12.20252</t>
-  </si>
-  <si>
-    <t>03.12.20253</t>
-  </si>
-  <si>
-    <t>03.12.20254</t>
-  </si>
-  <si>
-    <t>03.12.20255</t>
-  </si>
-  <si>
-    <t>03.12.20256</t>
-  </si>
-  <si>
-    <t>03.12.20257</t>
-  </si>
-  <si>
-    <t>03.12.20258</t>
-  </si>
-  <si>
-    <t>03.12.20259</t>
-  </si>
-  <si>
-    <t>03.12.202510</t>
-  </si>
-  <si>
-    <t>03.12.202511</t>
-  </si>
-  <si>
-    <t>03.12.202512</t>
-  </si>
-  <si>
-    <t>03.12.202513</t>
-  </si>
-  <si>
-    <t>03.12.202514</t>
-  </si>
-  <si>
-    <t>03.12.202515</t>
-  </si>
-  <si>
-    <t>03.12.202516</t>
-  </si>
-  <si>
-    <t>03.12.202517</t>
-  </si>
-  <si>
-    <t>03.12.202518</t>
-  </si>
-  <si>
-    <t>03.12.202519</t>
-  </si>
-  <si>
-    <t>03.12.202520</t>
-  </si>
-  <si>
-    <t>03.12.202521</t>
-  </si>
-  <si>
-    <t>03.12.202522</t>
-  </si>
-  <si>
-    <t>03.12.202523</t>
-  </si>
-  <si>
-    <t>03.12.202524</t>
-  </si>
-  <si>
-    <t>04.12.20251</t>
-  </si>
-  <si>
-    <t>04.12.20252</t>
-  </si>
-  <si>
-    <t>04.12.20253</t>
-  </si>
-  <si>
-    <t>04.12.20254</t>
-  </si>
-  <si>
-    <t>04.12.20255</t>
-  </si>
-  <si>
-    <t>04.12.20256</t>
-  </si>
-  <si>
-    <t>04.12.20257</t>
-  </si>
-  <si>
-    <t>04.12.20258</t>
-  </si>
-  <si>
-    <t>04.12.20259</t>
-  </si>
-  <si>
-    <t>04.12.202510</t>
-  </si>
-  <si>
-    <t>04.12.202511</t>
-  </si>
-  <si>
-    <t>04.12.202512</t>
-  </si>
-  <si>
-    <t>04.12.202513</t>
-  </si>
-  <si>
-    <t>04.12.202514</t>
-  </si>
-  <si>
-    <t>04.12.202515</t>
-  </si>
-  <si>
-    <t>04.12.202516</t>
-  </si>
-  <si>
     <t>04.12.202517</t>
   </si>
   <si>
@@ -533,6 +377,162 @@
   </si>
   <si>
     <t>09.12.202513</t>
+  </si>
+  <si>
+    <t>09.12.202514</t>
+  </si>
+  <si>
+    <t>09.12.202515</t>
+  </si>
+  <si>
+    <t>09.12.202516</t>
+  </si>
+  <si>
+    <t>09.12.202517</t>
+  </si>
+  <si>
+    <t>09.12.202518</t>
+  </si>
+  <si>
+    <t>09.12.202519</t>
+  </si>
+  <si>
+    <t>09.12.202520</t>
+  </si>
+  <si>
+    <t>09.12.202521</t>
+  </si>
+  <si>
+    <t>09.12.202522</t>
+  </si>
+  <si>
+    <t>09.12.202523</t>
+  </si>
+  <si>
+    <t>09.12.202524</t>
+  </si>
+  <si>
+    <t>10.12.20251</t>
+  </si>
+  <si>
+    <t>10.12.20252</t>
+  </si>
+  <si>
+    <t>10.12.20253</t>
+  </si>
+  <si>
+    <t>10.12.20254</t>
+  </si>
+  <si>
+    <t>10.12.20255</t>
+  </si>
+  <si>
+    <t>10.12.20256</t>
+  </si>
+  <si>
+    <t>10.12.20257</t>
+  </si>
+  <si>
+    <t>10.12.20258</t>
+  </si>
+  <si>
+    <t>10.12.20259</t>
+  </si>
+  <si>
+    <t>10.12.202510</t>
+  </si>
+  <si>
+    <t>10.12.202511</t>
+  </si>
+  <si>
+    <t>10.12.202512</t>
+  </si>
+  <si>
+    <t>10.12.202513</t>
+  </si>
+  <si>
+    <t>10.12.202514</t>
+  </si>
+  <si>
+    <t>10.12.202515</t>
+  </si>
+  <si>
+    <t>10.12.202516</t>
+  </si>
+  <si>
+    <t>10.12.202517</t>
+  </si>
+  <si>
+    <t>10.12.202518</t>
+  </si>
+  <si>
+    <t>10.12.202519</t>
+  </si>
+  <si>
+    <t>10.12.202520</t>
+  </si>
+  <si>
+    <t>10.12.202521</t>
+  </si>
+  <si>
+    <t>10.12.202522</t>
+  </si>
+  <si>
+    <t>10.12.202523</t>
+  </si>
+  <si>
+    <t>10.12.202524</t>
+  </si>
+  <si>
+    <t>11.12.20251</t>
+  </si>
+  <si>
+    <t>11.12.20252</t>
+  </si>
+  <si>
+    <t>11.12.20253</t>
+  </si>
+  <si>
+    <t>11.12.20254</t>
+  </si>
+  <si>
+    <t>11.12.20255</t>
+  </si>
+  <si>
+    <t>11.12.20256</t>
+  </si>
+  <si>
+    <t>11.12.20257</t>
+  </si>
+  <si>
+    <t>11.12.20258</t>
+  </si>
+  <si>
+    <t>11.12.20259</t>
+  </si>
+  <si>
+    <t>11.12.202510</t>
+  </si>
+  <si>
+    <t>11.12.202511</t>
+  </si>
+  <si>
+    <t>11.12.202512</t>
+  </si>
+  <si>
+    <t>11.12.202513</t>
+  </si>
+  <si>
+    <t>11.12.202514</t>
+  </si>
+  <si>
+    <t>11.12.202515</t>
+  </si>
+  <si>
+    <t>11.12.202516</t>
+  </si>
+  <si>
+    <t>11.12.202517</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>0.034</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>0.034</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>0.408</v>
+        <v>0.043</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>0.47</v>
+        <v>0.048</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>0.251</v>
+        <v>0.048</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C7">
-        <v>0.09</v>
+        <v>0.011</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B8">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>0.038</v>
+        <v>0.011</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45993</v>
+        <v>45995</v>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C9">
-        <v>0.043</v>
+        <v>0.109</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45993</v>
+        <v>45996</v>
       </c>
       <c r="B10">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0.043</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45993</v>
+        <v>45996</v>
       </c>
       <c r="B11">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45993</v>
+        <v>45996</v>
       </c>
       <c r="B12">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45993</v>
+        <v>45996</v>
       </c>
       <c r="B13">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>0.011</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.123</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.265</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>0.305</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C21">
-        <v>0.123</v>
+        <v>0.404</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C22">
-        <v>0.173</v>
+        <v>0.409</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C23">
-        <v>0.265</v>
+        <v>0.408</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C24">
-        <v>0.483</v>
+        <v>0.335</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C25">
-        <v>0.647</v>
+        <v>0.292</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B26">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>0.722</v>
+        <v>0.246</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B27">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C27">
-        <v>0.984</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B28">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C28">
-        <v>0.706</v>
+        <v>0.043</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B29">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>0.47</v>
+        <v>0.048</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B30">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C30">
-        <v>0.246</v>
+        <v>0.048</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B31">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C31">
-        <v>0.08599999999999999</v>
+        <v>0.016</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B32">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C32">
-        <v>0.038</v>
+        <v>0.016</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45994</v>
+        <v>45996</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C33">
-        <v>0.043</v>
+        <v>0.016</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45994</v>
+        <v>45997</v>
       </c>
       <c r="B34">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>0.043</v>
+        <v>0.013</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45994</v>
+        <v>45997</v>
       </c>
       <c r="B35">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45994</v>
+        <v>45997</v>
       </c>
       <c r="B36">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45994</v>
+        <v>45997</v>
       </c>
       <c r="B37">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C37">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>0.091</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.445</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>0.297</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B45">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C45">
-        <v>0.192</v>
+        <v>0.292</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C46">
-        <v>0.242</v>
+        <v>0.341</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B47">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C47">
-        <v>0.484</v>
+        <v>0.47</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B48">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C48">
-        <v>0.609</v>
+        <v>0.47</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B49">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C49">
-        <v>0.465</v>
+        <v>0.297</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B50">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C50">
-        <v>0.6879999999999999</v>
+        <v>0.426</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B51">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C51">
-        <v>1.023</v>
+        <v>0.091</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B52">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C52">
-        <v>0.897</v>
+        <v>0.043</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B53">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C53">
-        <v>0.47</v>
+        <v>0.048</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B54">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C54">
-        <v>0.251</v>
+        <v>0.048</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B55">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C55">
-        <v>0.091</v>
+        <v>0.016</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B56">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C56">
-        <v>0.043</v>
+        <v>0.016</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45995</v>
+        <v>45997</v>
       </c>
       <c r="B57">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C57">
-        <v>0.048</v>
+        <v>0.016</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45995</v>
+        <v>45998</v>
       </c>
       <c r="B58">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>0.048</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45995</v>
+        <v>45998</v>
       </c>
       <c r="B59">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C59">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45995</v>
+        <v>45998</v>
       </c>
       <c r="B60">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C60">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45995</v>
+        <v>45998</v>
       </c>
       <c r="B61">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C61">
-        <v>0.109</v>
+        <v>0.013</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B65">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>0.091</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B67">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B68">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>0.416</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C69">
-        <v>0.035</v>
+        <v>0.545</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B70">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C70">
-        <v>0.08599999999999999</v>
+        <v>0.714</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B71">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C71">
-        <v>0.265</v>
+        <v>0.951</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B72">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C72">
-        <v>0.305</v>
+        <v>0.86</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B73">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C73">
-        <v>0.404</v>
+        <v>0.478</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B74">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C74">
-        <v>0.528</v>
+        <v>0.251</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B75">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C75">
-        <v>0.651</v>
+        <v>0.091</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B76">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C76">
-        <v>0.636</v>
+        <v>0.043</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B77">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C77">
-        <v>0.47</v>
+        <v>0.048</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B78">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C78">
-        <v>0.251</v>
+        <v>0.048</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B79">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C79">
-        <v>0.091</v>
+        <v>0.016</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B80">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C80">
-        <v>0.043</v>
+        <v>0.016</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45996</v>
+        <v>45998</v>
       </c>
       <c r="B81">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C81">
-        <v>0.048</v>
+        <v>0.016</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="B82">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C82">
-        <v>0.048</v>
+        <v>0.013</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="B83">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C83">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="B84">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C84">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="B85">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C85">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B89">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B90">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>0.091</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B91">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B92">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>0.416</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B93">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C93">
-        <v>0.035</v>
+        <v>0.644</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B94">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C94">
-        <v>0.08599999999999999</v>
+        <v>1.014</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B95">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C95">
-        <v>0.265</v>
+        <v>1.014</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B96">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C96">
-        <v>0.488</v>
+        <v>1.014</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B97">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C97">
-        <v>0.706</v>
+        <v>0.715</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B98">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C98">
-        <v>1.021</v>
+        <v>0.292</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B99">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C99">
-        <v>0.721</v>
+        <v>0.137</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B100">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C100">
-        <v>0.636</v>
+        <v>0.043</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B101">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C101">
-        <v>0.402</v>
+        <v>0.048</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B102">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C102">
-        <v>0.251</v>
+        <v>0.048</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B103">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C103">
-        <v>0.091</v>
+        <v>0.016</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B104">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C104">
-        <v>0.043</v>
+        <v>0.016</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45997</v>
+        <v>45999</v>
       </c>
       <c r="B105">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C105">
-        <v>0.048</v>
+        <v>0.016</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B106">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C106">
-        <v>0.048</v>
+        <v>0.013</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B107">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C107">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B108">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C108">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>45997</v>
+        <v>46000</v>
       </c>
       <c r="B109">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C109">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C110">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B111">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C111">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B112">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C112">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B113">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C113">
-        <v>0.013</v>
+        <v>0.035</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B114">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C114">
-        <v>0.013</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B115">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C115">
-        <v>0.013</v>
+        <v>0.265</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B116">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C116">
-        <v>0.013</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B117">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C117">
-        <v>0.04</v>
+        <v>1.014</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B118">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C118">
-        <v>0.091</v>
+        <v>1.054</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B119">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C119">
-        <v>0.27</v>
+        <v>0.99</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B120">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C120">
-        <v>0.31</v>
+        <v>1.034</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B121">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C121">
-        <v>0.409</v>
+        <v>0.975</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B122">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C122">
-        <v>0.533</v>
+        <v>0.292</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B123">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C123">
-        <v>0.59</v>
+        <v>0.137</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B124">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C124">
-        <v>0.469</v>
+        <v>0.043</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B125">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C125">
-        <v>0.336</v>
+        <v>0.048</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B126">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C126">
-        <v>0.251</v>
+        <v>0.048</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B127">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C127">
-        <v>0.091</v>
+        <v>0.016</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B128">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C128">
-        <v>0.043</v>
+        <v>0.016</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>45998</v>
+        <v>46000</v>
       </c>
       <c r="B129">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C129">
-        <v>0.048</v>
+        <v>0.016</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>45998</v>
+        <v>46001</v>
       </c>
       <c r="B130">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C130">
-        <v>0.048</v>
+        <v>0.013</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>45998</v>
+        <v>46001</v>
       </c>
       <c r="B131">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C131">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>45998</v>
+        <v>46001</v>
       </c>
       <c r="B132">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C132">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>45998</v>
+        <v>46001</v>
       </c>
       <c r="B133">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C133">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,10 +2764,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C134">
         <v>0.013</v>
@@ -2778,10 +2778,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B135">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C135">
         <v>0.013</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B136">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B137">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B138">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>0.091</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B139">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>0.318</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B140">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>0.734</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B141">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C141">
-        <v>0.035</v>
+        <v>1.011</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B142">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C142">
-        <v>0.08599999999999999</v>
+        <v>1.599</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B143">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C143">
-        <v>0.265</v>
+        <v>1.812</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B144">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C144">
-        <v>0.497</v>
+        <v>1.139</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B145">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C145">
-        <v>1.014</v>
+        <v>0.991</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B146">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C146">
-        <v>1.022</v>
+        <v>0.292</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B147">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C147">
-        <v>1.031</v>
+        <v>0.095</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B148">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C148">
-        <v>1.014</v>
+        <v>0.043</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B149">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C149">
-        <v>0.587</v>
+        <v>0.048</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B150">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C150">
-        <v>0.297</v>
+        <v>0.048</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B151">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C151">
-        <v>0.095</v>
+        <v>0.016</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B152">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C152">
-        <v>0.043</v>
+        <v>0.016</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>45999</v>
+        <v>46001</v>
       </c>
       <c r="B153">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C153">
-        <v>0.048</v>
+        <v>0.016</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>45999</v>
+        <v>46002</v>
       </c>
       <c r="B154">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C154">
-        <v>0.048</v>
+        <v>0.013</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>45999</v>
+        <v>46002</v>
       </c>
       <c r="B155">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C155">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>45999</v>
+        <v>46002</v>
       </c>
       <c r="B156">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C156">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>45999</v>
+        <v>46002</v>
       </c>
       <c r="B157">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C157">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B158">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B159">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B160">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B161">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B162">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>0.091</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B163">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>0.318</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B164">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C164">
-        <v>0.013</v>
+        <v>0.712</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B165">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C165">
-        <v>0.043</v>
+        <v>1.028</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B166">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C166">
-        <v>0.093</v>
+        <v>1.878</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B167">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C167">
-        <v>0.273</v>
+        <v>1.64</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B168">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C168">
-        <v>0.418</v>
+        <v>1.434</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B169">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C169">
-        <v>0.654</v>
+        <v>0.971</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B170">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C170">
-        <v>1.023</v>
+        <v>0.41</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Updating the Forecast Portfolio
</commit_message>
<xml_diff>
--- a/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
+++ b/3D_Steel/Results_Production_3D_Steel_xgb.xlsx
@@ -28,511 +28,511 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>04.12.202517</t>
-  </si>
-  <si>
-    <t>04.12.202518</t>
-  </si>
-  <si>
-    <t>04.12.202519</t>
-  </si>
-  <si>
-    <t>04.12.202520</t>
-  </si>
-  <si>
-    <t>04.12.202521</t>
-  </si>
-  <si>
-    <t>04.12.202522</t>
-  </si>
-  <si>
-    <t>04.12.202523</t>
-  </si>
-  <si>
-    <t>04.12.202524</t>
-  </si>
-  <si>
-    <t>05.12.20251</t>
-  </si>
-  <si>
-    <t>05.12.20252</t>
-  </si>
-  <si>
-    <t>05.12.20253</t>
-  </si>
-  <si>
-    <t>05.12.20254</t>
-  </si>
-  <si>
-    <t>05.12.20255</t>
-  </si>
-  <si>
-    <t>05.12.20256</t>
-  </si>
-  <si>
-    <t>05.12.20257</t>
-  </si>
-  <si>
-    <t>05.12.20258</t>
-  </si>
-  <si>
-    <t>05.12.20259</t>
-  </si>
-  <si>
-    <t>05.12.202510</t>
-  </si>
-  <si>
-    <t>05.12.202511</t>
-  </si>
-  <si>
-    <t>05.12.202512</t>
-  </si>
-  <si>
-    <t>05.12.202513</t>
-  </si>
-  <si>
-    <t>05.12.202514</t>
-  </si>
-  <si>
-    <t>05.12.202515</t>
-  </si>
-  <si>
-    <t>05.12.202516</t>
-  </si>
-  <si>
-    <t>05.12.202517</t>
-  </si>
-  <si>
-    <t>05.12.202518</t>
-  </si>
-  <si>
-    <t>05.12.202519</t>
-  </si>
-  <si>
-    <t>05.12.202520</t>
-  </si>
-  <si>
-    <t>05.12.202521</t>
-  </si>
-  <si>
-    <t>05.12.202522</t>
-  </si>
-  <si>
-    <t>05.12.202523</t>
-  </si>
-  <si>
-    <t>05.12.202524</t>
-  </si>
-  <si>
-    <t>06.12.20251</t>
-  </si>
-  <si>
-    <t>06.12.20252</t>
-  </si>
-  <si>
-    <t>06.12.20253</t>
-  </si>
-  <si>
-    <t>06.12.20254</t>
-  </si>
-  <si>
-    <t>06.12.20255</t>
-  </si>
-  <si>
-    <t>06.12.20256</t>
-  </si>
-  <si>
-    <t>06.12.20257</t>
-  </si>
-  <si>
-    <t>06.12.20258</t>
-  </si>
-  <si>
-    <t>06.12.20259</t>
-  </si>
-  <si>
-    <t>06.12.202510</t>
-  </si>
-  <si>
-    <t>06.12.202511</t>
-  </si>
-  <si>
-    <t>06.12.202512</t>
-  </si>
-  <si>
-    <t>06.12.202513</t>
-  </si>
-  <si>
-    <t>06.12.202514</t>
-  </si>
-  <si>
-    <t>06.12.202515</t>
-  </si>
-  <si>
-    <t>06.12.202516</t>
-  </si>
-  <si>
-    <t>06.12.202517</t>
-  </si>
-  <si>
-    <t>06.12.202518</t>
-  </si>
-  <si>
-    <t>06.12.202519</t>
-  </si>
-  <si>
-    <t>06.12.202520</t>
-  </si>
-  <si>
-    <t>06.12.202521</t>
-  </si>
-  <si>
-    <t>06.12.202522</t>
-  </si>
-  <si>
-    <t>06.12.202523</t>
-  </si>
-  <si>
-    <t>06.12.202524</t>
-  </si>
-  <si>
-    <t>07.12.20251</t>
-  </si>
-  <si>
-    <t>07.12.20252</t>
-  </si>
-  <si>
-    <t>07.12.20253</t>
-  </si>
-  <si>
-    <t>07.12.20254</t>
-  </si>
-  <si>
-    <t>07.12.20255</t>
-  </si>
-  <si>
-    <t>07.12.20256</t>
-  </si>
-  <si>
-    <t>07.12.20257</t>
-  </si>
-  <si>
-    <t>07.12.20258</t>
-  </si>
-  <si>
-    <t>07.12.20259</t>
-  </si>
-  <si>
-    <t>07.12.202510</t>
-  </si>
-  <si>
-    <t>07.12.202511</t>
-  </si>
-  <si>
-    <t>07.12.202512</t>
-  </si>
-  <si>
-    <t>07.12.202513</t>
-  </si>
-  <si>
-    <t>07.12.202514</t>
-  </si>
-  <si>
-    <t>07.12.202515</t>
-  </si>
-  <si>
-    <t>07.12.202516</t>
-  </si>
-  <si>
-    <t>07.12.202517</t>
-  </si>
-  <si>
-    <t>07.12.202518</t>
-  </si>
-  <si>
-    <t>07.12.202519</t>
-  </si>
-  <si>
-    <t>07.12.202520</t>
-  </si>
-  <si>
-    <t>07.12.202521</t>
-  </si>
-  <si>
-    <t>07.12.202522</t>
-  </si>
-  <si>
-    <t>07.12.202523</t>
-  </si>
-  <si>
-    <t>07.12.202524</t>
-  </si>
-  <si>
-    <t>08.12.20251</t>
-  </si>
-  <si>
-    <t>08.12.20252</t>
-  </si>
-  <si>
-    <t>08.12.20253</t>
-  </si>
-  <si>
-    <t>08.12.20254</t>
-  </si>
-  <si>
-    <t>08.12.20255</t>
-  </si>
-  <si>
-    <t>08.12.20256</t>
-  </si>
-  <si>
-    <t>08.12.20257</t>
-  </si>
-  <si>
-    <t>08.12.20258</t>
-  </si>
-  <si>
-    <t>08.12.20259</t>
-  </si>
-  <si>
-    <t>08.12.202510</t>
-  </si>
-  <si>
-    <t>08.12.202511</t>
-  </si>
-  <si>
-    <t>08.12.202512</t>
-  </si>
-  <si>
-    <t>08.12.202513</t>
-  </si>
-  <si>
-    <t>08.12.202514</t>
-  </si>
-  <si>
-    <t>08.12.202515</t>
-  </si>
-  <si>
-    <t>08.12.202516</t>
-  </si>
-  <si>
-    <t>08.12.202517</t>
-  </si>
-  <si>
-    <t>08.12.202518</t>
-  </si>
-  <si>
-    <t>08.12.202519</t>
-  </si>
-  <si>
-    <t>08.12.202520</t>
-  </si>
-  <si>
-    <t>08.12.202521</t>
-  </si>
-  <si>
-    <t>08.12.202522</t>
-  </si>
-  <si>
-    <t>08.12.202523</t>
-  </si>
-  <si>
-    <t>08.12.202524</t>
-  </si>
-  <si>
-    <t>09.12.20251</t>
-  </si>
-  <si>
-    <t>09.12.20252</t>
-  </si>
-  <si>
-    <t>09.12.20253</t>
-  </si>
-  <si>
-    <t>09.12.20254</t>
-  </si>
-  <si>
-    <t>09.12.20255</t>
-  </si>
-  <si>
-    <t>09.12.20256</t>
-  </si>
-  <si>
-    <t>09.12.20257</t>
-  </si>
-  <si>
-    <t>09.12.20258</t>
-  </si>
-  <si>
-    <t>09.12.20259</t>
-  </si>
-  <si>
-    <t>09.12.202510</t>
-  </si>
-  <si>
-    <t>09.12.202511</t>
-  </si>
-  <si>
-    <t>09.12.202512</t>
-  </si>
-  <si>
-    <t>09.12.202513</t>
-  </si>
-  <si>
-    <t>09.12.202514</t>
-  </si>
-  <si>
-    <t>09.12.202515</t>
-  </si>
-  <si>
-    <t>09.12.202516</t>
-  </si>
-  <si>
-    <t>09.12.202517</t>
-  </si>
-  <si>
-    <t>09.12.202518</t>
-  </si>
-  <si>
-    <t>09.12.202519</t>
-  </si>
-  <si>
-    <t>09.12.202520</t>
-  </si>
-  <si>
-    <t>09.12.202521</t>
-  </si>
-  <si>
-    <t>09.12.202522</t>
-  </si>
-  <si>
-    <t>09.12.202523</t>
-  </si>
-  <si>
-    <t>09.12.202524</t>
-  </si>
-  <si>
-    <t>10.12.20251</t>
-  </si>
-  <si>
-    <t>10.12.20252</t>
-  </si>
-  <si>
-    <t>10.12.20253</t>
-  </si>
-  <si>
-    <t>10.12.20254</t>
-  </si>
-  <si>
-    <t>10.12.20255</t>
-  </si>
-  <si>
-    <t>10.12.20256</t>
-  </si>
-  <si>
-    <t>10.12.20257</t>
-  </si>
-  <si>
-    <t>10.12.20258</t>
-  </si>
-  <si>
-    <t>10.12.20259</t>
-  </si>
-  <si>
-    <t>10.12.202510</t>
-  </si>
-  <si>
-    <t>10.12.202511</t>
-  </si>
-  <si>
-    <t>10.12.202512</t>
-  </si>
-  <si>
-    <t>10.12.202513</t>
-  </si>
-  <si>
-    <t>10.12.202514</t>
-  </si>
-  <si>
-    <t>10.12.202515</t>
-  </si>
-  <si>
-    <t>10.12.202516</t>
-  </si>
-  <si>
-    <t>10.12.202517</t>
-  </si>
-  <si>
-    <t>10.12.202518</t>
-  </si>
-  <si>
-    <t>10.12.202519</t>
-  </si>
-  <si>
-    <t>10.12.202520</t>
-  </si>
-  <si>
-    <t>10.12.202521</t>
-  </si>
-  <si>
-    <t>10.12.202522</t>
-  </si>
-  <si>
-    <t>10.12.202523</t>
-  </si>
-  <si>
-    <t>10.12.202524</t>
-  </si>
-  <si>
-    <t>11.12.20251</t>
-  </si>
-  <si>
-    <t>11.12.20252</t>
-  </si>
-  <si>
-    <t>11.12.20253</t>
-  </si>
-  <si>
-    <t>11.12.20254</t>
-  </si>
-  <si>
-    <t>11.12.20255</t>
-  </si>
-  <si>
-    <t>11.12.20256</t>
-  </si>
-  <si>
-    <t>11.12.20257</t>
-  </si>
-  <si>
-    <t>11.12.20258</t>
-  </si>
-  <si>
-    <t>11.12.20259</t>
-  </si>
-  <si>
-    <t>11.12.202510</t>
-  </si>
-  <si>
-    <t>11.12.202511</t>
-  </si>
-  <si>
-    <t>11.12.202512</t>
-  </si>
-  <si>
-    <t>11.12.202513</t>
-  </si>
-  <si>
-    <t>11.12.202514</t>
-  </si>
-  <si>
-    <t>11.12.202515</t>
-  </si>
-  <si>
-    <t>11.12.202516</t>
-  </si>
-  <si>
-    <t>11.12.202517</t>
+    <t>31.12.202510</t>
+  </si>
+  <si>
+    <t>31.12.202511</t>
+  </si>
+  <si>
+    <t>31.12.202512</t>
+  </si>
+  <si>
+    <t>31.12.202513</t>
+  </si>
+  <si>
+    <t>31.12.202514</t>
+  </si>
+  <si>
+    <t>31.12.202515</t>
+  </si>
+  <si>
+    <t>31.12.202516</t>
+  </si>
+  <si>
+    <t>31.12.202517</t>
+  </si>
+  <si>
+    <t>31.12.202518</t>
+  </si>
+  <si>
+    <t>31.12.202519</t>
+  </si>
+  <si>
+    <t>31.12.202520</t>
+  </si>
+  <si>
+    <t>31.12.202521</t>
+  </si>
+  <si>
+    <t>31.12.202522</t>
+  </si>
+  <si>
+    <t>31.12.202523</t>
+  </si>
+  <si>
+    <t>31.12.202524</t>
+  </si>
+  <si>
+    <t>01.01.20261</t>
+  </si>
+  <si>
+    <t>01.01.20262</t>
+  </si>
+  <si>
+    <t>01.01.20263</t>
+  </si>
+  <si>
+    <t>01.01.20264</t>
+  </si>
+  <si>
+    <t>01.01.20265</t>
+  </si>
+  <si>
+    <t>01.01.20266</t>
+  </si>
+  <si>
+    <t>01.01.20267</t>
+  </si>
+  <si>
+    <t>01.01.20268</t>
+  </si>
+  <si>
+    <t>01.01.20269</t>
+  </si>
+  <si>
+    <t>01.01.202610</t>
+  </si>
+  <si>
+    <t>01.01.202611</t>
+  </si>
+  <si>
+    <t>01.01.202612</t>
+  </si>
+  <si>
+    <t>01.01.202613</t>
+  </si>
+  <si>
+    <t>01.01.202614</t>
+  </si>
+  <si>
+    <t>01.01.202615</t>
+  </si>
+  <si>
+    <t>01.01.202616</t>
+  </si>
+  <si>
+    <t>01.01.202617</t>
+  </si>
+  <si>
+    <t>01.01.202618</t>
+  </si>
+  <si>
+    <t>01.01.202619</t>
+  </si>
+  <si>
+    <t>01.01.202620</t>
+  </si>
+  <si>
+    <t>01.01.202621</t>
+  </si>
+  <si>
+    <t>01.01.202622</t>
+  </si>
+  <si>
+    <t>01.01.202623</t>
+  </si>
+  <si>
+    <t>01.01.202624</t>
+  </si>
+  <si>
+    <t>02.01.20261</t>
+  </si>
+  <si>
+    <t>02.01.20262</t>
+  </si>
+  <si>
+    <t>02.01.20263</t>
+  </si>
+  <si>
+    <t>02.01.20264</t>
+  </si>
+  <si>
+    <t>02.01.20265</t>
+  </si>
+  <si>
+    <t>02.01.20266</t>
+  </si>
+  <si>
+    <t>02.01.20267</t>
+  </si>
+  <si>
+    <t>02.01.20268</t>
+  </si>
+  <si>
+    <t>02.01.20269</t>
+  </si>
+  <si>
+    <t>02.01.202610</t>
+  </si>
+  <si>
+    <t>02.01.202611</t>
+  </si>
+  <si>
+    <t>02.01.202612</t>
+  </si>
+  <si>
+    <t>02.01.202613</t>
+  </si>
+  <si>
+    <t>02.01.202614</t>
+  </si>
+  <si>
+    <t>02.01.202615</t>
+  </si>
+  <si>
+    <t>02.01.202616</t>
+  </si>
+  <si>
+    <t>02.01.202617</t>
+  </si>
+  <si>
+    <t>02.01.202618</t>
+  </si>
+  <si>
+    <t>02.01.202619</t>
+  </si>
+  <si>
+    <t>02.01.202620</t>
+  </si>
+  <si>
+    <t>02.01.202621</t>
+  </si>
+  <si>
+    <t>02.01.202622</t>
+  </si>
+  <si>
+    <t>02.01.202623</t>
+  </si>
+  <si>
+    <t>02.01.202624</t>
+  </si>
+  <si>
+    <t>03.01.20261</t>
+  </si>
+  <si>
+    <t>03.01.20262</t>
+  </si>
+  <si>
+    <t>03.01.20263</t>
+  </si>
+  <si>
+    <t>03.01.20264</t>
+  </si>
+  <si>
+    <t>03.01.20265</t>
+  </si>
+  <si>
+    <t>03.01.20266</t>
+  </si>
+  <si>
+    <t>03.01.20267</t>
+  </si>
+  <si>
+    <t>03.01.20268</t>
+  </si>
+  <si>
+    <t>03.01.20269</t>
+  </si>
+  <si>
+    <t>03.01.202610</t>
+  </si>
+  <si>
+    <t>03.01.202611</t>
+  </si>
+  <si>
+    <t>03.01.202612</t>
+  </si>
+  <si>
+    <t>03.01.202613</t>
+  </si>
+  <si>
+    <t>03.01.202614</t>
+  </si>
+  <si>
+    <t>03.01.202615</t>
+  </si>
+  <si>
+    <t>03.01.202616</t>
+  </si>
+  <si>
+    <t>03.01.202617</t>
+  </si>
+  <si>
+    <t>03.01.202618</t>
+  </si>
+  <si>
+    <t>03.01.202619</t>
+  </si>
+  <si>
+    <t>03.01.202620</t>
+  </si>
+  <si>
+    <t>03.01.202621</t>
+  </si>
+  <si>
+    <t>03.01.202622</t>
+  </si>
+  <si>
+    <t>03.01.202623</t>
+  </si>
+  <si>
+    <t>03.01.202624</t>
+  </si>
+  <si>
+    <t>04.01.20261</t>
+  </si>
+  <si>
+    <t>04.01.20262</t>
+  </si>
+  <si>
+    <t>04.01.20263</t>
+  </si>
+  <si>
+    <t>04.01.20264</t>
+  </si>
+  <si>
+    <t>04.01.20265</t>
+  </si>
+  <si>
+    <t>04.01.20266</t>
+  </si>
+  <si>
+    <t>04.01.20267</t>
+  </si>
+  <si>
+    <t>04.01.20268</t>
+  </si>
+  <si>
+    <t>04.01.20269</t>
+  </si>
+  <si>
+    <t>04.01.202610</t>
+  </si>
+  <si>
+    <t>04.01.202611</t>
+  </si>
+  <si>
+    <t>04.01.202612</t>
+  </si>
+  <si>
+    <t>04.01.202613</t>
+  </si>
+  <si>
+    <t>04.01.202614</t>
+  </si>
+  <si>
+    <t>04.01.202615</t>
+  </si>
+  <si>
+    <t>04.01.202616</t>
+  </si>
+  <si>
+    <t>04.01.202617</t>
+  </si>
+  <si>
+    <t>04.01.202618</t>
+  </si>
+  <si>
+    <t>04.01.202619</t>
+  </si>
+  <si>
+    <t>04.01.202620</t>
+  </si>
+  <si>
+    <t>04.01.202621</t>
+  </si>
+  <si>
+    <t>04.01.202622</t>
+  </si>
+  <si>
+    <t>04.01.202623</t>
+  </si>
+  <si>
+    <t>04.01.202624</t>
+  </si>
+  <si>
+    <t>05.01.20261</t>
+  </si>
+  <si>
+    <t>05.01.20262</t>
+  </si>
+  <si>
+    <t>05.01.20263</t>
+  </si>
+  <si>
+    <t>05.01.20264</t>
+  </si>
+  <si>
+    <t>05.01.20265</t>
+  </si>
+  <si>
+    <t>05.01.20266</t>
+  </si>
+  <si>
+    <t>05.01.20267</t>
+  </si>
+  <si>
+    <t>05.01.20268</t>
+  </si>
+  <si>
+    <t>05.01.20269</t>
+  </si>
+  <si>
+    <t>05.01.202610</t>
+  </si>
+  <si>
+    <t>05.01.202611</t>
+  </si>
+  <si>
+    <t>05.01.202612</t>
+  </si>
+  <si>
+    <t>05.01.202613</t>
+  </si>
+  <si>
+    <t>05.01.202614</t>
+  </si>
+  <si>
+    <t>05.01.202615</t>
+  </si>
+  <si>
+    <t>05.01.202616</t>
+  </si>
+  <si>
+    <t>05.01.202617</t>
+  </si>
+  <si>
+    <t>05.01.202618</t>
+  </si>
+  <si>
+    <t>05.01.202619</t>
+  </si>
+  <si>
+    <t>05.01.202620</t>
+  </si>
+  <si>
+    <t>05.01.202621</t>
+  </si>
+  <si>
+    <t>05.01.202622</t>
+  </si>
+  <si>
+    <t>05.01.202623</t>
+  </si>
+  <si>
+    <t>05.01.202624</t>
+  </si>
+  <si>
+    <t>06.01.20261</t>
+  </si>
+  <si>
+    <t>06.01.20262</t>
+  </si>
+  <si>
+    <t>06.01.20263</t>
+  </si>
+  <si>
+    <t>06.01.20264</t>
+  </si>
+  <si>
+    <t>06.01.20265</t>
+  </si>
+  <si>
+    <t>06.01.20266</t>
+  </si>
+  <si>
+    <t>06.01.20267</t>
+  </si>
+  <si>
+    <t>06.01.20268</t>
+  </si>
+  <si>
+    <t>06.01.20269</t>
+  </si>
+  <si>
+    <t>06.01.202610</t>
+  </si>
+  <si>
+    <t>06.01.202611</t>
+  </si>
+  <si>
+    <t>06.01.202612</t>
+  </si>
+  <si>
+    <t>06.01.202613</t>
+  </si>
+  <si>
+    <t>06.01.202614</t>
+  </si>
+  <si>
+    <t>06.01.202615</t>
+  </si>
+  <si>
+    <t>06.01.202616</t>
+  </si>
+  <si>
+    <t>06.01.202617</t>
+  </si>
+  <si>
+    <t>06.01.202618</t>
+  </si>
+  <si>
+    <t>06.01.202619</t>
+  </si>
+  <si>
+    <t>06.01.202620</t>
+  </si>
+  <si>
+    <t>06.01.202621</t>
+  </si>
+  <si>
+    <t>06.01.202622</t>
+  </si>
+  <si>
+    <t>06.01.202623</t>
+  </si>
+  <si>
+    <t>06.01.202624</t>
+  </si>
+  <si>
+    <t>07.01.20261</t>
+  </si>
+  <si>
+    <t>07.01.20262</t>
+  </si>
+  <si>
+    <t>07.01.20263</t>
+  </si>
+  <si>
+    <t>07.01.20264</t>
+  </si>
+  <si>
+    <t>07.01.20265</t>
+  </si>
+  <si>
+    <t>07.01.20266</t>
+  </si>
+  <si>
+    <t>07.01.20267</t>
+  </si>
+  <si>
+    <t>07.01.20268</t>
+  </si>
+  <si>
+    <t>07.01.20269</t>
+  </si>
+  <si>
+    <t>07.01.202610</t>
   </si>
 </sst>
 </file>
@@ -916,10 +916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>45995</v>
+        <v>46022</v>
       </c>
       <c r="B2">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>0.034</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>45995</v>
+        <v>46022</v>
       </c>
       <c r="B3">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>0.034</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>45995</v>
+        <v>46022</v>
       </c>
       <c r="B4">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>0.043</v>
+        <v>1.509</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -958,13 +958,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>45995</v>
+        <v>46022</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>0.048</v>
+        <v>1.714</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>45995</v>
+        <v>46022</v>
       </c>
       <c r="B6">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>0.048</v>
+        <v>1.603</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>45995</v>
+        <v>46022</v>
       </c>
       <c r="B7">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>0.011</v>
+        <v>1.468</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>45995</v>
+        <v>46022</v>
       </c>
       <c r="B8">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>0.011</v>
+        <v>1.235</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>45995</v>
+        <v>46022</v>
       </c>
       <c r="B9">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>0.109</v>
+        <v>0.679</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>45996</v>
+        <v>46022</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.421</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>45996</v>
+        <v>46022</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>45996</v>
+        <v>46022</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.049</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>45996</v>
+        <v>46022</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>45996</v>
+        <v>46022</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>45996</v>
+        <v>46022</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>45996</v>
+        <v>46022</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1126,13 +1126,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0.123</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>0.08599999999999999</v>
+        <v>0.014</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>0.265</v>
+        <v>0.014</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B20">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>0.305</v>
+        <v>0.014</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>0.404</v>
+        <v>0.014</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B22">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>0.409</v>
+        <v>0.014</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B23">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>0.408</v>
+        <v>0.014</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B24">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>0.335</v>
+        <v>0.041</v>
       </c>
       <c r="D24" t="s">
         <v>26</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B25">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>0.292</v>
+        <v>0.06</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B26">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>0.246</v>
+        <v>0.334</v>
       </c>
       <c r="D26" t="s">
         <v>28</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B27">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>0.08599999999999999</v>
+        <v>1.057</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B28">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>0.043</v>
+        <v>1.652</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B29">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>0.048</v>
+        <v>2.17</v>
       </c>
       <c r="D29" t="s">
         <v>31</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B30">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>0.048</v>
+        <v>1.983</v>
       </c>
       <c r="D30" t="s">
         <v>32</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B31">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>0.016</v>
+        <v>1.764</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B32">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>0.016</v>
+        <v>1.184</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>45996</v>
+        <v>46023</v>
       </c>
       <c r="B33">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>0.016</v>
+        <v>0.583</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>45997</v>
+        <v>46023</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C34">
-        <v>0.013</v>
+        <v>0.427</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>45997</v>
+        <v>46023</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C35">
-        <v>0.013</v>
+        <v>0.035</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>45997</v>
+        <v>46023</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C36">
-        <v>0.013</v>
+        <v>0.091</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>45997</v>
+        <v>46023</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C37">
-        <v>0.013</v>
+        <v>0.091</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>45997</v>
+        <v>46023</v>
       </c>
       <c r="B38">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C38">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>40</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>45997</v>
+        <v>46023</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C39">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>41</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>45997</v>
+        <v>46023</v>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C40">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B42">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>0.091</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>44</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B43">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C43">
-        <v>0.445</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B44">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>0.297</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>46</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B45">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>0.292</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B46">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>0.341</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>48</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B47">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C47">
-        <v>0.47</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B48">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>0.47</v>
+        <v>0.033</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B49">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>0.297</v>
+        <v>0.051</v>
       </c>
       <c r="D49" t="s">
         <v>51</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B50">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>0.426</v>
+        <v>0.28</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B51">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>0.091</v>
+        <v>1.108</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B52">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C52">
-        <v>0.043</v>
+        <v>1.505</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B53">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C53">
-        <v>0.048</v>
+        <v>2.043</v>
       </c>
       <c r="D53" t="s">
         <v>55</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B54">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C54">
-        <v>0.048</v>
+        <v>1.84</v>
       </c>
       <c r="D54" t="s">
         <v>56</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B55">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C55">
-        <v>0.016</v>
+        <v>1.826</v>
       </c>
       <c r="D55" t="s">
         <v>57</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B56">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>0.016</v>
+        <v>1.02</v>
       </c>
       <c r="D56" t="s">
         <v>58</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>45997</v>
+        <v>46024</v>
       </c>
       <c r="B57">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C57">
-        <v>0.016</v>
+        <v>0.508</v>
       </c>
       <c r="D57" t="s">
         <v>59</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>45998</v>
+        <v>46024</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>0.422</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>45998</v>
+        <v>46024</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="D59" t="s">
         <v>61</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>45998</v>
+        <v>46024</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C60">
-        <v>0.013</v>
+        <v>0.096</v>
       </c>
       <c r="D60" t="s">
         <v>62</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>45998</v>
+        <v>46024</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C61">
-        <v>0.013</v>
+        <v>0.096</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>45998</v>
+        <v>46024</v>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C62">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>64</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>45998</v>
+        <v>46024</v>
       </c>
       <c r="B63">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C63">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>65</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>45998</v>
+        <v>46024</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C64">
-        <v>0.013</v>
+        <v>0.014</v>
       </c>
       <c r="D64" t="s">
         <v>66</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B65">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C65">
-        <v>0.04</v>
+        <v>0.011</v>
       </c>
       <c r="D65" t="s">
         <v>67</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B66">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C66">
-        <v>0.091</v>
+        <v>0.011</v>
       </c>
       <c r="D66" t="s">
         <v>68</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B67">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>0.27</v>
+        <v>0.011</v>
       </c>
       <c r="D67" t="s">
         <v>69</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B68">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>0.416</v>
+        <v>0.011</v>
       </c>
       <c r="D68" t="s">
         <v>70</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B69">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C69">
-        <v>0.545</v>
+        <v>0.011</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B70">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>0.714</v>
+        <v>0.011</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B71">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C71">
-        <v>0.951</v>
+        <v>0.011</v>
       </c>
       <c r="D71" t="s">
         <v>73</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B72">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>0.86</v>
+        <v>0.038</v>
       </c>
       <c r="D72" t="s">
         <v>74</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B73">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C73">
-        <v>0.478</v>
+        <v>0.056</v>
       </c>
       <c r="D73" t="s">
         <v>75</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B74">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>0.251</v>
+        <v>0.29</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B75">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C75">
-        <v>0.091</v>
+        <v>0.96</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B76">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C76">
-        <v>0.043</v>
+        <v>1.436</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B77">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C77">
-        <v>0.048</v>
+        <v>1.977</v>
       </c>
       <c r="D77" t="s">
         <v>79</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B78">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C78">
-        <v>0.048</v>
+        <v>1.827</v>
       </c>
       <c r="D78" t="s">
         <v>80</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B79">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C79">
-        <v>0.016</v>
+        <v>1.35</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B80">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C80">
-        <v>0.016</v>
+        <v>0.888</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>45998</v>
+        <v>46025</v>
       </c>
       <c r="B81">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C81">
-        <v>0.016</v>
+        <v>0.297</v>
       </c>
       <c r="D81" t="s">
         <v>83</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>45999</v>
+        <v>46025</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C82">
-        <v>0.013</v>
+        <v>0.132</v>
       </c>
       <c r="D82" t="s">
         <v>84</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>45999</v>
+        <v>46025</v>
       </c>
       <c r="B83">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C83">
-        <v>0.013</v>
+        <v>0.038</v>
       </c>
       <c r="D83" t="s">
         <v>85</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>45999</v>
+        <v>46025</v>
       </c>
       <c r="B84">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C84">
-        <v>0.013</v>
+        <v>0.094</v>
       </c>
       <c r="D84" t="s">
         <v>86</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>45999</v>
+        <v>46025</v>
       </c>
       <c r="B85">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C85">
-        <v>0.013</v>
+        <v>0.094</v>
       </c>
       <c r="D85" t="s">
         <v>87</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>45999</v>
+        <v>46025</v>
       </c>
       <c r="B86">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C86">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D86" t="s">
         <v>88</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>45999</v>
+        <v>46025</v>
       </c>
       <c r="B87">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C87">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D87" t="s">
         <v>89</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>45999</v>
+        <v>46025</v>
       </c>
       <c r="B88">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C88">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
       <c r="D88" t="s">
         <v>90</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B89">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C89">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
         <v>91</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B90">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C90">
-        <v>0.091</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
         <v>92</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B91">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C91">
-        <v>0.27</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
         <v>93</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B92">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C92">
-        <v>0.416</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
         <v>94</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B93">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C93">
-        <v>0.644</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
         <v>95</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B94">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C94">
-        <v>1.014</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
         <v>96</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B95">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C95">
-        <v>1.014</v>
+        <v>0</v>
       </c>
       <c r="D95" t="s">
         <v>97</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B96">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C96">
-        <v>1.014</v>
+        <v>0.192</v>
       </c>
       <c r="D96" t="s">
         <v>98</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B97">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C97">
-        <v>0.715</v>
+        <v>0.21</v>
       </c>
       <c r="D97" t="s">
         <v>99</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B98">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C98">
-        <v>0.292</v>
+        <v>0.501</v>
       </c>
       <c r="D98" t="s">
         <v>100</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B99">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C99">
-        <v>0.137</v>
+        <v>0.678</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B100">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C100">
-        <v>0.043</v>
+        <v>1.135</v>
       </c>
       <c r="D100" t="s">
         <v>102</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B101">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C101">
-        <v>0.048</v>
+        <v>1.387</v>
       </c>
       <c r="D101" t="s">
         <v>103</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B102">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C102">
-        <v>0.048</v>
+        <v>1.534</v>
       </c>
       <c r="D102" t="s">
         <v>104</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B103">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C103">
-        <v>0.016</v>
+        <v>1.228</v>
       </c>
       <c r="D103" t="s">
         <v>105</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B104">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C104">
-        <v>0.016</v>
+        <v>0.991</v>
       </c>
       <c r="D104" t="s">
         <v>106</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>45999</v>
+        <v>46026</v>
       </c>
       <c r="B105">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C105">
-        <v>0.016</v>
+        <v>0.369</v>
       </c>
       <c r="D105" t="s">
         <v>107</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>46000</v>
+        <v>46026</v>
       </c>
       <c r="B106">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C106">
-        <v>0.013</v>
+        <v>0.421</v>
       </c>
       <c r="D106" t="s">
         <v>108</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>46000</v>
+        <v>46026</v>
       </c>
       <c r="B107">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C107">
-        <v>0.013</v>
+        <v>0.126</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>46000</v>
+        <v>46026</v>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>0.181</v>
       </c>
       <c r="D108" t="s">
         <v>110</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>46000</v>
+        <v>46026</v>
       </c>
       <c r="B109">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.181</v>
       </c>
       <c r="D109" t="s">
         <v>111</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>46000</v>
+        <v>46026</v>
       </c>
       <c r="B110">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>0.109</v>
       </c>
       <c r="D110" t="s">
         <v>112</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>46000</v>
+        <v>46026</v>
       </c>
       <c r="B111">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D111" t="s">
         <v>113</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>46000</v>
+        <v>46026</v>
       </c>
       <c r="B112">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>0.011</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -2470,13 +2470,13 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B113">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C113">
-        <v>0.035</v>
+        <v>0</v>
       </c>
       <c r="D113" t="s">
         <v>115</v>
@@ -2484,13 +2484,13 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B114">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C114">
-        <v>0.08599999999999999</v>
+        <v>0</v>
       </c>
       <c r="D114" t="s">
         <v>116</v>
@@ -2498,13 +2498,13 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B115">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C115">
-        <v>0.265</v>
+        <v>0</v>
       </c>
       <c r="D115" t="s">
         <v>117</v>
@@ -2512,13 +2512,13 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B116">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C116">
-        <v>0.5570000000000001</v>
+        <v>0</v>
       </c>
       <c r="D116" t="s">
         <v>118</v>
@@ -2526,13 +2526,13 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B117">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C117">
-        <v>1.014</v>
+        <v>0</v>
       </c>
       <c r="D117" t="s">
         <v>119</v>
@@ -2540,13 +2540,13 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B118">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>1.054</v>
+        <v>0</v>
       </c>
       <c r="D118" t="s">
         <v>120</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B119">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C119">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="D119" t="s">
         <v>121</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B120">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C120">
-        <v>1.034</v>
+        <v>0.192</v>
       </c>
       <c r="D120" t="s">
         <v>122</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B121">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C121">
-        <v>0.975</v>
+        <v>0.21</v>
       </c>
       <c r="D121" t="s">
         <v>123</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B122">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C122">
-        <v>0.292</v>
+        <v>0.501</v>
       </c>
       <c r="D122" t="s">
         <v>124</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B123">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C123">
-        <v>0.137</v>
+        <v>0.678</v>
       </c>
       <c r="D123" t="s">
         <v>125</v>
@@ -2624,13 +2624,13 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B124">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C124">
-        <v>0.043</v>
+        <v>0.954</v>
       </c>
       <c r="D124" t="s">
         <v>126</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B125">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C125">
-        <v>0.048</v>
+        <v>1.021</v>
       </c>
       <c r="D125" t="s">
         <v>127</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B126">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C126">
-        <v>0.048</v>
+        <v>0.797</v>
       </c>
       <c r="D126" t="s">
         <v>128</v>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B127">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C127">
-        <v>0.016</v>
+        <v>0.505</v>
       </c>
       <c r="D127" t="s">
         <v>129</v>
@@ -2680,13 +2680,13 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B128">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C128">
-        <v>0.016</v>
+        <v>0.505</v>
       </c>
       <c r="D128" t="s">
         <v>130</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>46000</v>
+        <v>46027</v>
       </c>
       <c r="B129">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C129">
-        <v>0.016</v>
+        <v>0.465</v>
       </c>
       <c r="D129" t="s">
         <v>131</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>46001</v>
+        <v>46027</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C130">
-        <v>0.013</v>
+        <v>0.242</v>
       </c>
       <c r="D130" t="s">
         <v>132</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="2">
-        <v>46001</v>
+        <v>46027</v>
       </c>
       <c r="B131">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C131">
-        <v>0.013</v>
+        <v>0.195</v>
       </c>
       <c r="D131" t="s">
         <v>133</v>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>46001</v>
+        <v>46027</v>
       </c>
       <c r="B132">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C132">
-        <v>0.013</v>
+        <v>0.25</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -2750,13 +2750,13 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>46001</v>
+        <v>46027</v>
       </c>
       <c r="B133">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C133">
-        <v>0.013</v>
+        <v>0.25</v>
       </c>
       <c r="D133" t="s">
         <v>135</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>46001</v>
+        <v>46027</v>
       </c>
       <c r="B134">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C134">
-        <v>0.013</v>
+        <v>0.109</v>
       </c>
       <c r="D134" t="s">
         <v>136</v>
@@ -2778,13 +2778,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>46001</v>
+        <v>46027</v>
       </c>
       <c r="B135">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C135">
-        <v>0.013</v>
+        <v>0.112</v>
       </c>
       <c r="D135" t="s">
         <v>137</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>46001</v>
+        <v>46027</v>
       </c>
       <c r="B136">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C136">
-        <v>0.013</v>
+        <v>0.112</v>
       </c>
       <c r="D136" t="s">
         <v>138</v>
@@ -2806,13 +2806,13 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B137">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C137">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="D137" t="s">
         <v>139</v>
@@ -2820,13 +2820,13 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B138">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C138">
-        <v>0.091</v>
+        <v>0.01</v>
       </c>
       <c r="D138" t="s">
         <v>140</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B139">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C139">
-        <v>0.318</v>
+        <v>0.015</v>
       </c>
       <c r="D139" t="s">
         <v>141</v>
@@ -2848,13 +2848,13 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B140">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C140">
-        <v>0.734</v>
+        <v>0.015</v>
       </c>
       <c r="D140" t="s">
         <v>142</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B141">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C141">
-        <v>1.011</v>
+        <v>0.015</v>
       </c>
       <c r="D141" t="s">
         <v>143</v>
@@ -2876,13 +2876,13 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B142">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C142">
-        <v>1.599</v>
+        <v>0.015</v>
       </c>
       <c r="D142" t="s">
         <v>144</v>
@@ -2890,13 +2890,13 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B143">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C143">
-        <v>1.812</v>
+        <v>0.01</v>
       </c>
       <c r="D143" t="s">
         <v>145</v>
@@ -2904,13 +2904,13 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B144">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C144">
-        <v>1.139</v>
+        <v>0.038</v>
       </c>
       <c r="D144" t="s">
         <v>146</v>
@@ -2918,13 +2918,13 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B145">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C145">
-        <v>0.991</v>
+        <v>0.056</v>
       </c>
       <c r="D145" t="s">
         <v>147</v>
@@ -2932,13 +2932,13 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B146">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C146">
-        <v>0.292</v>
+        <v>0.462</v>
       </c>
       <c r="D146" t="s">
         <v>148</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B147">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C147">
-        <v>0.095</v>
+        <v>0.314</v>
       </c>
       <c r="D147" t="s">
         <v>149</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B148">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C148">
-        <v>0.043</v>
+        <v>0.43</v>
       </c>
       <c r="D148" t="s">
         <v>150</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B149">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C149">
-        <v>0.048</v>
+        <v>0.734</v>
       </c>
       <c r="D149" t="s">
         <v>151</v>
@@ -2988,13 +2988,13 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B150">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C150">
-        <v>0.048</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="D150" t="s">
         <v>152</v>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B151">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C151">
-        <v>0.016</v>
+        <v>0.41</v>
       </c>
       <c r="D151" t="s">
         <v>153</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B152">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C152">
-        <v>0.016</v>
+        <v>0.289</v>
       </c>
       <c r="D152" t="s">
         <v>154</v>
@@ -3030,13 +3030,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>46001</v>
+        <v>46028</v>
       </c>
       <c r="B153">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C153">
-        <v>0.016</v>
+        <v>0.336</v>
       </c>
       <c r="D153" t="s">
         <v>155</v>
@@ -3044,13 +3044,13 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>46002</v>
+        <v>46028</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C154">
-        <v>0.013</v>
+        <v>0.244</v>
       </c>
       <c r="D154" t="s">
         <v>156</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>46002</v>
+        <v>46028</v>
       </c>
       <c r="B155">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C155">
-        <v>0.013</v>
+        <v>0.197</v>
       </c>
       <c r="D155" t="s">
         <v>157</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>46002</v>
+        <v>46028</v>
       </c>
       <c r="B156">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C156">
-        <v>0.013</v>
+        <v>0.252</v>
       </c>
       <c r="D156" t="s">
         <v>158</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>46002</v>
+        <v>46028</v>
       </c>
       <c r="B157">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C157">
-        <v>0.013</v>
+        <v>0.252</v>
       </c>
       <c r="D157" t="s">
         <v>159</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>46002</v>
+        <v>46028</v>
       </c>
       <c r="B158">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C158">
-        <v>0.013</v>
+        <v>0.112</v>
       </c>
       <c r="D158" t="s">
         <v>160</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>46002</v>
+        <v>46028</v>
       </c>
       <c r="B159">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C159">
-        <v>0.013</v>
+        <v>0.112</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>46002</v>
+        <v>46028</v>
       </c>
       <c r="B160">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C160">
-        <v>0.013</v>
+        <v>0.112</v>
       </c>
       <c r="D160" t="s">
         <v>162</v>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
-        <v>46002</v>
+        <v>46029</v>
       </c>
       <c r="B161">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C161">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="D161" t="s">
         <v>163</v>
@@ -3156,13 +3156,13 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="2">
-        <v>46002</v>
+        <v>46029</v>
       </c>
       <c r="B162">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C162">
-        <v>0.091</v>
+        <v>0.01</v>
       </c>
       <c r="D162" t="s">
         <v>164</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="2">
-        <v>46002</v>
+        <v>46029</v>
       </c>
       <c r="B163">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C163">
-        <v>0.318</v>
+        <v>0.01</v>
       </c>
       <c r="D163" t="s">
         <v>165</v>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="2">
-        <v>46002</v>
+        <v>46029</v>
       </c>
       <c r="B164">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C164">
-        <v>0.712</v>
+        <v>0.01</v>
       </c>
       <c r="D164" t="s">
         <v>166</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="2">
-        <v>46002</v>
+        <v>46029</v>
       </c>
       <c r="B165">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C165">
-        <v>1.028</v>
+        <v>0.01</v>
       </c>
       <c r="D165" t="s">
         <v>167</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="2">
-        <v>46002</v>
+        <v>46029</v>
       </c>
       <c r="B166">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C166">
-        <v>1.878</v>
+        <v>0.01</v>
       </c>
       <c r="D166" t="s">
         <v>168</v>
@@ -3226,13 +3226,13 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="2">
-        <v>46002</v>
+        <v>46029</v>
       </c>
       <c r="B167">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C167">
-        <v>1.64</v>
+        <v>0.01</v>
       </c>
       <c r="D167" t="s">
         <v>169</v>
@@ -3240,13 +3240,13 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="2">
-        <v>46002</v>
+        <v>46029</v>
       </c>
       <c r="B168">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C168">
-        <v>1.434</v>
+        <v>0.194</v>
       </c>
       <c r="D168" t="s">
         <v>170</v>
@@ -3254,13 +3254,13 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="2">
-        <v>46002</v>
+        <v>46029</v>
       </c>
       <c r="B169">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C169">
-        <v>0.971</v>
+        <v>0.212</v>
       </c>
       <c r="D169" t="s">
         <v>171</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="2">
-        <v>46002</v>
+        <v>46029</v>
       </c>
       <c r="B170">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C170">
-        <v>0.41</v>
+        <v>1.081</v>
       </c>
       <c r="D170" t="s">
         <v>172</v>

</xml_diff>